<commit_message>
Excel progress ausgefüllt und überflüssige Variablen gelöscht
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A36EA5A-5FC7-4B07-9785-F1B948735AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2772B99D-0CD5-4291-A6F5-9747E07851EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$K$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$K$74</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="339">
   <si>
     <t>Concept Id</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Selbstzahler</t>
   </si>
   <si>
-    <t>zusammen mit dn</t>
-  </si>
-  <si>
     <t>ClinicalDocument/participant/associatedOrganisation/name</t>
   </si>
   <si>
@@ -414,22 +411,6 @@
     <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
   </si>
   <si>
-    <t>Transportmittel</t>
-  </si>
-  <si>
-    <t>transportmittel_name</t>
-  </si>
-  <si>
-    <t>RTW</t>
-  </si>
-  <si>
-    <t>value_set=[KTW, RTW, NAW/NEF/ITW]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/text
-ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@displayName</t>
-  </si>
-  <si>
     <t>Transportmittel Code</t>
   </si>
   <si>
@@ -451,21 +432,6 @@
     <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
   </si>
   <si>
-    <t>Zuweisung</t>
-  </si>
-  <si>
-    <t>zuweisung_name</t>
-  </si>
-  <si>
-    <t>KV-Notdienst außerhalb des Krankenhauses</t>
-  </si>
-  <si>
-    <t>displayname</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@displayName</t>
-  </si>
-  <si>
     <t>Notfallanamnese</t>
   </si>
   <si>
@@ -475,21 +441,12 @@
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t>ChatGPT</t>
-  </si>
-  <si>
     <t>ClinicalDocument/component/structuredBody/component/section/text</t>
   </si>
   <si>
-    <t>Beschwerde bei Vorstellung Text</t>
-  </si>
-  <si>
     <t>beschwerden_txt</t>
   </si>
   <si>
-    <t>AZ-Verschlechterun</t>
-  </si>
-  <si>
     <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
   </si>
   <si>
@@ -532,24 +489,9 @@
     <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
   </si>
   <si>
-    <t>Beschwerde Name</t>
-  </si>
-  <si>
-    <t>beschwerde_name</t>
-  </si>
-  <si>
-    <t>Diarrhea</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@displayName</t>
-  </si>
-  <si>
     <t>Beschwerde originaltext</t>
   </si>
   <si>
-    <t>beschwerde_original</t>
-  </si>
-  <si>
     <t>Durchfall und Erbrechen</t>
   </si>
   <si>
@@ -565,9 +507,6 @@
     <t>|triageval|5|triageval|</t>
   </si>
   <si>
-    <t>Liste aus TriageEval</t>
-  </si>
-  <si>
     <t>Ersteinschätzung zeit start</t>
   </si>
   <si>
@@ -613,36 +552,9 @@
     <t>value_set=[1.2.276.0.76.5.438]</t>
   </si>
   <si>
-    <t>Nicht fertig</t>
-  </si>
-  <si>
     <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
   </si>
   <si>
-    <t>Ersteinschaetzung name</t>
-  </si>
-  <si>
-    <t>ersteinschaetzung_name</t>
-  </si>
-  <si>
-    <t>nicht dringend - blau - 120 Minuten</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@displayName</t>
-  </si>
-  <si>
-    <t>Basisinfo Schwangerschaftsstatus displayName</t>
-  </si>
-  <si>
-    <t>schwanger_name</t>
-  </si>
-  <si>
-    <t>Patient ist schwanger</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/text, ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
     <t>Basisinfo Schwangerschaftsstatus code</t>
   </si>
   <si>
@@ -691,9 +603,6 @@
     <t>3MRGN</t>
   </si>
   <si>
-    <t>value_set=[MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
     <t>Diagnostik ganzer Text</t>
   </si>
   <si>
@@ -712,9 +621,6 @@
     <t>37637-6</t>
   </si>
   <si>
-    <t>Blockweise Generieren, REGEX</t>
-  </si>
-  <si>
     <t>0..n</t>
   </si>
   <si>
@@ -760,27 +666,6 @@
     <t>value_set=[PB, OPB]</t>
   </si>
   <si>
-    <t>Diagnostik Ergebnis_text</t>
-  </si>
-  <si>
-    <t>diagnostik_ergebnis_name</t>
-  </si>
-  <si>
-    <t>ohne path. Befund</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@displayName</t>
-  </si>
-  <si>
-    <t>Vitalparameter Text</t>
-  </si>
-  <si>
-    <t>vitalparameter_text</t>
-  </si>
-  <si>
-    <t>nicht angegeben</t>
-  </si>
-  <si>
     <t>Vitalparameter Entry Atemfrequenz</t>
   </si>
   <si>
@@ -913,9 +798,6 @@
     <t>|Allergien|Antibiotika : |</t>
   </si>
   <si>
-    <t>enthält alle alllergien (spezifisch verweist darauf)</t>
-  </si>
-  <si>
     <t>Allergien vorhanden?</t>
   </si>
   <si>
@@ -967,9 +849,6 @@
     <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
   </si>
   <si>
-    <t>Diagnose ICD10 CODE displayName</t>
-  </si>
-  <si>
     <t>diagnose_name</t>
   </si>
   <si>
@@ -985,9 +864,6 @@
     <t>approved</t>
   </si>
   <si>
-    <t>fehlerfrei</t>
-  </si>
-  <si>
     <t>format=yyyymmddhhmm</t>
   </si>
   <si>
@@ -1082,6 +958,96 @@
   </si>
   <si>
     <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t>generating</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>Blockweise</t>
+  </si>
+  <si>
+    <t>Verweise auf andere Allergien sollten hier gemacht werden</t>
+  </si>
+  <si>
+    <t>Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t>generting</t>
+  </si>
+  <si>
+    <t>Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t>ManchesterTriageSystem ist default Wieso überhaupt speichern</t>
+  </si>
+  <si>
+    <t>scope=0-6</t>
+  </si>
+  <si>
+    <t>(1-6)?</t>
+  </si>
+  <si>
+    <t>startunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Generieren </t>
+  </si>
+  <si>
+    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t>Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t>Cardinality, Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert)</t>
+  </si>
+  <si>
+    <t>Verweise auf andere…</t>
+  </si>
+  <si>
+    <t>ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t>genreating</t>
+  </si>
+  <si>
+    <t>chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t>beschwerde_liste</t>
+  </si>
+  <si>
+    <t>AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Diagnostik </t>
+  </si>
+  <si>
+    <t>Keine Validierung von Neg Ind (da kann alles drinn stehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja </t>
+  </si>
+  <si>
+    <t>Valueset?</t>
+  </si>
+  <si>
+    <t>zusammen mit Block</t>
+  </si>
+  <si>
+    <t>Cardinality;nullflavor</t>
+  </si>
+  <si>
+    <t>Cardinality,Nullflavor</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE originalText</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1166,9 +1132,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1362,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1385,7 +1348,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>339</v>
+        <v>298</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1394,13 +1357,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>338</v>
+        <v>297</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>337</v>
+        <v>296</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>314</v>
+        <v>274</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -1417,10 +1380,10 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -1429,22 +1392,27 @@
         <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>284</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2">
         <v>174</v>
@@ -1453,26 +1421,30 @@
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
+        <v>285</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="C4" s="2">
         <v>174</v>
@@ -1481,18 +1453,22 @@
         <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
+        <v>285</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1509,9 +1485,14 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>286</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1536,9 +1517,14 @@
         <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>287</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1560,9 +1546,11 @@
         <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1572,80 +1560,88 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>177</v>
+        <v>313</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
+        <v>288</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1661,8 +1657,8 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>9</v>
+      <c r="F11" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>17</v>
@@ -1676,21 +1672,26 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>289</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1698,62 +1699,68 @@
         <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
+        <v>290</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>193</v>
+        <v>316</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1770,10 +1777,10 @@
         <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>316</v>
+        <v>276</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>27</v>
@@ -1800,10 +1807,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
+        <v>310</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>10</v>
@@ -1829,9 +1833,11 @@
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>278</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1841,48 +1847,55 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>291</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="H19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1890,35 +1903,39 @@
         <v>33</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
+        <v>284</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1935,9 +1952,11 @@
         <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1959,10 +1978,10 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -1976,303 +1995,336 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>280</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G23" s="1" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>281</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>282</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>282</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
       <c r="A29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>282</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="H31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>306</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H32" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>307</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>226</v>
+        <v>320</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>321</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H34" s="1" t="s">
         <v>27</v>
       </c>
@@ -2280,26 +2332,28 @@
         <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>292</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
@@ -2307,234 +2361,269 @@
         <v>27</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="H36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
+        <v>291</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="6"/>
+        <v>292</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="6"/>
+        <v>293</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="6"/>
+        <v>294</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="6"/>
+        <v>295</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>323</v>
+      </c>
       <c r="H41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>330</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>150</v>
+        <v>328</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>151</v>
+        <v>329</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="6" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G44" s="6" t="s">
         <v>54</v>
       </c>
@@ -2542,49 +2631,54 @@
         <v>10</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>147</v>
+        <v>325</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>242</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G46" s="6" t="s">
         <v>54</v>
       </c>
@@ -2592,29 +2686,31 @@
         <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>242</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G47" s="6" t="s">
         <v>54</v>
       </c>
@@ -2622,29 +2718,31 @@
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G48" s="6" t="s">
         <v>54</v>
       </c>
@@ -2652,10 +2750,10 @@
         <v>10</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2672,7 +2770,12 @@
         <v>32</v>
       </c>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="F49" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="H49" s="1" t="s">
         <v>17</v>
       </c>
@@ -2685,146 +2788,166 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>266</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>168</v>
+        <v>267</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G50" s="1" t="s">
-        <v>142</v>
+        <v>327</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>304</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>305</v>
+        <v>65</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>306</v>
+        <v>66</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H51" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>209</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="H53" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I53" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="J53" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>210</v>
+        <v>259</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H55" s="1" t="s">
         <v>27</v>
       </c>
@@ -2832,51 +2955,56 @@
         <v>33</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>299</v>
+        <v>178</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>211</v>
+        <v>333</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F56" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="H56" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>297</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>207</v>
+        <v>46</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H57" s="1" t="s">
         <v>17</v>
       </c>
@@ -2884,669 +3012,549 @@
         <v>33</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="E58" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H58" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E59" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="F59" s="8"/>
+      <c r="E59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H59" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J59" s="1" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E60" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="1" t="s">
-        <v>142</v>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>143</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G61" s="1" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
-        <v>68</v>
+        <v>207</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>208</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="H62" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I63" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="J63" s="1" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>248</v>
+        <v>191</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
-        <v>195</v>
+        <v>268</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>197</v>
+        <v>270</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G65" s="1" t="s">
-        <v>142</v>
+        <v>334</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>198</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>243</v>
+        <v>94</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>244</v>
+        <v>96</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G66" s="1" t="s">
-        <v>236</v>
+        <v>335</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>227</v>
+        <v>27</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
-        <v>238</v>
+        <v>83</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>239</v>
+        <v>84</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>240</v>
+        <v>85</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="G67" s="1" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>227</v>
+        <v>89</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>206</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
-        <v>199</v>
+        <v>79</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>201</v>
+        <v>81</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1" t="s">
-        <v>142</v>
+      <c r="F68" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="J68" s="1" t="s">
-        <v>202</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="H69" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I69" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="J69" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="H70" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
-        <v>127</v>
+        <v>261</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>128</v>
+        <v>262</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>129</v>
+        <v>257</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F71" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G71" s="1" t="s">
-        <v>54</v>
+        <v>337</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>131</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
-        <v>307</v>
+        <v>263</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>308</v>
+        <v>264</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>309</v>
+        <v>257</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="H72" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>95</v>
+        <v>338</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>96</v>
+        <v>273</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1" t="s">
-        <v>97</v>
+      <c r="F73" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>98</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="B74" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>85</v>
+        <v>299</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>90</v>
+        <v>300</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="B75" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>81</v>
+        <v>301</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="H75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J75" s="1" t="s">
-        <v>82</v>
+        <v>26</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="B76" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>44</v>
+        <v>302</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="H76" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J76" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="B77" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F77" s="1"/>
-      <c r="H77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F78" s="1"/>
-      <c r="H78" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J78" s="1" t="s">
-        <v>297</v>
+      <c r="F78" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="B79" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F79" s="1"/>
-      <c r="H79" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5">
-      <c r="B81" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5">
-      <c r="B82" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5">
-      <c r="B83" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="B84" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5">
-      <c r="B85" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5">
-      <c r="B86" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>341</v>
+        <v>300</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes in formatting
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add new parameter "column" which represent a column that should be used in .csv. Every link parameter should be followed by "link" parameter
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -513,7 +513,7 @@
     <t xml:space="preserve">254</t>
   </si>
   <si>
-    <t xml:space="preserve">link=cedis.csv</t>
+    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
@@ -531,7 +531,7 @@
     <t xml:space="preserve">String_test</t>
   </si>
   <si>
-    <t xml:space="preserve">link=diagnostic_codes.csv</t>
+    <t xml:space="preserve">link=diagnostic_codes.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
@@ -750,7 +750,7 @@
     <t xml:space="preserve">Dr. med.</t>
   </si>
   <si>
-    <t xml:space="preserve">value_set=[Dr. med.,Dr. rer. med, Dr. rer. med., Dr. rer. Medic.]  </t>
+    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic.]  </t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
@@ -813,7 +813,7 @@
     <t xml:space="preserve">Keine Validierung von Neg Ind (da kann alles drinn stehen</t>
   </si>
   <si>
-    <t xml:space="preserve">Patirnt family name</t>
+    <t xml:space="preserve">Patient family name</t>
   </si>
   <si>
     <t xml:space="preserve">family_patient</t>
@@ -822,7 +822,7 @@
     <t xml:space="preserve">Kicker</t>
   </si>
   <si>
-    <t xml:space="preserve">link=family_names.csv</t>
+    <t xml:space="preserve">link=family_names.csv;column=family_name</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
@@ -867,7 +867,7 @@
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
-    <t xml:space="preserve">link=first_names.csv</t>
+    <t xml:space="preserve">link=first_names.csv;column=first_name</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
@@ -1386,18 +1386,18 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="33.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="66.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>

</xml_diff>

<commit_message>
Fix reading number of datasets from CLI
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -774,7 +774,7 @@
     <t xml:space="preserve">Extremity X-ray</t>
   </si>
   <si>
-    <t xml:space="preserve">Blockweise Diagnostik </t>
+    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
@@ -1386,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add for city and corresponding organisation a table
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="343">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -880,6 +880,9 @@
   </si>
   <si>
     <t xml:space="preserve">München</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=cities.csv;column=city</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
@@ -1386,8 +1389,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E63" activeCellId="0" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1398,7 +1401,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="66.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="66.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="112.75"/>
@@ -3178,7 +3181,9 @@
       <c r="D61" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="F61" s="1" t="s">
         <v>21</v>
       </c>
@@ -3192,24 +3197,24 @@
         <v>23</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
@@ -3229,13 +3234,13 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>45</v>
@@ -3250,18 +3255,18 @@
         <v>40</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>45</v>
@@ -3282,13 +3287,13 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>45</v>
@@ -3298,7 +3303,7 @@
         <v>21</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
@@ -3307,18 +3312,18 @@
         <v>27</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>45</v>
@@ -3328,53 +3333,53 @@
         <v>14</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>261</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>45</v>
@@ -3387,18 +3392,18 @@
         <v>40</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>45</v>
@@ -3416,18 +3421,18 @@
         <v>23</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>45</v>
@@ -3439,7 +3444,7 @@
         <v>14</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
@@ -3453,13 +3458,13 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>45</v>
@@ -3471,7 +3476,7 @@
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>16</v>
@@ -3485,13 +3490,13 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>45</v>
@@ -3503,7 +3508,7 @@
         <v>14</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>16</v>
@@ -3517,13 +3522,13 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>45</v>
@@ -3539,18 +3544,18 @@
         <v>27</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>21</v>
@@ -3558,13 +3563,13 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>21</v>
@@ -3572,13 +3577,13 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>21</v>
@@ -3586,13 +3591,13 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>21</v>
@@ -3600,13 +3605,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>21</v>
@@ -3614,13 +3619,13 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Add streets and postalcodes.
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="344">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -718,6 +718,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=streets.csv;column=street_address_line</t>
   </si>
   <si>
     <t xml:space="preserve">genreating</t>
@@ -1389,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E63" activeCellId="0" sqref="E63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2831,9 +2834,11 @@
       <c r="D49" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="F49" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>8</v>
@@ -2845,18 +2850,18 @@
         <v>23</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>45</v>
@@ -2866,7 +2871,7 @@
         <v>21</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>16</v>
@@ -2880,19 +2885,19 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>21</v>
@@ -2901,18 +2906,18 @@
         <v>40</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>45</v>
@@ -2925,18 +2930,18 @@
         <v>40</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>45</v>
@@ -2946,7 +2951,7 @@
         <v>79</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>40</v>
@@ -2955,24 +2960,24 @@
         <v>27</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>14</v>
@@ -2992,19 +2997,19 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>14</v>
@@ -3019,28 +3024,28 @@
         <v>23</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>40</v>
@@ -3054,19 +3059,19 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>21</v>
@@ -3078,24 +3083,24 @@
         <v>23</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>14</v>
@@ -3110,24 +3115,24 @@
         <v>62</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>14</v>
@@ -3139,24 +3144,24 @@
         <v>16</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>21</v>
@@ -3165,24 +3170,24 @@
         <v>40</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>21</v>
@@ -3197,24 +3202,24 @@
         <v>23</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>14</v>
@@ -3234,19 +3239,19 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>21</v>
@@ -3255,18 +3260,18 @@
         <v>40</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>45</v>
@@ -3287,13 +3292,13 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>45</v>
@@ -3303,7 +3308,7 @@
         <v>21</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>16</v>
@@ -3312,18 +3317,18 @@
         <v>27</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>45</v>
@@ -3333,53 +3338,53 @@
         <v>14</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>45</v>
@@ -3392,24 +3397,24 @@
         <v>40</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>21</v>
@@ -3421,30 +3426,30 @@
         <v>23</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
@@ -3453,30 +3458,30 @@
         <v>23</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>16</v>
@@ -3485,30 +3490,30 @@
         <v>23</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>16</v>
@@ -3517,18 +3522,18 @@
         <v>23</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>45</v>
@@ -3544,18 +3549,18 @@
         <v>27</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>21</v>
@@ -3563,13 +3568,13 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>21</v>
@@ -3577,13 +3582,13 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>21</v>
@@ -3591,13 +3596,13 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>21</v>
@@ -3605,13 +3610,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>21</v>
@@ -3619,13 +3624,13 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Add Associated Person for patients with family insurance
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1392,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E67" activeCellId="0" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2353,7 +2353,7 @@
         <v>168</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>169</v>
@@ -2603,7 +2603,7 @@
         <v>200</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>201</v>
@@ -3358,7 +3358,7 @@
         <v>312</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>313</v>

</xml_diff>

<commit_message>
added new Variable: _diagnostik_id
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC3C0F2-AD59-4C51-8FF2-8FA37FBD1BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,1073 +25,1057 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="344">
-  <si>
-    <t xml:space="preserve">Variable name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generation type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DWH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportmittel Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transportmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blutdruck_sys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postleitzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=01067-99998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsidentifikation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_iknr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=100000000-999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1000000000-9999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/id/@extension
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="345">
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Concept Id</t>
+  </si>
+  <si>
+    <t>Default values</t>
+  </si>
+  <si>
+    <t>Generation type</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Commentar</t>
+  </si>
+  <si>
+    <t>DWH</t>
+  </si>
+  <si>
+    <t>Cardinality</t>
+  </si>
+  <si>
+    <t>Pfad</t>
+  </si>
+  <si>
+    <t>Transportmittel Code</t>
+  </si>
+  <si>
+    <t>transportmittel</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>scope=1-4</t>
+  </si>
+  <si>
+    <t>generating</t>
+  </si>
+  <si>
+    <t>nullflavor</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t>blutdruck_sys</t>
+  </si>
+  <si>
+    <t>scope=0-300</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry herzfrequenz</t>
+  </si>
+  <si>
+    <t>herzfrequenz</t>
+  </si>
+  <si>
+    <t>0..n</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>postleitzahl</t>
+  </si>
+  <si>
+    <t>scope=01067-99998</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
+  </si>
+  <si>
+    <t>Versicherungsidentifikation</t>
+  </si>
+  <si>
+    <t>versicherung_iknr</t>
+  </si>
+  <si>
+    <t>scope=100000000-999999999</t>
+  </si>
+  <si>
+    <t>Blockweise</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedOrganisation/id/@extension</t>
+  </si>
+  <si>
+    <t>Organisation ID</t>
+  </si>
+  <si>
+    <t>organisation_id</t>
+  </si>
+  <si>
+    <t>scope=1000000000-9999999999</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/id/@extension
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/id/@extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Allergien spezifisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergien_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|Allergien|Antibiotika : |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verweise auf andere Allergien sollten hier gemacht werden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ersteinschaetzung_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|triageval|5|triageval|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste Verweise auf triageEVAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Körpertemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kerntemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0.0-45.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UUID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/setId/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo Schwangerschaftsstatus code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schwangerschaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kein Fehler bei Gender Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS verbale Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_verbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung Codesystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.276.0.76.5.438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[1.2.276.0.76.5.438]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ManchesterTriageSystem ist default Wieso überhaupt speichern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dokument_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geburtsdatum patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geburtsdatum_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19960531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=19200101;end_date=20200730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerdedauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">symptomdauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_ranking_skala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rankin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1-6)?</t>
+    <t>Allergien spezifisch</t>
+  </si>
+  <si>
+    <t>allergien_txt</t>
+  </si>
+  <si>
+    <t>|Allergien|Antibiotika : |</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Verweise auf andere Allergien sollten hier gemacht werden</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung text</t>
+  </si>
+  <si>
+    <t>ersteinschaetzung_text</t>
+  </si>
+  <si>
+    <t>|triageval|5|triageval|</t>
+  </si>
+  <si>
+    <t>Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Körpertemperatur</t>
+  </si>
+  <si>
+    <t>kerntemperatur</t>
+  </si>
+  <si>
+    <t>0.335</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>scope=0.0-45.0</t>
+  </si>
+  <si>
+    <t>Version ID</t>
+  </si>
+  <si>
+    <t>version_id</t>
+  </si>
+  <si>
+    <t>0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/setId/@extension</t>
+  </si>
+  <si>
+    <t>Basisinfo Schwangerschaftsstatus code</t>
+  </si>
+  <si>
+    <t>schwangerschaft</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>scope=0-1</t>
+  </si>
+  <si>
+    <t>generting</t>
+  </si>
+  <si>
+    <t>Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS verbale Antwort</t>
+  </si>
+  <si>
+    <t>gcs_verbal</t>
+  </si>
+  <si>
+    <t>scope=1-5</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung Codesystem</t>
+  </si>
+  <si>
+    <t>triage_system</t>
+  </si>
+  <si>
+    <t>1.2.276.0.76.5.438</t>
+  </si>
+  <si>
+    <t>value_set=[1.2.276.0.76.5.438]</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>ManchesterTriageSystem ist default Wieso überhaupt speichern</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/id/@extension</t>
+  </si>
+  <si>
+    <t>Document ID</t>
+  </si>
+  <si>
+    <t>dokument_id</t>
+  </si>
+  <si>
+    <t>14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/id/@extension</t>
+  </si>
+  <si>
+    <t>Geburtsdatum patient</t>
+  </si>
+  <si>
+    <t>geburtsdatum_ts</t>
+  </si>
+  <si>
+    <t>19960531</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerdedauer</t>
+  </si>
+  <si>
+    <t>symptomdauer</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>scope=0-99</t>
+  </si>
+  <si>
+    <t>1..n</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
+  </si>
+  <si>
+    <t>Basisinfo_ranking_skala</t>
+  </si>
+  <si>
+    <t>rankin</t>
+  </si>
+  <si>
+    <t>scope=0-6</t>
+  </si>
+  <si>
+    <t>(1-6)?</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text </t>
   </si>
   <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS Augenöffnen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_augen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erstellung durch Author zeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">author_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117160900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/time/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum der DokumentErstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datum_erstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117163300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201501171650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Beginn der Symptome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerde_begin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Patientenkontakt Ankunfszeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aufnahme_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118070100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Therapiebeginn, Aufnahme, Behandlung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">therapiebeginn_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118071200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Begin des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118073500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ende des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118075100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verlegungs-/Entlassungszeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118083000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
+    <t>Vitalparameter Entry GCS Augenöffnen</t>
+  </si>
+  <si>
+    <t>gcs_augen</t>
+  </si>
+  <si>
+    <t>Erstellung durch Author zeit</t>
+  </si>
+  <si>
+    <t>author_ts</t>
+  </si>
+  <si>
+    <t>20150117160900</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/time/@value</t>
+  </si>
+  <si>
+    <t>Datum der DokumentErstellung</t>
+  </si>
+  <si>
+    <t>datum_erstellung</t>
+  </si>
+  <si>
+    <t>20150117163300</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t>diagnostik_ts</t>
+  </si>
+  <si>
+    <t>201501171650</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>Blockweise Generieren</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Beginn der Symptome</t>
+  </si>
+  <si>
+    <t>beschwerde_begin</t>
+  </si>
+  <si>
+    <t>20150118</t>
+  </si>
+  <si>
+    <t>format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Start Patientenkontakt Ankunfszeit</t>
+  </si>
+  <si>
+    <t>aufnahme_ts</t>
+  </si>
+  <si>
+    <t>20150118070100</t>
+  </si>
+  <si>
+    <t>startunkt</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Therapiebeginn, Aufnahme, Behandlung</t>
+  </si>
+  <si>
+    <t>therapiebeginn_ts</t>
+  </si>
+  <si>
+    <t>20150118071200</t>
+  </si>
+  <si>
+    <t>Begin des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118073500</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmmss</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
+  </si>
+  <si>
+    <t>Ende des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>end_arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118075100</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
+  </si>
+  <si>
+    <t>Verlegungs-/Entlassungszeitpunkt</t>
+  </si>
+  <si>
+    <t>entlassung_ts</t>
+  </si>
+  <si>
+    <t>20150118083000</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
 ClinicalDocument/componentOf/encompassingEncounter/effectiveTime/high/@value</t>
   </si>
   <si>
-    <t xml:space="preserve">Ersteinschätzung zeit start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung zeit ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Code Welche Untersuchung?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37637-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=diagnostik.csv;column=diagnostik_code</t>
+    <t>Ersteinschätzung zeit start</t>
+  </si>
+  <si>
+    <t>triage_ts_start</t>
+  </si>
+  <si>
+    <t>202006201603</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmm</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung zeit ende</t>
+  </si>
+  <si>
+    <t>triage_ts_end</t>
+  </si>
+  <si>
+    <t>202006201608</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Code</t>
+  </si>
+  <si>
+    <t>cedis</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>link=cedis.csv;column=cedis</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Diagnostik Code Welche Untersuchung?</t>
+  </si>
+  <si>
+    <t>diagnostik_code</t>
+  </si>
+  <si>
+    <t>37637-6</t>
+  </si>
+  <si>
+    <t>link=diagnostik.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
   </si>
   <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo multiresistente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3MRGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EntlassungsGrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beide Systeme haben 1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS motorische Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_motorisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Sauerstoffsättigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saettigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry  Schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Glasgoe Coma Scale Summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=3-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality, Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahme ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">987654321-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regex=\d{9}-\d\d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t>Basisinfo multiresistente</t>
+  </si>
+  <si>
+    <t>keime</t>
+  </si>
+  <si>
+    <t>3MRGN</t>
+  </si>
+  <si>
+    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t>EntlassungsGrund</t>
+  </si>
+  <si>
+    <t>entlassung</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>scope=1-6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung code</t>
+  </si>
+  <si>
+    <t>triage</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Atemfrequenz</t>
+  </si>
+  <si>
+    <t>atemfrequenz</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS motorische Antwort</t>
+  </si>
+  <si>
+    <t>gcs_motorisch</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Sauerstoffsättigung</t>
+  </si>
+  <si>
+    <t>saettigung</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>scope=0-100</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry  Schmerzskala</t>
+  </si>
+  <si>
+    <t>schmerzskala</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>scope=0-10</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Glasgoe Coma Scale Summe</t>
+  </si>
+  <si>
+    <t>gcs_summe</t>
+  </si>
+  <si>
+    <t>scope=3-15</t>
+  </si>
+  <si>
+    <t>Cardinality, Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert)</t>
+  </si>
+  <si>
+    <t>Aufnahme ID</t>
+  </si>
+  <si>
+    <t>encounter_id</t>
+  </si>
+  <si>
+    <t>987654321-04</t>
+  </si>
+  <si>
+    <t>regex=\d{9}-\d\d</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
   </si>
   <si>
     <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
   </si>
   <si>
-    <t xml:space="preserve">beschwerde_liste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ-Verschlechterung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verweise auf andere…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text/content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[B, D, A]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notfallanamnese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notfallanamnese</t>
+    <t>beschwerde_liste</t>
+  </si>
+  <si>
+    <t>AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t>Verweise auf andere…</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (links)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_links</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>value_set=[B, D, A]</t>
+  </si>
+  <si>
+    <t>Notfallanamnese</t>
+  </si>
+  <si>
+    <t>notfallanamnese</t>
   </si>
   <si>
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t xml:space="preserve">ChatGPT Text gnerierung aus allen Parametern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[D, M, C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Address Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dachauer Straße 112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=streets.csv;column=street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genreating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abschlussdiagnose Freitext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chatGPT text aus Beschwerde code generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. med.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde originaltext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerden_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durchfall und Erbrechen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_display_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extremity X-ray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[true,false]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antibiotikaallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_antibiotika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tetanusschutz_text</t>
+    <t>ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (links)</t>
+  </si>
+  <si>
+    <t>pupillenweite_links</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>value_set=[D, M, C]</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenweite_rechts</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_rechts</t>
+  </si>
+  <si>
+    <t>Street Address Line</t>
+  </si>
+  <si>
+    <t>street_address_line</t>
+  </si>
+  <si>
+    <t>Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t>link=streets.csv;column=street_address_line</t>
+  </si>
+  <si>
+    <t>genreating</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
+  </si>
+  <si>
+    <t>Abschlussdiagnose Freitext</t>
+  </si>
+  <si>
+    <t>diagnose_txt</t>
+  </si>
+  <si>
+    <t>Distorsion unteres Sprunggelenk (S96.3)</t>
+  </si>
+  <si>
+    <t>chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t>Author prefix</t>
+  </si>
+  <si>
+    <t>prefix_author</t>
+  </si>
+  <si>
+    <t>Dr. med.</t>
+  </si>
+  <si>
+    <t>value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
+  </si>
+  <si>
+    <t>Beschwerde originaltext</t>
+  </si>
+  <si>
+    <t>beschwerden_txt</t>
+  </si>
+  <si>
+    <t>Durchfall und Erbrechen</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
+  </si>
+  <si>
+    <t>Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t>diagnostik_display_name</t>
+  </si>
+  <si>
+    <t>Extremity X-ray</t>
+  </si>
+  <si>
+    <t>Blockweise Diagnostik REMOVE</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t>Basisinfo_tetanusschutz</t>
+  </si>
+  <si>
+    <t>tetanusschutz</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>value_set=[true,false]</t>
+  </si>
+  <si>
+    <t>Antibiotikaallergie</t>
+  </si>
+  <si>
+    <t>allergie_antibiotika</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
+  </si>
+  <si>
+    <t>tetanusschutz_text</t>
   </si>
   <si>
     <t xml:space="preserve">Ja </t>
   </si>
   <si>
-    <t xml:space="preserve">String_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keine Validierung von Neg Ind (da kann alles drinn stehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kicker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=family_names.csv;column=family_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuweisung Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zuweisung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KVNDAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[M,F,UN]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=first_names.csv;column=first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">München</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=cities.csv;column=city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Ergebnis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ergebnis_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[PB, OPB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regensburger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik ganzer Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S93.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valueset?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungs Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selbstzahler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zusammen mit Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsfall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insurance_case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedEntity/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
+    <t>String_test</t>
+  </si>
+  <si>
+    <t>Keine Validierung von Neg Ind (da kann alles drinn stehen</t>
+  </si>
+  <si>
+    <t>Patient family name</t>
+  </si>
+  <si>
+    <t>family_patient</t>
+  </si>
+  <si>
+    <t>Kicker</t>
+  </si>
+  <si>
+    <t>link=family_names.csv;column=family_name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
+  </si>
+  <si>
+    <t>Zuweisung Code</t>
+  </si>
+  <si>
+    <t>zuweisung</t>
+  </si>
+  <si>
+    <t>KVNDAK</t>
+  </si>
+  <si>
+    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>value_set=[M,F,UN]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
+  </si>
+  <si>
+    <t>Author given name</t>
+  </si>
+  <si>
+    <t>given_author</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>link=first_names.csv;column=first_name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>München</t>
+  </si>
+  <si>
+    <t>link=cities.csv;column=city</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
+  </si>
+  <si>
+    <t>Diagnostik Ergebnis</t>
+  </si>
+  <si>
+    <t>diagnostik_ergebnis_code</t>
+  </si>
+  <si>
+    <t>OPB</t>
+  </si>
+  <si>
+    <t>value_set=[PB, OPB]</t>
+  </si>
+  <si>
+    <t>Author family name</t>
+  </si>
+  <si>
+    <t>family_author</t>
+  </si>
+  <si>
+    <t>Regensburger</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
+  </si>
+  <si>
+    <t>Diagnostik ganzer Text</t>
+  </si>
+  <si>
+    <t>diagnostik_text</t>
+  </si>
+  <si>
+    <t>Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE</t>
+  </si>
+  <si>
+    <t>diagnose_code</t>
+  </si>
+  <si>
+    <t>S93.6</t>
+  </si>
+  <si>
+    <t>Valueset?</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
+  </si>
+  <si>
+    <t>Versicherungs Name</t>
+  </si>
+  <si>
+    <t>versicherung_txt</t>
+  </si>
+  <si>
+    <t>Selbstzahler</t>
+  </si>
+  <si>
+    <t>zusammen mit Block</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedOrganisation/name</t>
+  </si>
+  <si>
+    <t>Versicherungsfall</t>
+  </si>
+  <si>
+    <t>insurance_case</t>
+  </si>
+  <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>value_set=[FAMDEP,SELF]</t>
+  </si>
+  <si>
+    <t>If FAMDEP then AssociatedPerson</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
+  </si>
+  <si>
+    <t>Organisation name</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
+    <t>Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/name
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/name</t>
   </si>
   <si>
-    <t xml:space="preserve">Patient given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergien vorhanden?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality;nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kontrastmittelallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality,Nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonstige allergien vorhanden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_sonstige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=10-120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_arztkontakt_endarztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_endarztkontakt_entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_entlassung_triagestart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_triagestart_triageend</t>
+    <t>Patient given name</t>
+  </si>
+  <si>
+    <t>given_patient</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
+  </si>
+  <si>
+    <t>Allergien vorhanden?</t>
+  </si>
+  <si>
+    <t>allergie</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Cardinality;nullflavor</t>
+  </si>
+  <si>
+    <t>Kontrastmittelallergie</t>
+  </si>
+  <si>
+    <t>allergie_kontrastmittel</t>
+  </si>
+  <si>
+    <t>Cardinality,Nullflavor</t>
+  </si>
+  <si>
+    <t>sonstige allergien vorhanden</t>
+  </si>
+  <si>
+    <t>allergie_sonstige</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE originalText</t>
+  </si>
+  <si>
+    <t>diagnose_name</t>
+  </si>
+  <si>
+    <t>Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
+  </si>
+  <si>
+    <t>_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t>scope=10-120</t>
+  </si>
+  <si>
+    <t>_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t>_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t>_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t>_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t>_triagestart_triageend</t>
+  </si>
+  <si>
+    <t>_diagnostik_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1096,7 +1085,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1127,7 +1116,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1135,133 +1124,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145f82"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e87331"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186c24"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1293,7 +1239,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1317,7 +1263,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1377,41 +1323,40 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="66.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="66.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="112.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="9"/>
+    <col min="1" max="1" width="30.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="66.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="112.75" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1443,14 +1388,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1472,14 +1417,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1504,14 +1449,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1536,14 +1481,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1568,14 +1513,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="2">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1597,14 +1542,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="2">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1623,7 +1568,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1650,7 +1595,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1677,7 +1622,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1709,7 +1654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1735,7 +1680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
@@ -1767,7 +1712,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
         <v>71</v>
       </c>
@@ -1799,7 +1744,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -1828,7 +1773,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -1857,7 +1802,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -1884,7 +1829,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>91</v>
       </c>
@@ -1910,7 +1855,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
@@ -1939,7 +1884,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -1971,7 +1916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -2003,7 +1948,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>110</v>
       </c>
@@ -2029,7 +1974,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -2058,7 +2003,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>119</v>
       </c>
@@ -2090,7 +2035,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>125</v>
       </c>
@@ -2119,7 +2064,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>130</v>
       </c>
@@ -2148,7 +2093,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>135</v>
       </c>
@@ -2174,7 +2119,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>138</v>
       </c>
@@ -2200,7 +2145,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>143</v>
       </c>
@@ -2226,7 +2171,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="1" t="s">
         <v>147</v>
       </c>
@@ -2252,7 +2197,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>151</v>
       </c>
@@ -2278,7 +2223,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>156</v>
       </c>
@@ -2304,7 +2249,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
@@ -2336,7 +2281,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>165</v>
       </c>
@@ -2368,7 +2313,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>171</v>
       </c>
@@ -2400,7 +2345,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>175</v>
       </c>
@@ -2429,7 +2374,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>180</v>
       </c>
@@ -2458,7 +2403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>184</v>
       </c>
@@ -2490,7 +2435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
         <v>187</v>
       </c>
@@ -2522,7 +2467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>190</v>
       </c>
@@ -2554,7 +2499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>194</v>
       </c>
@@ -2586,7 +2531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>198</v>
       </c>
@@ -2618,7 +2563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>202</v>
       </c>
@@ -2644,7 +2589,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>207</v>
       </c>
@@ -2670,7 +2615,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:10">
       <c r="A44" s="6" t="s">
         <v>212</v>
       </c>
@@ -2702,7 +2647,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>216</v>
       </c>
@@ -2725,7 +2670,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:10">
       <c r="A46" s="6" t="s">
         <v>220</v>
       </c>
@@ -2757,7 +2702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:10">
       <c r="A47" s="6" t="s">
         <v>224</v>
       </c>
@@ -2789,7 +2734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
         <v>227</v>
       </c>
@@ -2821,7 +2766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
         <v>229</v>
       </c>
@@ -2853,7 +2798,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
         <v>235</v>
       </c>
@@ -2883,7 +2828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
         <v>239</v>
       </c>
@@ -2909,7 +2854,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
         <v>244</v>
       </c>
@@ -2933,7 +2878,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
         <v>248</v>
       </c>
@@ -2963,7 +2908,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
         <v>253</v>
       </c>
@@ -2995,7 +2940,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>257</v>
       </c>
@@ -3027,7 +2972,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
         <v>253</v>
       </c>
@@ -3057,7 +3002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
         <v>264</v>
       </c>
@@ -3086,7 +3031,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
         <v>269</v>
       </c>
@@ -3118,7 +3063,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
         <v>274</v>
       </c>
@@ -3147,7 +3092,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
         <v>279</v>
       </c>
@@ -3173,7 +3118,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
         <v>284</v>
       </c>
@@ -3205,7 +3150,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
         <v>289</v>
       </c>
@@ -3237,7 +3182,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
         <v>293</v>
       </c>
@@ -3263,7 +3208,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
         <v>297</v>
       </c>
@@ -3290,7 +3235,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:10">
       <c r="A65" s="1" t="s">
         <v>300</v>
       </c>
@@ -3320,7 +3265,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:10">
       <c r="A66" s="1" t="s">
         <v>305</v>
       </c>
@@ -3347,7 +3292,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:10">
       <c r="A67" s="1" t="s">
         <v>310</v>
       </c>
@@ -3376,7 +3321,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:10">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3400,7 +3345,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:10">
       <c r="A69" s="1" t="s">
         <v>321</v>
       </c>
@@ -3429,7 +3374,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="s">
         <v>325</v>
       </c>
@@ -3461,7 +3406,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:10">
       <c r="A71" s="1" t="s">
         <v>329</v>
       </c>
@@ -3493,7 +3438,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:10">
       <c r="A72" s="1" t="s">
         <v>332</v>
       </c>
@@ -3525,7 +3470,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:10">
       <c r="A73" s="1" t="s">
         <v>334</v>
       </c>
@@ -3552,7 +3497,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:10">
       <c r="B74" s="1" t="s">
         <v>337</v>
       </c>
@@ -3566,7 +3511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:10">
       <c r="B75" s="1" t="s">
         <v>339</v>
       </c>
@@ -3580,7 +3525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:10">
       <c r="B76" s="1" t="s">
         <v>340</v>
       </c>
@@ -3594,7 +3539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:10">
       <c r="B77" s="1" t="s">
         <v>341</v>
       </c>
@@ -3608,7 +3553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:10">
       <c r="B78" s="1" t="s">
         <v>342</v>
       </c>
@@ -3622,7 +3567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:10">
       <c r="B79" s="1" t="s">
         <v>343</v>
       </c>
@@ -3636,13 +3581,16 @@
         <v>21</v>
       </c>
     </row>
+    <row r="80" spans="1:10">
+      <c r="B80" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
associated Person in Excel eingefügt nicht mehr in dependencies; added docs in dependencies
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC3C0F2-AD59-4C51-8FF2-8FA37FBD1BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888AC91-12B0-4F21-A313-8B71418984E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="347">
   <si>
     <t>Variable name</t>
   </si>
@@ -1063,6 +1063,12 @@
   </si>
   <si>
     <t>_diagnostik_id</t>
+  </si>
+  <si>
+    <t>_associatedPerson_given</t>
+  </si>
+  <si>
+    <t>_associatedPerson_family</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K80"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -3589,8 +3595,33 @@
         <v>45</v>
       </c>
     </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
XSLT prüfen und Variablen überarbeiten bis tetanus
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0683AFA-21DF-45E5-8414-9A70882EEC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE29702-780E-43A1-AF31-094411762D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="356">
   <si>
     <t>Variable name</t>
   </si>
@@ -611,9 +612,6 @@
     <t>scope=3-15</t>
   </si>
   <si>
-    <t>Cardinality, Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert)</t>
-  </si>
-  <si>
     <t>Aufnahme ID</t>
   </si>
   <si>
@@ -638,9 +636,6 @@
     <t>AZ-Verschlechterung</t>
   </si>
   <si>
-    <t>Verweise auf andere…</t>
-  </si>
-  <si>
     <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
   </si>
   <si>
@@ -707,9 +702,6 @@
     <t>link=streets.csv;column=street_address_line</t>
   </si>
   <si>
-    <t>genreating</t>
-  </si>
-  <si>
     <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
   </si>
   <si>
@@ -788,18 +780,6 @@
     <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
   </si>
   <si>
-    <t>tetanusschutz_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja </t>
-  </si>
-  <si>
-    <t>String_test</t>
-  </si>
-  <si>
-    <t>Keine Validierung von Neg Ind (da kann alles drinn stehen</t>
-  </si>
-  <si>
     <t>Patient family name</t>
   </si>
   <si>
@@ -915,9 +895,6 @@
   </si>
   <si>
     <t>S93.6</t>
-  </si>
-  <si>
-    <t>Valueset?</t>
   </si>
   <si>
     <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
@@ -1101,6 +1078,27 @@
   </si>
   <si>
     <t xml:space="preserve">	Multiresistenter Keim Ja/Nein/Verdacht; wenn angegeben soll, dass der in observation.value angegebene Keim NICHT vorliegt, wird observation.@negationInd="true" gesetzt. Bei "Verdacht" ist der Befundstatus in observation.value.qualifier entsprechend zu setzen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
+  </si>
+  <si>
+    <t>Verweise auf Beschwerde</t>
+  </si>
+  <si>
+    <t>ist 0..1 in doku soll aber immer da sein</t>
+  </si>
+  <si>
+    <t>Auf Diagnose abstimmen</t>
+  </si>
+  <si>
+    <t>NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
   </si>
 </sst>
 </file>
@@ -1391,15 +1389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
@@ -1430,13 +1428,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -1468,7 +1466,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -1615,13 +1613,13 @@
         <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1651,7 +1649,7 @@
         <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>38</v>
@@ -1804,7 +1802,7 @@
         <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -1850,7 +1848,7 @@
         <v>60</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>22</v>
@@ -1873,7 +1871,7 @@
         <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1998,7 +1996,7 @@
         <v>94</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>21</v>
@@ -2041,7 +2039,7 @@
         <v>60</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>16</v>
@@ -2175,7 +2173,7 @@
         <v>60</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>16</v>
@@ -2201,7 +2199,7 @@
         <v>121</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>21</v>
@@ -2371,7 +2369,7 @@
         <v>23</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>16</v>
@@ -2405,7 +2403,7 @@
         <v>60</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>16</v>
@@ -2439,7 +2437,7 @@
         <v>23</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>38</v>
@@ -2465,7 +2463,7 @@
         <v>156</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>14</v>
@@ -2535,7 +2533,7 @@
         <v>167</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -2545,7 +2543,7 @@
         <v>23</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>16</v>
@@ -2570,11 +2568,16 @@
       <c r="E35" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>15</v>
       </c>
@@ -2606,6 +2609,9 @@
         <v>21</v>
       </c>
       <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>176</v>
       </c>
@@ -2636,9 +2642,11 @@
       <c r="G37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I37" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>8</v>
@@ -2670,9 +2678,11 @@
       <c r="G38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I38" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>8</v>
@@ -2704,9 +2714,11 @@
       <c r="G39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I39" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>8</v>
@@ -2738,9 +2750,11 @@
       <c r="G40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I40" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>8</v>
@@ -2772,12 +2786,14 @@
       <c r="G41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I41" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>194</v>
+        <v>349</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>22</v>
@@ -2788,41 +2804,46 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>43</v>
@@ -2831,39 +2852,46 @@
         <v>21</v>
       </c>
       <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J43" s="1" t="s">
-        <v>203</v>
+        <v>350</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I44" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>15</v>
@@ -2877,13 +2905,13 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>43</v>
@@ -2892,8 +2920,11 @@
         <v>21</v>
       </c>
       <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J45" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>50</v>
@@ -2901,27 +2932,31 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>214</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I46" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>15</v>
@@ -2935,27 +2970,31 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>214</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J47" s="6" t="s">
         <v>15</v>
@@ -2969,27 +3008,31 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="G48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H48" s="1"/>
+      <c r="H48" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I48" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="J48" s="6" t="s">
         <v>15</v>
@@ -3003,47 +3046,46 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H49" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="K49" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>43</v>
@@ -3055,10 +3097,10 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>16</v>
@@ -3069,67 +3111,80 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="K51" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="G52" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="1"/>
+      <c r="I52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="K52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>43</v>
@@ -3144,32 +3199,34 @@
         <v>27</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F54" s="1"/>
+        <v>246</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
       </c>
@@ -3178,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>15</v>
+        <v>355</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>16</v>
@@ -3189,19 +3246,19 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
@@ -3218,96 +3275,95 @@
         <v>16</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="K56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" s="1"/>
+      <c r="E57" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="9"/>
       <c r="I57" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9" t="s">
+      <c r="E58" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H58" s="9"/>
-      <c r="I58" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="H58" s="1"/>
       <c r="J58" s="1" t="s">
         <v>15</v>
       </c>
@@ -3315,173 +3371,170 @@
         <v>16</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H59" s="1"/>
-      <c r="J59" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="K59" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>281</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H62" s="1"/>
-      <c r="I62" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="K62" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>67</v>
+        <v>282</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>260</v>
-      </c>
+      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H63" s="1"/>
+      <c r="I63" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="K63" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>289</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>43</v>
@@ -3491,26 +3544,31 @@
       <c r="G64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H64" s="1"/>
+      <c r="H64" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I64" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="J64" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="K64" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>100</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>291</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>43</v>
@@ -3518,154 +3576,156 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H65" s="1"/>
-      <c r="I65" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="J65" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="H66" s="1"/>
       <c r="J66" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>306</v>
-      </c>
+      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="H67" s="1"/>
-      <c r="J67" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="K67" s="1" t="s">
-        <v>308</v>
+        <v>38</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="1"/>
+      <c r="E68" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H68" s="1"/>
+      <c r="I68" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="K68" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="J69" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="K69" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>317</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3676,30 +3736,30 @@
         <v>23</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
@@ -3710,87 +3770,72 @@
         <v>23</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="B73" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H73" s="1"/>
-      <c r="I73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>297</v>
-      </c>
     </row>
     <row r="74" spans="1:12">
       <c r="B74" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -3800,13 +3845,13 @@
     </row>
     <row r="75" spans="1:12">
       <c r="B75" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -3816,13 +3861,13 @@
     </row>
     <row r="76" spans="1:12">
       <c r="B76" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -3832,13 +3877,13 @@
     </row>
     <row r="77" spans="1:12">
       <c r="B77" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -3848,13 +3893,13 @@
     </row>
     <row r="78" spans="1:12">
       <c r="B78" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -3864,55 +3909,39 @@
     </row>
     <row r="79" spans="1:12">
       <c r="B79" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H79" s="1"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="80" spans="1:12">
       <c r="B80" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E80" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H80" s="1"/>
     </row>
     <row r="81" spans="2:8">
       <c r="B81" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="2:8">
-      <c r="B82" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H82" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
XSLT prüfen und Variablen überarbeiten fertig
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE29702-780E-43A1-AF31-094411762D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EAFBE5-3579-4D71-AF8E-2B2B38BA2E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="368">
   <si>
     <t>Variable name</t>
   </si>
@@ -161,9 +161,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>Verweise auf andere Allergien sollten hier gemacht werden</t>
-  </si>
-  <si>
     <t>ClinicalDicument/component/structuredBody/component/section/text</t>
   </si>
   <si>
@@ -909,9 +906,6 @@
     <t>Selbstzahler</t>
   </si>
   <si>
-    <t>zusammen mit Block</t>
-  </si>
-  <si>
     <t>ClinicalDocument/participant/associatedOrganisation/name</t>
   </si>
   <si>
@@ -928,9 +922,6 @@
   </si>
   <si>
     <t>If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
@@ -970,16 +961,10 @@
     <t>true</t>
   </si>
   <si>
-    <t>Cardinality;nullflavor</t>
-  </si>
-  <si>
     <t>Kontrastmittelallergie</t>
   </si>
   <si>
     <t>allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t>Cardinality,Nullflavor</t>
   </si>
   <si>
     <t>sonstige allergien vorhanden</t>
@@ -1099,13 +1084,64 @@
   </si>
   <si>
     <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
+  </si>
+  <si>
+    <t>mindestens eine Allergy obsseration muss da sein</t>
+  </si>
+  <si>
+    <t>Sonstige Allergien sollten hier genannt werden</t>
+  </si>
+  <si>
+    <t>diagnostik_labor</t>
+  </si>
+  <si>
+    <t>diagnostik_blutgase</t>
+  </si>
+  <si>
+    <t>diagnostik_urinschnelltest</t>
+  </si>
+  <si>
+    <t>diagnostik_ekg</t>
+  </si>
+  <si>
+    <t>diagnostik_sonographie</t>
+  </si>
+  <si>
+    <t>diagnostik_echokardiographie</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_kopf</t>
+  </si>
+  <si>
+    <t>diagnostik_ct</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_trauma</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_wirbelsaeule</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_thorax</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_becken</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_extremitaeten</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_sonstiges</t>
+  </si>
+  <si>
+    <t>diagnostik_mrt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1156,6 +1192,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1178,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -1195,6 +1237,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1389,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1428,13 +1471,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -1466,7 +1509,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -1475,7 +1518,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
@@ -1508,7 +1551,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="1" t="s">
@@ -1542,7 +1585,7 @@
         <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="1" t="s">
@@ -1613,13 +1656,13 @@
         <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1649,7 +1692,7 @@
         <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>38</v>
@@ -1678,27 +1721,27 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>44</v>
+        <v>352</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>43</v>
@@ -1710,33 +1753,33 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
@@ -1746,7 +1789,7 @@
         <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>8</v>
@@ -1760,82 +1803,82 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1845,33 +1888,33 @@
         <v>23</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1879,24 +1922,24 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1910,27 +1953,27 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1939,30 +1982,30 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -1970,65 +2013,65 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -2036,27 +2079,27 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -2072,64 +2115,64 @@
         <v>23</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
@@ -2137,30 +2180,30 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
@@ -2170,66 +2213,66 @@
         <v>23</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2240,63 +2283,63 @@
         <v>23</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2304,30 +2347,30 @@
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
@@ -2335,30 +2378,30 @@
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
@@ -2369,30 +2412,30 @@
         <v>23</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
@@ -2400,33 +2443,33 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="360">
       <c r="A31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
@@ -2437,40 +2480,40 @@
         <v>23</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>15</v>
@@ -2479,24 +2522,24 @@
         <v>16</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="1" t="s">
@@ -2507,33 +2550,33 @@
         <v>27</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -2543,33 +2586,33 @@
         <v>23</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
@@ -2585,24 +2628,24 @@
         <v>16</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
@@ -2610,10 +2653,10 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>16</v>
@@ -2624,19 +2667,19 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
@@ -2646,7 +2689,7 @@
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>8</v>
@@ -2660,19 +2703,19 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
@@ -2682,7 +2725,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>8</v>
@@ -2691,24 +2734,24 @@
         <v>22</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
@@ -2718,7 +2761,7 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>8</v>
@@ -2732,19 +2775,19 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
@@ -2754,7 +2797,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>8</v>
@@ -2768,19 +2811,19 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
@@ -2790,10 +2833,10 @@
         <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>22</v>
@@ -2804,26 +2847,26 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>27</v>
@@ -2832,18 +2875,18 @@
         <v>16</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>43</v>
@@ -2853,36 +2896,36 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="C44" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
@@ -2891,7 +2934,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>15</v>
@@ -2905,13 +2948,13 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>43</v>
@@ -2921,33 +2964,33 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
@@ -2956,7 +2999,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>15</v>
@@ -2970,22 +3013,22 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>14</v>
@@ -2994,7 +3037,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J47" s="6" t="s">
         <v>15</v>
@@ -3008,22 +3051,22 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>219</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>14</v>
@@ -3032,7 +3075,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J48" s="6" t="s">
         <v>15</v>
@@ -3046,19 +3089,19 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -3074,18 +3117,18 @@
         <v>38</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>43</v>
@@ -3097,40 +3140,40 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>23</v>
@@ -3139,52 +3182,52 @@
         <v>38</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>43</v>
@@ -3192,40 +3235,40 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
@@ -3235,64 +3278,63 @@
         <v>23</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I55" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
@@ -3300,30 +3342,30 @@
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9" t="s">
@@ -3331,92 +3373,92 @@
       </c>
       <c r="H57" s="9"/>
       <c r="I57" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="J58" s="1" t="s">
-        <v>15</v>
+      <c r="I58" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H59" s="1"/>
+      <c r="I59" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="K59" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
@@ -3432,24 +3474,24 @@
         <v>38</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
@@ -3460,52 +3502,55 @@
         <v>27</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H62" s="1"/>
+      <c r="I62" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K62" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>43</v>
@@ -3517,58 +3562,60 @@
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="G64" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>43</v>
@@ -3576,59 +3623,62 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H65" s="1"/>
-      <c r="J65" s="1" t="s">
-        <v>293</v>
+      <c r="I65" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="H66" s="1"/>
+      <c r="I66" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="J66" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>300</v>
+        <v>38</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>43</v>
@@ -3638,29 +3688,34 @@
       <c r="G67" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H67" s="1"/>
+      <c r="H67" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K67" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -3674,152 +3729,156 @@
         <v>38</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I69" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>313</v>
+        <v>351</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>316</v>
+        <v>59</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I71" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J71" s="1" t="s">
-        <v>316</v>
+        <v>59</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
+      <c r="F72" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="G72" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I72" s="1" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="B73" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3829,13 +3888,13 @@
     </row>
     <row r="74" spans="1:12">
       <c r="B74" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -3845,13 +3904,13 @@
     </row>
     <row r="75" spans="1:12">
       <c r="B75" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -3861,13 +3920,13 @@
     </row>
     <row r="76" spans="1:12">
       <c r="B76" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -3877,13 +3936,13 @@
     </row>
     <row r="77" spans="1:12">
       <c r="B77" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -3893,13 +3952,13 @@
     </row>
     <row r="78" spans="1:12">
       <c r="B78" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -3909,7 +3968,7 @@
     </row>
     <row r="79" spans="1:12">
       <c r="B79" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>43</v>
@@ -3917,13 +3976,13 @@
     </row>
     <row r="80" spans="1:12">
       <c r="B80" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
@@ -3933,7 +3992,7 @@
     </row>
     <row r="81" spans="2:8">
       <c r="B81" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>43</v>
@@ -3942,6 +4001,81 @@
         <v>21</v>
       </c>
       <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="2:8">
+      <c r="B82" s="12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8">
+      <c r="B83" s="12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8">
+      <c r="B84" s="12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8">
+      <c r="B85" s="12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8">
+      <c r="B86" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8">
+      <c r="B87" s="12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8">
+      <c r="B88" s="12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8">
+      <c r="B89" s="12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8">
+      <c r="B91" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8">
+      <c r="B92" s="12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8">
+      <c r="B93" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8">
+      <c r="B94" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8">
+      <c r="B95" s="12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8">
+      <c r="B96" s="12" t="s">
+        <v>367</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Dignostik alle Felder in XSLT
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EAFBE5-3579-4D71-AF8E-2B2B38BA2E04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD59D233-53A5-4535-953B-05C3976E383A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="369">
   <si>
     <t>Variable name</t>
   </si>
@@ -1135,6 +1135,9 @@
   </si>
   <si>
     <t>diagnostik_mrt</t>
+  </si>
+  <si>
+    <t>String_test</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -4006,75 +4009,165 @@
       <c r="B82" s="12" t="s">
         <v>353</v>
       </c>
+      <c r="C82" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="83" spans="2:8">
       <c r="B83" s="12" t="s">
         <v>354</v>
       </c>
+      <c r="C83" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="84" spans="2:8">
       <c r="B84" s="12" t="s">
         <v>355</v>
       </c>
+      <c r="C84" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="85" spans="2:8">
       <c r="B85" s="12" t="s">
         <v>356</v>
       </c>
+      <c r="C85" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="86" spans="2:8">
       <c r="B86" s="12" t="s">
         <v>357</v>
       </c>
+      <c r="C86" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="87" spans="2:8">
       <c r="B87" s="12" t="s">
         <v>358</v>
       </c>
+      <c r="C87" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="88" spans="2:8">
       <c r="B88" s="12" t="s">
         <v>359</v>
       </c>
+      <c r="C88" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="89" spans="2:8">
       <c r="B89" s="12" t="s">
         <v>360</v>
       </c>
+      <c r="C89" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="90" spans="2:8">
       <c r="B90" s="12" t="s">
         <v>361</v>
       </c>
+      <c r="C90" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="91" spans="2:8">
       <c r="B91" s="12" t="s">
         <v>362</v>
       </c>
+      <c r="C91" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="92" spans="2:8">
       <c r="B92" s="12" t="s">
         <v>363</v>
       </c>
+      <c r="C92" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="93" spans="2:8">
       <c r="B93" s="12" t="s">
         <v>364</v>
       </c>
+      <c r="C93" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="12" t="s">
         <v>365</v>
       </c>
+      <c r="C94" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="12" t="s">
         <v>366</v>
       </c>
+      <c r="C95" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="96" spans="2:8">
       <c r="B96" s="12" t="s">
         <v>367</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dignostik implementiert und refactoring
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD59D233-53A5-4535-953B-05C3976E383A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4046C973-D5D0-48B6-AD93-2251F1272085}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="369">
   <si>
     <t>Variable name</t>
   </si>
@@ -1137,7 +1137,7 @@
     <t>diagnostik_mrt</t>
   </si>
   <si>
-    <t>String_test</t>
+    <t>value_set=[PB,OPB,ND]</t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="2:8">
+    <row r="81" spans="2:12">
       <c r="B81" s="1" t="s">
         <v>326</v>
       </c>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="2:8">
+    <row r="82" spans="2:12">
       <c r="B82" s="12" t="s">
         <v>353</v>
       </c>
@@ -4013,10 +4013,19 @@
         <v>276</v>
       </c>
       <c r="D82" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="83" spans="2:8">
+      <c r="G82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L82" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12">
       <c r="B83" s="12" t="s">
         <v>354</v>
       </c>
@@ -4024,10 +4033,19 @@
         <v>276</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="84" spans="2:8">
+      <c r="G83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L83" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12">
       <c r="B84" s="12" t="s">
         <v>355</v>
       </c>
@@ -4035,10 +4053,19 @@
         <v>276</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="85" spans="2:8">
+      <c r="G84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L84" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12">
       <c r="B85" s="12" t="s">
         <v>356</v>
       </c>
@@ -4046,10 +4073,19 @@
         <v>276</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="86" spans="2:8">
+      <c r="G85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L85" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12">
       <c r="B86" s="12" t="s">
         <v>357</v>
       </c>
@@ -4057,10 +4093,19 @@
         <v>276</v>
       </c>
       <c r="D86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="87" spans="2:8">
+      <c r="G86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L86" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12">
       <c r="B87" s="12" t="s">
         <v>358</v>
       </c>
@@ -4068,10 +4113,19 @@
         <v>276</v>
       </c>
       <c r="D87" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="88" spans="2:8">
+      <c r="G87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L87" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12">
       <c r="B88" s="12" t="s">
         <v>359</v>
       </c>
@@ -4079,10 +4133,19 @@
         <v>276</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="89" spans="2:8">
+      <c r="G88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L88" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12">
       <c r="B89" s="12" t="s">
         <v>360</v>
       </c>
@@ -4090,10 +4153,19 @@
         <v>276</v>
       </c>
       <c r="D89" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="90" spans="2:8">
+      <c r="G89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L89" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12">
       <c r="B90" s="12" t="s">
         <v>361</v>
       </c>
@@ -4101,10 +4173,19 @@
         <v>276</v>
       </c>
       <c r="D90" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="91" spans="2:8">
+      <c r="G90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L90" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12">
       <c r="B91" s="12" t="s">
         <v>362</v>
       </c>
@@ -4112,10 +4193,19 @@
         <v>276</v>
       </c>
       <c r="D91" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="92" spans="2:8">
+      <c r="G91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L91" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12">
       <c r="B92" s="12" t="s">
         <v>363</v>
       </c>
@@ -4123,10 +4213,19 @@
         <v>276</v>
       </c>
       <c r="D92" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="93" spans="2:8">
+      <c r="G92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L92" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12">
       <c r="B93" s="12" t="s">
         <v>364</v>
       </c>
@@ -4134,10 +4233,19 @@
         <v>276</v>
       </c>
       <c r="D93" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="94" spans="2:8">
+      <c r="G93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L93" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12">
       <c r="B94" s="12" t="s">
         <v>365</v>
       </c>
@@ -4145,10 +4253,19 @@
         <v>276</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="95" spans="2:8">
+      <c r="G94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L94" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12">
       <c r="B95" s="12" t="s">
         <v>366</v>
       </c>
@@ -4156,10 +4273,19 @@
         <v>276</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="96" spans="2:8">
+      <c r="G95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L95" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12">
       <c r="B96" s="12" t="s">
         <v>367</v>
       </c>
@@ -4167,7 +4293,16 @@
         <v>276</v>
       </c>
       <c r="D96" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>368</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L96" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nullflavors implementiert für alle die einen Nullflavor haben
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC613C4-2154-45FF-B48A-248F8E23503D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEF5EDD-02DC-453A-95CF-A7015DB59DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="359">
   <si>
     <t>Variable name</t>
   </si>
@@ -976,9 +976,6 @@
     <t>_associatedPerson_family</t>
   </si>
   <si>
-    <t>Nullflavor</t>
-  </si>
-  <si>
     <t>OTH,NA</t>
   </si>
   <si>
@@ -1104,6 +1101,12 @@
   </si>
   <si>
     <t>Diagnostik Befund Oder Durchführung</t>
+  </si>
+  <si>
+    <t>NullFlavor</t>
+  </si>
+  <si>
+    <t>Nur NA implementiert</t>
   </si>
 </sst>
 </file>
@@ -1403,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1440,13 +1443,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>315</v>
+        <v>357</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -1478,16 +1481,19 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>358</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
@@ -1625,13 +1631,13 @@
         <v>26</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1661,7 +1667,7 @@
         <v>26</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>37</v>
@@ -1693,7 +1699,7 @@
         <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>15</v>
@@ -1812,10 +1818,10 @@
         <v>63</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
@@ -1858,7 +1864,7 @@
         <v>58</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>21</v>
@@ -1881,7 +1887,7 @@
         <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -2006,7 +2012,7 @@
         <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>20</v>
@@ -2049,7 +2055,7 @@
         <v>58</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>15</v>
@@ -2183,7 +2189,7 @@
         <v>58</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>15</v>
@@ -2209,7 +2215,7 @@
         <v>117</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>20</v>
@@ -2379,7 +2385,7 @@
         <v>22</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>15</v>
@@ -2413,7 +2419,7 @@
         <v>58</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>15</v>
@@ -2447,7 +2453,7 @@
         <v>22</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>37</v>
@@ -2473,10 +2479,10 @@
         <v>152</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
@@ -2540,17 +2546,17 @@
         <v>163</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>15</v>
@@ -2576,10 +2582,10 @@
         <v>167</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
@@ -2789,7 +2795,7 @@
         <v>58</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>21</v>
@@ -2852,7 +2858,7 @@
         <v>58</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>15</v>
@@ -2878,10 +2884,10 @@
         <v>202</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>22</v>
@@ -2941,10 +2947,10 @@
         <v>210</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>22</v>
@@ -2977,10 +2983,10 @@
         <v>210</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>22</v>
@@ -3013,10 +3019,10 @@
         <v>202</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>22</v>
@@ -3145,7 +3151,7 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>20</v>
@@ -3155,7 +3161,7 @@
         <v>58</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>37</v>
@@ -3181,17 +3187,17 @@
         <v>237</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>15</v>
@@ -3465,7 +3471,7 @@
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>20</v>
@@ -3477,7 +3483,7 @@
         <v>58</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>15</v>
@@ -3638,7 +3644,7 @@
         <v>58</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>15</v>
@@ -3728,7 +3734,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>20</v>
@@ -3740,7 +3746,7 @@
         <v>58</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>37</v>
@@ -3878,10 +3884,10 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>266</v>
@@ -3890,7 +3896,7 @@
         <v>42</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>14</v>
@@ -3901,10 +3907,10 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>266</v>
@@ -3913,7 +3919,7 @@
         <v>42</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>14</v>
@@ -3924,10 +3930,10 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>266</v>
@@ -3936,7 +3942,7 @@
         <v>42</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>14</v>
@@ -3947,10 +3953,10 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>266</v>
@@ -3959,7 +3965,7 @@
         <v>42</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>14</v>
@@ -3970,10 +3976,10 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>266</v>
@@ -3982,7 +3988,7 @@
         <v>42</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>14</v>
@@ -3993,10 +3999,10 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>266</v>
@@ -4005,7 +4011,7 @@
         <v>42</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>14</v>
@@ -4016,10 +4022,10 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>266</v>
@@ -4028,7 +4034,7 @@
         <v>42</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>14</v>
@@ -4039,10 +4045,10 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>266</v>
@@ -4051,7 +4057,7 @@
         <v>42</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>14</v>
@@ -4062,10 +4068,10 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>266</v>
@@ -4074,7 +4080,7 @@
         <v>42</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>14</v>
@@ -4085,10 +4091,10 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>266</v>
@@ -4097,7 +4103,7 @@
         <v>42</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>14</v>
@@ -4108,10 +4114,10 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>266</v>
@@ -4120,7 +4126,7 @@
         <v>42</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>14</v>
@@ -4131,10 +4137,10 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>266</v>
@@ -4143,7 +4149,7 @@
         <v>42</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>14</v>
@@ -4154,10 +4160,10 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>266</v>
@@ -4166,7 +4172,7 @@
         <v>42</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>14</v>
@@ -4177,10 +4183,10 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>266</v>
@@ -4189,7 +4195,7 @@
         <v>42</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>14</v>
@@ -4200,10 +4206,10 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>266</v>
@@ -4212,7 +4218,7 @@
         <v>42</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Add NullFlavor support for Transportmittel
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="371">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -64,34 +64,37 @@
     <t xml:space="preserve">transportmittel</t>
   </si>
   <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[1,2,3,4,OTH]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH,NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blutdruck_sys</t>
+  </si>
+  <si>
     <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH,NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blutdruck_sys</t>
   </si>
   <si>
     <t xml:space="preserve">scope=0-300</t>
@@ -170,9 +173,6 @@
     <t xml:space="preserve">|Allergien|Antibiotika : |</t>
   </si>
   <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sonstige Allergien sollten hier genannt werden</t>
   </si>
   <si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t xml:space="preserve">gcs_augen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-4</t>
   </si>
   <si>
     <t xml:space="preserve">Erstellung durch Author zeit</t>
@@ -1576,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1680,14 +1683,14 @@
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -1697,31 +1700,31 @@
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -1731,27 +1734,27 @@
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
@@ -1768,24 +1771,24 @@
         <v>20</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1795,33 +1798,33 @@
         <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1831,30 +1834,30 @@
         <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>17</v>
@@ -1884,7 +1887,7 @@
         <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>17</v>
@@ -1896,7 +1899,7 @@
         <v>55</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>56</v>
@@ -1921,7 +1924,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
@@ -1933,10 +1936,10 @@
         <v>8</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,14 +1956,14 @@
         <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>66</v>
@@ -1977,7 +1980,7 @@
         <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>70</v>
@@ -2013,14 +2016,14 @@
         <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>18</v>
@@ -2032,7 +2035,7 @@
         <v>77</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>78</v>
@@ -2049,13 +2052,13 @@
         <v>81</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>19</v>
@@ -2079,13 +2082,13 @@
         <v>86</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>19</v>
@@ -2112,13 +2115,13 @@
         <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>91</v>
@@ -2142,7 +2145,7 @@
         <v>96</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>19</v>
@@ -2166,7 +2169,7 @@
         <v>100</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>101</v>
@@ -2175,7 +2178,7 @@
         <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>19</v>
@@ -2201,13 +2204,13 @@
         <v>100</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>105</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>19</v>
@@ -2234,14 +2237,14 @@
         <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>18</v>
@@ -2251,7 +2254,7 @@
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>78</v>
@@ -2259,82 +2262,82 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
@@ -2347,100 +2350,100 @@
         <v>19</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>19</v>
@@ -2452,27 +2455,27 @@
         <v>20</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>19</v>
@@ -2481,88 +2484,88 @@
         <v>20</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M27" s="3"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M28" s="3"/>
     </row>
     <row r="29" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M29" s="3"/>
     </row>
     <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>17</v>
@@ -2571,31 +2574,31 @@
         <v>19</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M30" s="3"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>17</v>
@@ -2604,34 +2607,34 @@
         <v>18</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>17</v>
@@ -2641,67 +2644,67 @@
         <v>19</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>17</v>
@@ -2711,7 +2714,7 @@
         <v>18</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>20</v>
@@ -2722,22 +2725,22 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>17</v>
@@ -2747,39 +2750,39 @@
         <v>18</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>20</v>
@@ -2791,23 +2794,23 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>18</v>
@@ -2819,31 +2822,31 @@
         <v>8</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>18</v>
@@ -2855,7 +2858,7 @@
         <v>8</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>78</v>
@@ -2863,23 +2866,23 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>18</v>
@@ -2891,31 +2894,31 @@
         <v>8</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>18</v>
@@ -2927,31 +2930,31 @@
         <v>8</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>18</v>
@@ -2960,93 +2963,93 @@
         <v>19</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>71</v>
@@ -3061,37 +3064,37 @@
         <v>19</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>56</v>
@@ -3099,19 +3102,19 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>71</v>
@@ -3126,30 +3129,30 @@
         <v>19</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>71</v>
@@ -3164,30 +3167,30 @@
         <v>19</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>71</v>
@@ -3202,34 +3205,34 @@
         <v>19</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>18</v>
@@ -3238,33 +3241,33 @@
         <v>18</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>20</v>
@@ -3276,118 +3279,118 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M52" s="3"/>
     </row>
     <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>17</v>
@@ -3397,7 +3400,7 @@
         <v>18</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>20</v>
@@ -3408,19 +3411,19 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
@@ -3436,54 +3439,54 @@
         <v>20</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11" t="s">
@@ -3497,24 +3500,24 @@
         <v>20</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>17</v>
@@ -3526,59 +3529,59 @@
         <v>20</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M58" s="3"/>
     </row>
     <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>18</v>
@@ -3587,36 +3590,36 @@
         <v>18</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>20</v>
@@ -3628,55 +3631,55 @@
     </row>
     <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M62" s="3"/>
     </row>
     <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>107</v>
@@ -3685,25 +3688,25 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>18</v>
@@ -3712,30 +3715,30 @@
         <v>19</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>19</v>
@@ -3744,58 +3747,58 @@
         <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M65" s="3"/>
     </row>
     <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M66" s="3"/>
     </row>
     <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>18</v>
@@ -3804,62 +3807,62 @@
         <v>19</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M67" s="3"/>
     </row>
     <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>18</v>
@@ -3868,34 +3871,34 @@
         <v>19</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>18</v>
@@ -3907,28 +3910,28 @@
         <v>20</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>18</v>
@@ -3940,28 +3943,28 @@
         <v>20</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>18</v>
@@ -3970,310 +3973,310 @@
         <v>19</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="6" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add NullFlavors for Diagnose ICD10 and function with statistics
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="370">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -962,25 +962,7 @@
     <t xml:space="preserve">S93.6</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">link=icd10gm2023.csv;column=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen</t>
-    </r>
+    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen</t>
   </si>
   <si>
     <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
@@ -1111,9 +1093,6 @@
   </si>
   <si>
     <t xml:space="preserve">diagnostik_labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String_test</t>
   </si>
   <si>
     <t xml:space="preserve">diagnostik_blutgase</t>
@@ -1166,7 +1145,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1223,12 +1202,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1579,8 +1552,8 @@
   </sheetPr>
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E64" activeCellId="0" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4122,161 +4095,251 @@
         <v>299</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mehrere Diagnosen mit Qualifier added
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47480AD-7E29-4193-A46B-522025844DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,1153 +25,1146 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="370">
-  <si>
-    <t xml:space="preserve">Variable name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generation type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Block Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DWH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportmittel Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transportmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[1,2,3,4,OTH]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH,NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blutdruck_sys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postleitzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=01067-99998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsidentifikation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_iknr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=100000000-999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise mit Versicherungsnamen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1000000000-9999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kinda sus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/id/@extension
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="374">
+  <si>
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Concept Id</t>
+  </si>
+  <si>
+    <t>Default values</t>
+  </si>
+  <si>
+    <t>Generation type</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Nullflavor</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Block Cardinality</t>
+  </si>
+  <si>
+    <t>Cardinality</t>
+  </si>
+  <si>
+    <t>Commentar</t>
+  </si>
+  <si>
+    <t>DWH</t>
+  </si>
+  <si>
+    <t>Pfad</t>
+  </si>
+  <si>
+    <t>Transportmittel Code</t>
+  </si>
+  <si>
+    <t>transportmittel</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>value_set=[1,2,3,4,OTH]</t>
+  </si>
+  <si>
+    <t>OTH,NA</t>
+  </si>
+  <si>
+    <t>generating</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t>blutdruck_sys</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>scope=0-300</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry herzfrequenz</t>
+  </si>
+  <si>
+    <t>herzfrequenz</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>postleitzahl</t>
+  </si>
+  <si>
+    <t>scope=01067-99998</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
+  </si>
+  <si>
+    <t>Versicherungsidentifikation</t>
+  </si>
+  <si>
+    <t>versicherung_iknr</t>
+  </si>
+  <si>
+    <t>scope=100000000-999999999</t>
+  </si>
+  <si>
+    <t>0..n</t>
+  </si>
+  <si>
+    <t>Blockweise mit Versicherungsnamen</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
+  </si>
+  <si>
+    <t>Organisation ID</t>
+  </si>
+  <si>
+    <t>organisation_id</t>
+  </si>
+  <si>
+    <t>scope=1000000000-9999999999</t>
+  </si>
+  <si>
+    <t>kinda sus</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/id/@extension
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/id/@extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Allergien spezifisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergien_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|Allergien|Antibiotika : |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonstige Allergien sollten hier genannt werden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ersteinschaetzung_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|triageval|5|triageval|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste Verweise auf triageEVAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Körpertemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kerntemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0.0-45.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UUID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/setId/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo Schwangerschaftsstatus code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schwangerschaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kein Fehler bei Gender Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS verbale Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_verbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was Bei Summe, wenn einer fehlt?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung Codesystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.276.0.76.5.438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dokument_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geburtsdatum patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geburtsdatum_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19960531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=19200101;end_date=20200730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerdedauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">symptomdauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_ranking_skala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rankin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valueset(1-6)?</t>
+    <t>Allergien spezifisch</t>
+  </si>
+  <si>
+    <t>allergien_txt</t>
+  </si>
+  <si>
+    <t>|Allergien|Antibiotika : |</t>
+  </si>
+  <si>
+    <t>Sonstige Allergien sollten hier genannt werden</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung text</t>
+  </si>
+  <si>
+    <t>ersteinschaetzung_text</t>
+  </si>
+  <si>
+    <t>|triageval|5|triageval|</t>
+  </si>
+  <si>
+    <t>Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Körpertemperatur</t>
+  </si>
+  <si>
+    <t>kerntemperatur</t>
+  </si>
+  <si>
+    <t>0.335</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>scope=0.0-45.0</t>
+  </si>
+  <si>
+    <t>Version ID</t>
+  </si>
+  <si>
+    <t>version_id</t>
+  </si>
+  <si>
+    <t>0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/setId/@extension</t>
+  </si>
+  <si>
+    <t>Basisinfo Schwangerschaftsstatus code</t>
+  </si>
+  <si>
+    <t>schwangerschaft</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>scope=0-1</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS verbale Antwort</t>
+  </si>
+  <si>
+    <t>gcs_verbal</t>
+  </si>
+  <si>
+    <t>scope=1-5</t>
+  </si>
+  <si>
+    <t>Was Bei Summe, wenn einer fehlt?</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung Codesystem</t>
+  </si>
+  <si>
+    <t>triage_system</t>
+  </si>
+  <si>
+    <t>1.2.276.0.76.5.438</t>
+  </si>
+  <si>
+    <t>value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/id/@extension</t>
+  </si>
+  <si>
+    <t>Document ID</t>
+  </si>
+  <si>
+    <t>dokument_id</t>
+  </si>
+  <si>
+    <t>14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/id/@extension</t>
+  </si>
+  <si>
+    <t>Geburtsdatum patient</t>
+  </si>
+  <si>
+    <t>geburtsdatum_ts</t>
+  </si>
+  <si>
+    <t>19960531</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerdedauer</t>
+  </si>
+  <si>
+    <t>symptomdauer</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>scope=0-99</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
+  </si>
+  <si>
+    <t>Basisinfo_ranking_skala</t>
+  </si>
+  <si>
+    <t>rankin</t>
+  </si>
+  <si>
+    <t>scope=0-6</t>
+  </si>
+  <si>
+    <t>Valueset(1-6)?</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text </t>
   </si>
   <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS Augenöffnen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_augen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erstellung durch Author zeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">author_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117160900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/time/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum der DokumentErstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datum_erstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117163300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201501171650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik !!!!!!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Beginn der Symptome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerde_begin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Patientenkontakt Ankunfszeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aufnahme_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118070100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Therapiebeginn, Aufnahme, Behandlung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">therapiebeginn_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118071200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Begin des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118073500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ende des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118075100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verlegungs-/Entlassungszeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118083000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O..1 =&gt; Problem mit Dependency Triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
+    <t>Vitalparameter Entry GCS Augenöffnen</t>
+  </si>
+  <si>
+    <t>gcs_augen</t>
+  </si>
+  <si>
+    <t>scope=1-4</t>
+  </si>
+  <si>
+    <t>Erstellung durch Author zeit</t>
+  </si>
+  <si>
+    <t>author_ts</t>
+  </si>
+  <si>
+    <t>20150117160900</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>1..n</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/time/@value</t>
+  </si>
+  <si>
+    <t>Datum der DokumentErstellung</t>
+  </si>
+  <si>
+    <t>datum_erstellung</t>
+  </si>
+  <si>
+    <t>20150117163300</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t>diagnostik_ts</t>
+  </si>
+  <si>
+    <t>201501171650</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>Diagnostik !!!!!!!!</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Beginn der Symptome</t>
+  </si>
+  <si>
+    <t>beschwerde_begin</t>
+  </si>
+  <si>
+    <t>20150118</t>
+  </si>
+  <si>
+    <t>format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Start Patientenkontakt Ankunfszeit</t>
+  </si>
+  <si>
+    <t>aufnahme_ts</t>
+  </si>
+  <si>
+    <t>20150118070100</t>
+  </si>
+  <si>
+    <t>startunkt</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Therapiebeginn, Aufnahme, Behandlung</t>
+  </si>
+  <si>
+    <t>therapiebeginn_ts</t>
+  </si>
+  <si>
+    <t>20150118071200</t>
+  </si>
+  <si>
+    <t>Begin des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118073500</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmmss</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
+  </si>
+  <si>
+    <t>Ende des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>end_arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118075100</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
+  </si>
+  <si>
+    <t>Verlegungs-/Entlassungszeitpunkt</t>
+  </si>
+  <si>
+    <t>entlassung_ts</t>
+  </si>
+  <si>
+    <t>20150118083000</t>
+  </si>
+  <si>
+    <t>O..1 =&gt; Problem mit Dependency Triage</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
 ClinicalDocument/componentOf/encompassingEncounter/effectiveTime/high/@value</t>
   </si>
   <si>
-    <t xml:space="preserve">Ersteinschätzung zeit start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">format=yyyymmddhhmm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nach entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung zeit ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
+    <t>Ersteinschätzung zeit start</t>
+  </si>
+  <si>
+    <t>triage_ts_start</t>
+  </si>
+  <si>
+    <t>202006201603</t>
+  </si>
+  <si>
+    <t>format=yyyymmddhhmm</t>
+  </si>
+  <si>
+    <t>nach entlassung</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung zeit ende</t>
+  </si>
+  <si>
+    <t>triage_ts_end</t>
+  </si>
+  <si>
+    <t>202006201608</t>
+  </si>
+  <si>
+    <t>effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
 Beispiel: Für Gesundheitsdienstleister, die einen Patienten heute in der Klinik sehen anamenstisch einen Herzinfarkt erheben, der vor fünf Jahren stattgefunden hat, ist effectiveTime: vor fünf Jahren.
 Die effectiveTime hier ist die definitive Angabe, ob die zugrunde liegende Erkrankung behoben ist. effectiveTime.low ist der Beginn des Problems für den Patienten. Wenn das Problem noch nicht gelöst ist, wird effectiveTime.high nicht gesetzt. Wenn bekannt ist, dass das Problem gelöst werden kann, dann ist effectiveTime.high vorhanden. Wenn der genaue Zeitpunkt der Lösung des Problems nicht bekannt ist, dann ist effectiveTime.high vorhanden und auf nullFlavor "UNK" gesetzt.</t>
   </si>
   <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH,UNK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Code Welche Untersuchung?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37637-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=diagnostik.csv;column=diagnostik_code</t>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Code</t>
+  </si>
+  <si>
+    <t>cedis</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>link=cedis.csv;column=cedis</t>
+  </si>
+  <si>
+    <t>OTH,UNK</t>
+  </si>
+  <si>
+    <t>nullflavor</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Diagnostik Code Welche Untersuchung?</t>
+  </si>
+  <si>
+    <t>diagnostik_code</t>
+  </si>
+  <si>
+    <t>37637-6</t>
+  </si>
+  <si>
+    <t>link=diagnostik.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
   </si>
   <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo multiresistente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3MRGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH</t>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t>Basisinfo multiresistente</t>
+  </si>
+  <si>
+    <t>keime</t>
+  </si>
+  <si>
+    <t>3MRGN</t>
+  </si>
+  <si>
+    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t>OTH</t>
   </si>
   <si>
     <t xml:space="preserve">	Multiresistenter Keim Ja/Nein/Verdacht; wenn angegeben soll, dass der in observation.value angegebene Keim NICHT vorliegt, wird observation.@negationInd="true" gesetzt. Bei "Verdacht" ist der Befundstatus in observation.value.qualifier entsprechend zu setzen.</t>
   </si>
   <si>
-    <t xml:space="preserve">EntlassungsGrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beide Systeme haben 1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS motorische Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_motorisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Sauerstoffsättigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saettigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry  Schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Glasgoe Coma Scale Summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=3-15</t>
+    <t>EntlassungsGrund</t>
+  </si>
+  <si>
+    <t>entlassung</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>scope=1-6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung code</t>
+  </si>
+  <si>
+    <t>triage</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Atemfrequenz</t>
+  </si>
+  <si>
+    <t>atemfrequenz</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS motorische Antwort</t>
+  </si>
+  <si>
+    <t>gcs_motorisch</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Sauerstoffsättigung</t>
+  </si>
+  <si>
+    <t>saettigung</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>scope=0-100</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry  Schmerzskala</t>
+  </si>
+  <si>
+    <t>schmerzskala</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>scope=0-10</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Glasgoe Coma Scale Summe</t>
+  </si>
+  <si>
+    <t>gcs_summe</t>
+  </si>
+  <si>
+    <t>scope=3-15</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
   </si>
   <si>
-    <t xml:space="preserve">Aufnahme ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">987654321-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regex=\d{9}-\d\d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
+    <t>Aufnahme ID</t>
+  </si>
+  <si>
+    <t>encounter_id</t>
+  </si>
+  <si>
+    <t>987654321-04</t>
+  </si>
+  <si>
+    <t>regex=\d{9}-\d\d</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
   </si>
   <si>
     <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
   </si>
   <si>
-    <t xml:space="preserve">beschwerde_liste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ-Verschlechterung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verweise auf Beschwerde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text/content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[B, D, A]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notfallanamnese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notfallanamnese</t>
+    <t>beschwerde_liste</t>
+  </si>
+  <si>
+    <t>AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t>Verweise auf Beschwerde</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (links)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_links</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>value_set=[B, D, A]</t>
+  </si>
+  <si>
+    <t>Notfallanamnese</t>
+  </si>
+  <si>
+    <t>notfallanamnese</t>
   </si>
   <si>
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t xml:space="preserve">ChatGPT Text gnerierung aus allen Parametern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[D, M, C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Address Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dachauer Straße 112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=streets.csv;column=street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abschlussdiagnose Freitext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chatGPT text aus Beschwerde code generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. med.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde originaltext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerden_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durchfall und Erbrechen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ist 0..1 in doku soll aber immer da sein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_display_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extremity X-ray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[true,false]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NI</t>
+    <t>ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (links)</t>
+  </si>
+  <si>
+    <t>pupillenweite_links</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>value_set=[D, M, C]</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenweite_rechts</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_rechts</t>
+  </si>
+  <si>
+    <t>Street Address Line</t>
+  </si>
+  <si>
+    <t>street_address_line</t>
+  </si>
+  <si>
+    <t>Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t>link=streets.csv;column=street_address_line</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
+  </si>
+  <si>
+    <t>Abschlussdiagnose Freitext</t>
+  </si>
+  <si>
+    <t>diagnose_txt</t>
+  </si>
+  <si>
+    <t>Distorsion unteres Sprunggelenk (S96.3)</t>
+  </si>
+  <si>
+    <t>chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t>Author prefix</t>
+  </si>
+  <si>
+    <t>prefix_author</t>
+  </si>
+  <si>
+    <t>Dr. med.</t>
+  </si>
+  <si>
+    <t>value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
+  </si>
+  <si>
+    <t>Beschwerde originaltext</t>
+  </si>
+  <si>
+    <t>beschwerden_txt</t>
+  </si>
+  <si>
+    <t>Durchfall und Erbrechen</t>
+  </si>
+  <si>
+    <t>ist 0..1 in doku soll aber immer da sein</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
+  </si>
+  <si>
+    <t>Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t>diagnostik_display_name</t>
+  </si>
+  <si>
+    <t>Extremity X-ray</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Blockweise Diagnostik REMOVE</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t>Basisinfo_tetanusschutz</t>
+  </si>
+  <si>
+    <t>tetanusschutz</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>value_set=[true,false]</t>
+  </si>
+  <si>
+    <t>NI</t>
   </si>
   <si>
     <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
   </si>
   <si>
-    <t xml:space="preserve">Antibiotikaallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_antibiotika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kicker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=family_names.csv;column=family_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuweisung Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zuweisung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KVNDAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[M,F,UN]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=first_names.csv;column=first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">München</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=cities.csv;column=city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Ergebnis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ergebnis_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[PB, OPB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regensburger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik ganzer Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S93.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungs Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selbstzahler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsfall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insurance_case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedEntity/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
+    <t>Antibiotikaallergie</t>
+  </si>
+  <si>
+    <t>allergie_antibiotika</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
+  </si>
+  <si>
+    <t>Patient family name</t>
+  </si>
+  <si>
+    <t>family_patient</t>
+  </si>
+  <si>
+    <t>Kicker</t>
+  </si>
+  <si>
+    <t>link=family_names.csv;column=family_name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
+  </si>
+  <si>
+    <t>Zuweisung Code</t>
+  </si>
+  <si>
+    <t>zuweisung</t>
+  </si>
+  <si>
+    <t>KVNDAK</t>
+  </si>
+  <si>
+    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>value_set=[M,F,UN]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
+  </si>
+  <si>
+    <t>Author given name</t>
+  </si>
+  <si>
+    <t>given_author</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>link=first_names.csv;column=first_name</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>München</t>
+  </si>
+  <si>
+    <t>link=cities.csv;column=city</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
+  </si>
+  <si>
+    <t>Diagnostik Ergebnis</t>
+  </si>
+  <si>
+    <t>diagnostik_ergebnis_code</t>
+  </si>
+  <si>
+    <t>OPB</t>
+  </si>
+  <si>
+    <t>value_set=[PB, OPB]</t>
+  </si>
+  <si>
+    <t>Blockweise Generieren</t>
+  </si>
+  <si>
+    <t>Author family name</t>
+  </si>
+  <si>
+    <t>family_author</t>
+  </si>
+  <si>
+    <t>Regensburger</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
+  </si>
+  <si>
+    <t>Diagnostik ganzer Text</t>
+  </si>
+  <si>
+    <t>diagnostik_text</t>
+  </si>
+  <si>
+    <t>Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE</t>
+  </si>
+  <si>
+    <t>diagnose_code</t>
+  </si>
+  <si>
+    <t>S93.6</t>
+  </si>
+  <si>
+    <t>NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
+  </si>
+  <si>
+    <t>Versicherungs Name</t>
+  </si>
+  <si>
+    <t>versicherung_txt</t>
+  </si>
+  <si>
+    <t>Selbstzahler</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedOrganisation/name</t>
+  </si>
+  <si>
+    <t>Versicherungsfall</t>
+  </si>
+  <si>
+    <t>insurance_case</t>
+  </si>
+  <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>value_set=[FAMDEP,SELF]</t>
+  </si>
+  <si>
+    <t>If FAMDEP then AssociatedPerson</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
+  </si>
+  <si>
+    <t>Organisation name</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
+    <t>Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/name
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/name</t>
   </si>
   <si>
-    <t xml:space="preserve">Patient given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergien vorhanden?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mindestens eine Allergy obsseration muss da sein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kontrastmittelallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonstige allergien vorhanden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_sonstige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auf Diagnose abstimmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=10-120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_arztkontakt_endarztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_endarztkontakt_entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_entlassung_triagestart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_triagestart_triageend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_diagnostik_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_associatedPerson_given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_associatedPerson_family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_blutgase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_urinschnelltest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ekg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_sonographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_echokardiographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct_kopf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct_trauma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_wirbelsaeule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_thorax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_becken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_extremitaeten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_sonstiges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_mrt</t>
+    <t>Patient given name</t>
+  </si>
+  <si>
+    <t>given_patient</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
+  </si>
+  <si>
+    <t>Allergien vorhanden?</t>
+  </si>
+  <si>
+    <t>allergie</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>mindestens eine Allergy obsseration muss da sein</t>
+  </si>
+  <si>
+    <t>Kontrastmittelallergie</t>
+  </si>
+  <si>
+    <t>allergie_kontrastmittel</t>
+  </si>
+  <si>
+    <t>sonstige allergien vorhanden</t>
+  </si>
+  <si>
+    <t>allergie_sonstige</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE originalText</t>
+  </si>
+  <si>
+    <t>diagnose_name</t>
+  </si>
+  <si>
+    <t>Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
+  </si>
+  <si>
+    <t>Auf Diagnose abstimmen</t>
+  </si>
+  <si>
+    <t>_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t>scope=10-120</t>
+  </si>
+  <si>
+    <t>_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t>_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t>_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t>_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t>_triagestart_triageend</t>
+  </si>
+  <si>
+    <t>_diagnostik_id</t>
+  </si>
+  <si>
+    <t>_associatedPerson_given</t>
+  </si>
+  <si>
+    <t>_associatedPerson_family</t>
+  </si>
+  <si>
+    <t>diagnostik_labor</t>
+  </si>
+  <si>
+    <t>diagnostik_blutgase</t>
+  </si>
+  <si>
+    <t>diagnostik_urinschnelltest</t>
+  </si>
+  <si>
+    <t>diagnostik_ekg</t>
+  </si>
+  <si>
+    <t>diagnostik_sonographie</t>
+  </si>
+  <si>
+    <t>diagnostik_echokardiographie</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_kopf</t>
+  </si>
+  <si>
+    <t>diagnostik_ct</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_trauma</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_wirbelsaeule</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_thorax</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_becken</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_extremitaeten</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_sonstiges</t>
+  </si>
+  <si>
+    <t>diagnostik_mrt</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE Qualifier</t>
+  </si>
+  <si>
+    <t>diagnose_qualifier</t>
+  </si>
+  <si>
+    <t>value_set=[V,G,A,Z];number=3</t>
+  </si>
+  <si>
+    <t>number=3</t>
+  </si>
+  <si>
+    <t>link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1176,7 +1174,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1191,7 +1189,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -1215,7 +1213,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1223,93 +1221,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1368,60 +1307,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145f82"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e87331"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186c24"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1453,7 +1408,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1477,7 +1432,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1537,42 +1492,41 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E64" activeCellId="0" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="77.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="112.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
+    <col min="1" max="1" width="38.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="112.75" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1610,14 +1564,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1645,14 +1599,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1679,14 +1633,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1713,14 +1667,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1747,14 +1701,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="2">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1783,14 +1737,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="2">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1819,7 +1773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1832,9 +1786,12 @@
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1849,7 +1806,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1862,9 +1819,12 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1879,7 +1839,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1915,7 +1875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1942,7 +1902,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1978,7 +1938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:13">
       <c r="A13" s="6" t="s">
         <v>74</v>
       </c>
@@ -2014,7 +1974,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -2030,9 +1990,11 @@
       <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2044,7 +2006,7 @@
       </c>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2060,9 +2022,11 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2074,7 +2038,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -2087,9 +2051,12 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2101,7 +2068,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2117,9 +2084,11 @@
       <c r="E17" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2131,7 +2100,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2166,7 +2135,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2182,9 +2151,11 @@
       <c r="E19" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2199,7 +2170,7 @@
       </c>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:13">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -2233,7 +2204,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2266,7 +2237,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2282,9 +2253,11 @@
       <c r="E22" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2296,7 +2269,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -2332,7 +2305,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
@@ -2365,7 +2338,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>132</v>
       </c>
@@ -2381,9 +2354,11 @@
       <c r="E25" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2398,7 +2373,7 @@
       </c>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>137</v>
       </c>
@@ -2431,7 +2406,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>140</v>
       </c>
@@ -2447,9 +2422,11 @@
       <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2461,7 +2438,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -2477,9 +2454,11 @@
       <c r="E28" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2491,7 +2470,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:13" ht="30">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -2507,9 +2486,11 @@
       <c r="E29" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2524,7 +2505,7 @@
       </c>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -2540,9 +2521,11 @@
       <c r="E30" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2540,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" s="1" customFormat="true" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:13" ht="360">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -2573,9 +2556,11 @@
       <c r="E31" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
         <v>18</v>
       </c>
@@ -2590,7 +2575,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>165</v>
       </c>
@@ -2626,7 +2611,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:13" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>172</v>
       </c>
@@ -2660,7 +2645,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>178</v>
       </c>
@@ -2696,7 +2681,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -2732,7 +2717,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>189</v>
       </c>
@@ -2748,9 +2733,11 @@
       <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2765,7 +2752,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -2801,7 +2788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:13">
       <c r="A38" s="6" t="s">
         <v>196</v>
       </c>
@@ -2837,7 +2824,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>199</v>
       </c>
@@ -2873,7 +2860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
@@ -2909,7 +2896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>207</v>
       </c>
@@ -2945,7 +2932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
@@ -2978,7 +2965,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -3008,7 +2995,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:13">
       <c r="A44" s="6" t="s">
         <v>221</v>
       </c>
@@ -3046,7 +3033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -3073,7 +3060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:13">
       <c r="A46" s="6" t="s">
         <v>229</v>
       </c>
@@ -3111,7 +3098,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:13">
       <c r="A47" s="6" t="s">
         <v>233</v>
       </c>
@@ -3149,7 +3136,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:13">
       <c r="A48" s="6" t="s">
         <v>236</v>
       </c>
@@ -3187,7 +3174,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>238</v>
       </c>
@@ -3220,7 +3207,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
         <v>243</v>
       </c>
@@ -3233,9 +3220,12 @@
       <c r="D50" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>19</v>
       </c>
@@ -3250,7 +3240,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
         <v>247</v>
       </c>
@@ -3283,7 +3273,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
         <v>252</v>
       </c>
@@ -3296,12 +3286,14 @@
       <c r="D52" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>19</v>
       </c>
@@ -3316,7 +3308,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
         <v>257</v>
       </c>
@@ -3329,9 +3321,12 @@
       <c r="D53" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>38</v>
       </c>
@@ -3346,7 +3341,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>263</v>
       </c>
@@ -3382,7 +3377,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
         <v>269</v>
       </c>
@@ -3415,7 +3410,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
         <v>272</v>
       </c>
@@ -3431,9 +3426,11 @@
       <c r="E56" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>115</v>
       </c>
@@ -3445,7 +3442,7 @@
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
         <v>277</v>
       </c>
@@ -3476,7 +3473,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:13">
       <c r="A58" s="1" t="s">
         <v>282</v>
       </c>
@@ -3492,9 +3489,11 @@
       <c r="E58" s="1" t="s">
         <v>285</v>
       </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>19</v>
       </c>
@@ -3506,7 +3505,7 @@
       </c>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
         <v>287</v>
       </c>
@@ -3522,9 +3521,11 @@
       <c r="E59" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
@@ -3536,7 +3537,7 @@
       </c>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
         <v>292</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
         <v>297</v>
       </c>
@@ -3585,9 +3586,11 @@
       <c r="E61" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
         <v>38</v>
       </c>
@@ -3602,7 +3605,7 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:13">
       <c r="A62" s="1" t="s">
         <v>302</v>
       </c>
@@ -3618,9 +3621,11 @@
       <c r="E62" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
@@ -3632,7 +3637,7 @@
       </c>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
         <v>306</v>
       </c>
@@ -3645,9 +3650,12 @@
       <c r="D63" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
         <v>115</v>
       </c>
@@ -3659,7 +3667,7 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:13">
       <c r="A64" s="1" t="s">
         <v>309</v>
       </c>
@@ -3673,7 +3681,7 @@
         <v>14</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>312</v>
+        <v>373</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>169</v>
@@ -3688,31 +3696,34 @@
         <v>19</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L64" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
         <v>19</v>
       </c>
@@ -3720,56 +3731,60 @@
         <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="M65" s="3"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="M65" s="3"/>
-    </row>
-    <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L66" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="M66" s="3"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="M66" s="3"/>
-    </row>
-    <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>26</v>
       </c>
@@ -3783,19 +3798,19 @@
         <v>45</v>
       </c>
       <c r="L67" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="M67" s="3"/>
-    </row>
-    <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>14</v>
@@ -3803,9 +3818,11 @@
       <c r="E68" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
@@ -3813,19 +3830,19 @@
         <v>45</v>
       </c>
       <c r="L68" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="M68" s="3"/>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="M68" s="3"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>14</v>
@@ -3844,7 +3861,7 @@
         <v>19</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>20</v>
@@ -3853,15 +3870,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="C70" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>14</v>
@@ -3886,15 +3903,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="C71" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>14</v>
@@ -3919,20 +3936,22 @@
         <v>271</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="D72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="F72" s="1" t="s">
         <v>71</v>
       </c>
@@ -3946,24 +3965,24 @@
         <v>19</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="B73" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3971,15 +3990,15 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:13">
       <c r="B74" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -3987,15 +4006,15 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:13">
       <c r="B75" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -4003,15 +4022,15 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:13">
       <c r="B76" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -4019,15 +4038,15 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:13">
       <c r="B77" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -4035,15 +4054,15 @@
       </c>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:13">
       <c r="B78" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -4051,17 +4070,17 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:13">
       <c r="B79" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="B80" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
@@ -4075,21 +4094,21 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="2:8">
       <c r="B81" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="2:8">
+      <c r="B82" s="6" t="s">
         <v>354</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="6" t="s">
-        <v>355</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>299</v>
@@ -4104,9 +4123,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="2:8">
       <c r="B83" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>299</v>
@@ -4121,9 +4140,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="2:8">
       <c r="B84" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>299</v>
@@ -4138,9 +4157,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="2:8">
       <c r="B85" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>299</v>
@@ -4155,9 +4174,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="2:8">
       <c r="B86" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>299</v>
@@ -4172,9 +4191,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="2:8">
       <c r="B87" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>299</v>
@@ -4189,9 +4208,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="2:8">
       <c r="B88" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>299</v>
@@ -4206,9 +4225,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="2:8">
       <c r="B89" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>299</v>
@@ -4223,9 +4242,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="2:8">
       <c r="B90" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>299</v>
@@ -4240,9 +4259,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="2:8">
       <c r="B91" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>299</v>
@@ -4257,9 +4276,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="2:8">
       <c r="B92" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>299</v>
@@ -4274,9 +4293,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="2:8">
       <c r="B93" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>299</v>
@@ -4291,9 +4310,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="2:8">
       <c r="B94" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>299</v>
@@ -4308,9 +4327,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="2:8">
       <c r="B95" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>299</v>
@@ -4325,9 +4344,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="2:8">
       <c r="B96" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>299</v>
@@ -4342,16 +4361,49 @@
         <v>71</v>
       </c>
     </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L32" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
+    <hyperlink ref="L32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change name and order of columns in cities.csv to clinics.csv with more focus on clinics
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47480AD-7E29-4193-A46B-522025844DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,1144 +22,1163 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="374">
   <si>
-    <t>Variable name</t>
-  </si>
-  <si>
-    <t>Concept Id</t>
-  </si>
-  <si>
-    <t>Default values</t>
-  </si>
-  <si>
-    <t>Generation type</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>Nullflavor</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Block Cardinality</t>
-  </si>
-  <si>
-    <t>Cardinality</t>
-  </si>
-  <si>
-    <t>Commentar</t>
-  </si>
-  <si>
-    <t>DWH</t>
-  </si>
-  <si>
-    <t>Pfad</t>
-  </si>
-  <si>
-    <t>Transportmittel Code</t>
-  </si>
-  <si>
-    <t>transportmittel</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>value_set=[1,2,3,4,OTH]</t>
-  </si>
-  <si>
-    <t>OTH,NA</t>
-  </si>
-  <si>
-    <t>generating</t>
-  </si>
-  <si>
-    <t>0..1</t>
-  </si>
-  <si>
-    <t>1..1</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t>blutdruck_sys</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>scope=0-300</t>
-  </si>
-  <si>
-    <t>implemented</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry herzfrequenz</t>
-  </si>
-  <si>
-    <t>herzfrequenz</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>postleitzahl</t>
-  </si>
-  <si>
-    <t>scope=01067-99998</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
-  </si>
-  <si>
-    <t>Versicherungsidentifikation</t>
-  </si>
-  <si>
-    <t>versicherung_iknr</t>
-  </si>
-  <si>
-    <t>scope=100000000-999999999</t>
-  </si>
-  <si>
-    <t>0..n</t>
-  </si>
-  <si>
-    <t>Blockweise mit Versicherungsnamen</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
-  </si>
-  <si>
-    <t>Organisation ID</t>
-  </si>
-  <si>
-    <t>organisation_id</t>
-  </si>
-  <si>
-    <t>scope=1000000000-9999999999</t>
-  </si>
-  <si>
-    <t>kinda sus</t>
-  </si>
-  <si>
-    <t>nein</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/representedOrganisation/id/@extension
+    <t xml:space="preserve">Variable name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generation type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nullflavor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block Cardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportmittel Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transportmittel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[1,2,3,4,OTH]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH,NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blutdruck_sys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry herzfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herzfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postal Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postleitzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=01067-99998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherung_iknr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=100000000-999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise mit Versicherungsnamen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organisation_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1000000000-9999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinda sus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/id/@extension
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/id/@extension</t>
   </si>
   <si>
-    <t>Allergien spezifisch</t>
-  </si>
-  <si>
-    <t>allergien_txt</t>
-  </si>
-  <si>
-    <t>|Allergien|Antibiotika : |</t>
-  </si>
-  <si>
-    <t>Sonstige Allergien sollten hier genannt werden</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t>Ersteinschätzung text</t>
-  </si>
-  <si>
-    <t>ersteinschaetzung_text</t>
-  </si>
-  <si>
-    <t>|triageval|5|triageval|</t>
-  </si>
-  <si>
-    <t>Liste Verweise auf triageEVAL</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Körpertemperatur</t>
-  </si>
-  <si>
-    <t>kerntemperatur</t>
-  </si>
-  <si>
-    <t>0.335</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>scope=0.0-45.0</t>
-  </si>
-  <si>
-    <t>Version ID</t>
-  </si>
-  <si>
-    <t>version_id</t>
-  </si>
-  <si>
-    <t>0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
-  </si>
-  <si>
-    <t>UUID</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/setId/@extension</t>
-  </si>
-  <si>
-    <t>Basisinfo Schwangerschaftsstatus code</t>
-  </si>
-  <si>
-    <t>schwangerschaft</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>scope=0-1</t>
-  </si>
-  <si>
-    <t>UNK</t>
-  </si>
-  <si>
-    <t>Kein Fehler bei Gender Male</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry GCS verbale Antwort</t>
-  </si>
-  <si>
-    <t>gcs_verbal</t>
-  </si>
-  <si>
-    <t>scope=1-5</t>
-  </si>
-  <si>
-    <t>Was Bei Summe, wenn einer fehlt?</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
-  </si>
-  <si>
-    <t>Ersteinschaetzung Codesystem</t>
-  </si>
-  <si>
-    <t>triage_system</t>
-  </si>
-  <si>
-    <t>1.2.276.0.76.5.438</t>
-  </si>
-  <si>
-    <t>value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
-  </si>
-  <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
-    <t>patient_id</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/id/@extension</t>
-  </si>
-  <si>
-    <t>Document ID</t>
-  </si>
-  <si>
-    <t>dokument_id</t>
-  </si>
-  <si>
-    <t>14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/id/@extension</t>
-  </si>
-  <si>
-    <t>Geburtsdatum patient</t>
-  </si>
-  <si>
-    <t>geburtsdatum_ts</t>
-  </si>
-  <si>
-    <t>19960531</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>format=yyyymmdd;start_date=19200101;end_date=20200730</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
-  </si>
-  <si>
-    <t>Beschwerdedauer</t>
-  </si>
-  <si>
-    <t>symptomdauer</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>scope=0-99</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
-  </si>
-  <si>
-    <t>Basisinfo_ranking_skala</t>
-  </si>
-  <si>
-    <t>rankin</t>
-  </si>
-  <si>
-    <t>scope=0-6</t>
-  </si>
-  <si>
-    <t>Valueset(1-6)?</t>
+    <t xml:space="preserve">Allergien spezifisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergien_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Allergien|Antibiotika : |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige Allergien sollten hier genannt werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschätzung text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ersteinschaetzung_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|triageval|5|triageval|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Körpertemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerntemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0.0-45.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/setId/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo Schwangerschaftsstatus code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schwangerschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry GCS verbale Antwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_verbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was Bei Summe, wenn einer fehlt?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschaetzung Codesystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.276.0.76.5.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dokument_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geburtsdatum patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geburtsdatum_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19960531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerdedauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symptomdauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo_ranking_skala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rankin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valueset(1-6)?</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text </t>
   </si>
   <si>
-    <t>Vitalparameter Entry GCS Augenöffnen</t>
-  </si>
-  <si>
-    <t>gcs_augen</t>
-  </si>
-  <si>
-    <t>scope=1-4</t>
-  </si>
-  <si>
-    <t>Erstellung durch Author zeit</t>
-  </si>
-  <si>
-    <t>author_ts</t>
-  </si>
-  <si>
-    <t>20150117160900</t>
-  </si>
-  <si>
-    <t>format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>1..n</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/time/@value</t>
-  </si>
-  <si>
-    <t>Datum der DokumentErstellung</t>
-  </si>
-  <si>
-    <t>datum_erstellung</t>
-  </si>
-  <si>
-    <t>20150117163300</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t>Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t>diagnostik_ts</t>
-  </si>
-  <si>
-    <t>201501171650</t>
-  </si>
-  <si>
-    <t>format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>Diagnostik !!!!!!!!</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t>Beschwerde Beginn der Symptome</t>
-  </si>
-  <si>
-    <t>beschwerde_begin</t>
-  </si>
-  <si>
-    <t>20150118</t>
-  </si>
-  <si>
-    <t>format=yyyymmdd;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Start Patientenkontakt Ankunfszeit</t>
-  </si>
-  <si>
-    <t>aufnahme_ts</t>
-  </si>
-  <si>
-    <t>20150118070100</t>
-  </si>
-  <si>
-    <t>startunkt</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Therapiebeginn, Aufnahme, Behandlung</t>
-  </si>
-  <si>
-    <t>therapiebeginn_ts</t>
-  </si>
-  <si>
-    <t>20150118071200</t>
-  </si>
-  <si>
-    <t>Begin des Arztkontaktes</t>
-  </si>
-  <si>
-    <t>arztkontakt_ts</t>
-  </si>
-  <si>
-    <t>20150118073500</t>
-  </si>
-  <si>
-    <t>format=yyyymmddhhmmss</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
-  </si>
-  <si>
-    <t>Ende des Arztkontaktes</t>
-  </si>
-  <si>
-    <t>end_arztkontakt_ts</t>
-  </si>
-  <si>
-    <t>20150118075100</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
-  </si>
-  <si>
-    <t>Verlegungs-/Entlassungszeitpunkt</t>
-  </si>
-  <si>
-    <t>entlassung_ts</t>
-  </si>
-  <si>
-    <t>20150118083000</t>
-  </si>
-  <si>
-    <t>O..1 =&gt; Problem mit Dependency Triage</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
+    <t xml:space="preserve">Vitalparameter Entry GCS Augenöffnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_augen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung durch Author zeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150117160900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1..n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/time/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum der DokumentErstellung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datum_erstellung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150117163300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201501171650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik !!!!!!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde Beginn der Symptome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beschwerde_begin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Patientenkontakt Ankunfszeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aufnahme_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118070100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapiebeginn, Aufnahme, Behandlung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">therapiebeginn_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118071200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begin des Arztkontaktes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arztkontakt_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118073500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmddhhmmss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende des Arztkontaktes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_arztkontakt_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118075100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verlegungs-/Entlassungszeitpunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entlassung_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118083000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O..1 =&gt; Problem mit Dependency Triage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
 ClinicalDocument/componentOf/encompassingEncounter/effectiveTime/high/@value</t>
   </si>
   <si>
-    <t>Ersteinschätzung zeit start</t>
-  </si>
-  <si>
-    <t>triage_ts_start</t>
-  </si>
-  <si>
-    <t>202006201603</t>
-  </si>
-  <si>
-    <t>format=yyyymmddhhmm</t>
-  </si>
-  <si>
-    <t>nach entlassung</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Ersteinschätzung zeit ende</t>
-  </si>
-  <si>
-    <t>triage_ts_end</t>
-  </si>
-  <si>
-    <t>202006201608</t>
-  </si>
-  <si>
-    <t>effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
+    <t xml:space="preserve">Ersteinschätzung zeit start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_ts_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202006201603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format=yyyymmddhhmm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nach entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschätzung zeit ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_ts_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202006201608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
 Beispiel: Für Gesundheitsdienstleister, die einen Patienten heute in der Klinik sehen anamenstisch einen Herzinfarkt erheben, der vor fünf Jahren stattgefunden hat, ist effectiveTime: vor fünf Jahren.
 Die effectiveTime hier ist die definitive Angabe, ob die zugrunde liegende Erkrankung behoben ist. effectiveTime.low ist der Beginn des Problems für den Patienten. Wenn das Problem noch nicht gelöst ist, wird effectiveTime.high nicht gesetzt. Wenn bekannt ist, dass das Problem gelöst werden kann, dann ist effectiveTime.high vorhanden. Wenn der genaue Zeitpunkt der Lösung des Problems nicht bekannt ist, dann ist effectiveTime.high vorhanden und auf nullFlavor "UNK" gesetzt.</t>
   </si>
   <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
-  </si>
-  <si>
-    <t>Beschwerde Code</t>
-  </si>
-  <si>
-    <t>cedis</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>link=cedis.csv;column=cedis</t>
-  </si>
-  <si>
-    <t>OTH,UNK</t>
-  </si>
-  <si>
-    <t>nullflavor</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Diagnostik Code Welche Untersuchung?</t>
-  </si>
-  <si>
-    <t>diagnostik_code</t>
-  </si>
-  <si>
-    <t>37637-6</t>
-  </si>
-  <si>
-    <t>link=diagnostik.csv;column=diagnostik_code</t>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH,UNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nullflavor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Code Welche Untersuchung?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37637-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=diagnostik.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
   </si>
   <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t>Basisinfo multiresistente</t>
-  </si>
-  <si>
-    <t>keime</t>
-  </si>
-  <si>
-    <t>3MRGN</t>
-  </si>
-  <si>
-    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
-    <t>OTH</t>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo multiresistente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3MRGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH</t>
   </si>
   <si>
     <t xml:space="preserve">	Multiresistenter Keim Ja/Nein/Verdacht; wenn angegeben soll, dass der in observation.value angegebene Keim NICHT vorliegt, wird observation.@negationInd="true" gesetzt. Bei "Verdacht" ist der Befundstatus in observation.value.qualifier entsprechend zu setzen.</t>
   </si>
   <si>
-    <t>EntlassungsGrund</t>
-  </si>
-  <si>
-    <t>entlassung</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>scope=1-6</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
-  </si>
-  <si>
-    <t>Ersteinschaetzung code</t>
-  </si>
-  <si>
-    <t>triage</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Beide Systeme haben 1-5</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Atemfrequenz</t>
-  </si>
-  <si>
-    <t>atemfrequenz</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry GCS motorische Antwort</t>
-  </si>
-  <si>
-    <t>gcs_motorisch</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Sauerstoffsättigung</t>
-  </si>
-  <si>
-    <t>saettigung</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>scope=0-100</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry  Schmerzskala</t>
-  </si>
-  <si>
-    <t>schmerzskala</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>scope=0-10</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Glasgoe Coma Scale Summe</t>
-  </si>
-  <si>
-    <t>gcs_summe</t>
-  </si>
-  <si>
-    <t>scope=3-15</t>
+    <t xml:space="preserve">EntlassungsGrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschaetzung code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Atemfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atemfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry GCS motorische Antwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_motorisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Sauerstoffsättigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saettigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry  Schmerzskala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schmerzskala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Glasgoe Coma Scale Summe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_summe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=3-15</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
   </si>
   <si>
-    <t>Aufnahme ID</t>
-  </si>
-  <si>
-    <t>encounter_id</t>
-  </si>
-  <si>
-    <t>987654321-04</t>
-  </si>
-  <si>
-    <t>regex=\d{9}-\d\d</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
+    <t xml:space="preserve">Aufnahme ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654321-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regex=\d{9}-\d\d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
   </si>
   <si>
     <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
   </si>
   <si>
-    <t>beschwerde_liste</t>
-  </si>
-  <si>
-    <t>AZ-Verschlechterung</t>
-  </si>
-  <si>
-    <t>Verweise auf Beschwerde</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenreaktion (links)</t>
-  </si>
-  <si>
-    <t>pupillenreaktion_links</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>value_set=[B, D, A]</t>
-  </si>
-  <si>
-    <t>Notfallanamnese</t>
-  </si>
-  <si>
-    <t>notfallanamnese</t>
+    <t xml:space="preserve">beschwerde_liste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verweise auf Beschwerde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text/content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (links)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenreaktion_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[B, D, A]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notfallanamnese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notfallanamnese</t>
   </si>
   <si>
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t>ChatGPT Text gnerierung aus allen Parametern</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenweite (links)</t>
-  </si>
-  <si>
-    <t>pupillenweite_links</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>value_set=[D, M, C]</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenweite (rechts)</t>
-  </si>
-  <si>
-    <t>pupillenweite_rechts</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenreaktion (rechts)</t>
-  </si>
-  <si>
-    <t>pupillenreaktion_rechts</t>
-  </si>
-  <si>
-    <t>Street Address Line</t>
-  </si>
-  <si>
-    <t>street_address_line</t>
-  </si>
-  <si>
-    <t>Dachauer Straße 112</t>
-  </si>
-  <si>
-    <t>link=streets.csv;column=street_address_line</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
-  </si>
-  <si>
-    <t>Abschlussdiagnose Freitext</t>
-  </si>
-  <si>
-    <t>diagnose_txt</t>
-  </si>
-  <si>
-    <t>Distorsion unteres Sprunggelenk (S96.3)</t>
-  </si>
-  <si>
-    <t>chatGPT text aus Beschwerde code generieren</t>
-  </si>
-  <si>
-    <t>Author prefix</t>
-  </si>
-  <si>
-    <t>prefix_author</t>
-  </si>
-  <si>
-    <t>Dr. med.</t>
-  </si>
-  <si>
-    <t>value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
-  </si>
-  <si>
-    <t>Beschwerde originaltext</t>
-  </si>
-  <si>
-    <t>beschwerden_txt</t>
-  </si>
-  <si>
-    <t>Durchfall und Erbrechen</t>
-  </si>
-  <si>
-    <t>ist 0..1 in doku soll aber immer da sein</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
-  </si>
-  <si>
-    <t>Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t>diagnostik_display_name</t>
-  </si>
-  <si>
-    <t>Extremity X-ray</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Blockweise Diagnostik REMOVE</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t>Basisinfo_tetanusschutz</t>
-  </si>
-  <si>
-    <t>tetanusschutz</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>value_set=[true,false]</t>
-  </si>
-  <si>
-    <t>NI</t>
+    <t xml:space="preserve">ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (links)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenweite_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[D, M, C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (rechts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenweite_rechts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (rechts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenreaktion_rechts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street Address Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street_address_line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=streets.csv;column=street_address_line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abschlussdiagnose Freitext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. med.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde originaltext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beschwerden_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durchfall und Erbrechen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist 0..1 in doku soll aber immer da sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_display_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extremity X-ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo_tetanusschutz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tetanusschutz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[true,false]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NI</t>
   </si>
   <si>
     <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
   </si>
   <si>
-    <t>Antibiotikaallergie</t>
-  </si>
-  <si>
-    <t>allergie_antibiotika</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
-  </si>
-  <si>
-    <t>Patient family name</t>
-  </si>
-  <si>
-    <t>family_patient</t>
-  </si>
-  <si>
-    <t>Kicker</t>
-  </si>
-  <si>
-    <t>link=family_names.csv;column=family_name</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
-  </si>
-  <si>
-    <t>Zuweisung Code</t>
-  </si>
-  <si>
-    <t>zuweisung</t>
-  </si>
-  <si>
-    <t>KVNDAK</t>
-  </si>
-  <si>
-    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>value_set=[M,F,UN]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
-  </si>
-  <si>
-    <t>Author given name</t>
-  </si>
-  <si>
-    <t>given_author</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>link=first_names.csv;column=first_name</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>München</t>
-  </si>
-  <si>
-    <t>link=cities.csv;column=city</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
-  </si>
-  <si>
-    <t>Diagnostik Ergebnis</t>
-  </si>
-  <si>
-    <t>diagnostik_ergebnis_code</t>
-  </si>
-  <si>
-    <t>OPB</t>
-  </si>
-  <si>
-    <t>value_set=[PB, OPB]</t>
-  </si>
-  <si>
-    <t>Blockweise Generieren</t>
-  </si>
-  <si>
-    <t>Author family name</t>
-  </si>
-  <si>
-    <t>family_author</t>
-  </si>
-  <si>
-    <t>Regensburger</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
-  </si>
-  <si>
-    <t>Diagnostik ganzer Text</t>
-  </si>
-  <si>
-    <t>diagnostik_text</t>
-  </si>
-  <si>
-    <t>Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE</t>
-  </si>
-  <si>
-    <t>diagnose_code</t>
-  </si>
-  <si>
-    <t>S93.6</t>
-  </si>
-  <si>
-    <t>NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
-  </si>
-  <si>
-    <t>Versicherungs Name</t>
-  </si>
-  <si>
-    <t>versicherung_txt</t>
-  </si>
-  <si>
-    <t>Selbstzahler</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/associatedOrganisation/name</t>
-  </si>
-  <si>
-    <t>Versicherungsfall</t>
-  </si>
-  <si>
-    <t>insurance_case</t>
-  </si>
-  <si>
-    <t>SELF</t>
-  </si>
-  <si>
-    <t>value_set=[FAMDEP,SELF]</t>
-  </si>
-  <si>
-    <t>If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
-  </si>
-  <si>
-    <t>Organisation name</t>
-  </si>
-  <si>
-    <t>organisation_name</t>
-  </si>
-  <si>
-    <t>Städtisches Klinikum München GmbH</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/representedOrganisation/name
+    <t xml:space="preserve">Antibiotikaallergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_antibiotika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient family name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=family_names.csv;column=family_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zuweisung Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zuweisung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KVNDAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[M,F,UN]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author given name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=first_names.csv;column=first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">München</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=clinics.csv;column=city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Ergebnis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ergebnis_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[PB, OPB]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Generieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author family name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regensburger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik ganzer Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S93.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungs Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherung_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selbstzahler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungsfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insurance_case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/associatedEntity/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organisation_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/name</t>
   </si>
   <si>
-    <t>Patient given name</t>
-  </si>
-  <si>
-    <t>given_patient</t>
-  </si>
-  <si>
-    <t>Timo</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
-  </si>
-  <si>
-    <t>Allergien vorhanden?</t>
-  </si>
-  <si>
-    <t>allergie</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>mindestens eine Allergy obsseration muss da sein</t>
-  </si>
-  <si>
-    <t>Kontrastmittelallergie</t>
-  </si>
-  <si>
-    <t>allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t>sonstige allergien vorhanden</t>
-  </si>
-  <si>
-    <t>allergie_sonstige</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE originalText</t>
-  </si>
-  <si>
-    <t>diagnose_name</t>
-  </si>
-  <si>
-    <t>Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
-  </si>
-  <si>
-    <t>Auf Diagnose abstimmen</t>
-  </si>
-  <si>
-    <t>_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t>scope=10-120</t>
-  </si>
-  <si>
-    <t>_therapiebeginn_arztkontakt</t>
-  </si>
-  <si>
-    <t>_arztkontakt_endarztkontakt</t>
-  </si>
-  <si>
-    <t>_endarztkontakt_entlassung</t>
-  </si>
-  <si>
-    <t>_entlassung_triagestart</t>
-  </si>
-  <si>
-    <t>_triagestart_triageend</t>
-  </si>
-  <si>
-    <t>_diagnostik_id</t>
-  </si>
-  <si>
-    <t>_associatedPerson_given</t>
-  </si>
-  <si>
-    <t>_associatedPerson_family</t>
-  </si>
-  <si>
-    <t>diagnostik_labor</t>
-  </si>
-  <si>
-    <t>diagnostik_blutgase</t>
-  </si>
-  <si>
-    <t>diagnostik_urinschnelltest</t>
-  </si>
-  <si>
-    <t>diagnostik_ekg</t>
-  </si>
-  <si>
-    <t>diagnostik_sonographie</t>
-  </si>
-  <si>
-    <t>diagnostik_echokardiographie</t>
-  </si>
-  <si>
-    <t>diagnostik_ct_kopf</t>
-  </si>
-  <si>
-    <t>diagnostik_ct</t>
-  </si>
-  <si>
-    <t>diagnostik_ct_trauma</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_wirbelsaeule</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_thorax</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_becken</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_extremitaeten</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_sonstiges</t>
-  </si>
-  <si>
-    <t>diagnostik_mrt</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE Qualifier</t>
-  </si>
-  <si>
-    <t>diagnose_qualifier</t>
-  </si>
-  <si>
-    <t>value_set=[V,G,A,Z];number=3</t>
-  </si>
-  <si>
-    <t>number=3</t>
-  </si>
-  <si>
-    <t>link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
+    <t xml:space="preserve">Patient given name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allergien vorhanden?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mindestens eine Allergy obsseration muss da sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontrastmittelallergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_kontrastmittel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonstige allergien vorhanden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_sonstige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auf Diagnose abstimmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=10-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_triagestart_triageend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_diagnostik_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_associatedPerson_given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_associatedPerson_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_blutgase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_urinschnelltest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ekg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_sonographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_echokardiographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct_kopf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct_trauma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_wirbelsaeule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_thorax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_becken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_extremitaeten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_sonstiges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_mrt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE Qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[V,G,A,Z];number=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1174,7 +1188,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1189,7 +1203,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -1213,7 +1227,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1221,34 +1235,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1307,76 +1380,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145F82"/>
+        <a:srgbClr val="145f82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E87331"/>
+        <a:srgbClr val="e87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186C24"/>
+        <a:srgbClr val="186c24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1408,7 +1465,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1432,7 +1489,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1492,41 +1549,42 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="38.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="3" customWidth="1"/>
-    <col min="7" max="8" width="20.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="112.75" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="77.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="112.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1564,14 +1622,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1599,14 +1657,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1633,14 +1691,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1667,14 +1725,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1701,14 +1759,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1737,14 +1795,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1773,7 +1831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1786,12 +1844,9 @@
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1806,7 +1861,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1819,12 +1874,9 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1839,7 +1891,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1875,7 +1927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1902,7 +1954,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1938,7 +1990,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>74</v>
       </c>
@@ -1974,7 +2026,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -1990,11 +2042,9 @@
       <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2006,7 +2056,7 @@
       </c>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2022,11 +2072,9 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2038,7 +2086,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -2051,12 +2099,9 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2113,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2084,11 +2129,9 @@
       <c r="E17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2100,7 +2143,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2135,7 +2178,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2151,11 +2194,9 @@
       <c r="E19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2170,7 +2211,7 @@
       </c>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -2204,7 +2245,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2237,7 +2278,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2253,11 +2294,9 @@
       <c r="E22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2269,7 +2308,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -2305,7 +2344,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
@@ -2338,7 +2377,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>132</v>
       </c>
@@ -2354,11 +2393,9 @@
       <c r="E25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2410,7 @@
       </c>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>137</v>
       </c>
@@ -2406,7 +2443,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>140</v>
       </c>
@@ -2422,11 +2459,9 @@
       <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2438,7 +2473,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -2454,11 +2489,9 @@
       <c r="E28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2470,7 +2503,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="30">
+    <row r="29" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -2486,11 +2519,9 @@
       <c r="E29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2536,7 @@
       </c>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -2521,11 +2552,9 @@
       <c r="E30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
         <v>19</v>
       </c>
@@ -2540,7 +2569,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" ht="360">
+    <row r="31" s="1" customFormat="true" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -2556,11 +2585,9 @@
       <c r="E31" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
         <v>18</v>
       </c>
@@ -2575,7 +2602,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>165</v>
       </c>
@@ -2611,7 +2638,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.5" customHeight="1">
+    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>172</v>
       </c>
@@ -2645,7 +2672,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>178</v>
       </c>
@@ -2681,7 +2708,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -2717,7 +2744,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>189</v>
       </c>
@@ -2733,11 +2760,9 @@
       <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2752,7 +2777,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -2788,7 +2813,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>196</v>
       </c>
@@ -2824,7 +2849,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>199</v>
       </c>
@@ -2860,7 +2885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
@@ -2896,7 +2921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>207</v>
       </c>
@@ -2932,7 +2957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
@@ -2965,7 +2990,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -2995,7 +3020,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>221</v>
       </c>
@@ -3033,7 +3058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -3060,7 +3085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>229</v>
       </c>
@@ -3098,7 +3123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
         <v>233</v>
       </c>
@@ -3136,7 +3161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>236</v>
       </c>
@@ -3174,7 +3199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>238</v>
       </c>
@@ -3207,7 +3232,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>243</v>
       </c>
@@ -3220,12 +3245,9 @@
       <c r="D50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>19</v>
       </c>
@@ -3240,7 +3262,7 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>247</v>
       </c>
@@ -3273,7 +3295,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>252</v>
       </c>
@@ -3286,14 +3308,12 @@
       <c r="D52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>19</v>
       </c>
@@ -3308,7 +3328,7 @@
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>257</v>
       </c>
@@ -3321,12 +3341,9 @@
       <c r="D53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>38</v>
       </c>
@@ -3341,7 +3358,7 @@
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>263</v>
       </c>
@@ -3377,7 +3394,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>269</v>
       </c>
@@ -3410,7 +3427,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>272</v>
       </c>
@@ -3426,11 +3443,9 @@
       <c r="E56" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>115</v>
       </c>
@@ -3442,7 +3457,7 @@
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>277</v>
       </c>
@@ -3473,7 +3488,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>282</v>
       </c>
@@ -3489,11 +3504,9 @@
       <c r="E58" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>19</v>
       </c>
@@ -3505,7 +3518,7 @@
       </c>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>287</v>
       </c>
@@ -3521,11 +3534,9 @@
       <c r="E59" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
@@ -3537,7 +3548,7 @@
       </c>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>292</v>
       </c>
@@ -3570,7 +3581,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>297</v>
       </c>
@@ -3586,11 +3597,9 @@
       <c r="E61" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
         <v>38</v>
       </c>
@@ -3605,7 +3614,7 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>302</v>
       </c>
@@ -3621,11 +3630,9 @@
       <c r="E62" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
@@ -3637,7 +3644,7 @@
       </c>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>306</v>
       </c>
@@ -3650,12 +3657,9 @@
       <c r="D63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
         <v>115</v>
       </c>
@@ -3667,7 +3671,7 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>309</v>
       </c>
@@ -3681,7 +3685,7 @@
         <v>14</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>373</v>
+        <v>312</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>169</v>
@@ -3696,34 +3700,31 @@
         <v>19</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
         <v>19</v>
       </c>
@@ -3731,60 +3732,56 @@
         <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>322</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>26</v>
       </c>
@@ -3798,19 +3795,19 @@
         <v>45</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M67" s="3"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>14</v>
@@ -3818,11 +3815,9 @@
       <c r="E68" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
@@ -3830,19 +3825,19 @@
         <v>45</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>14</v>
@@ -3861,7 +3856,7 @@
         <v>19</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>20</v>
@@ -3870,15 +3865,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>14</v>
@@ -3903,15 +3898,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>14</v>
@@ -3936,21 +3931,21 @@
         <v>271</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>71</v>
@@ -3965,24 +3960,24 @@
         <v>19</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3990,15 +3985,15 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -4006,15 +4001,15 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -4022,15 +4017,15 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -4038,15 +4033,15 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -4054,15 +4049,15 @@
       </c>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -4070,17 +4065,17 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
@@ -4094,9 +4089,9 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="2:8">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>14</v>
@@ -4106,9 +4101,9 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="2:8">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="6" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>299</v>
@@ -4123,9 +4118,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="2:8">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="6" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>299</v>
@@ -4140,9 +4135,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="2:8">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="6" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>299</v>
@@ -4157,9 +4152,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="2:8">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="6" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>299</v>
@@ -4174,9 +4169,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="2:8">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>299</v>
@@ -4191,9 +4186,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="2:8">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="6" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>299</v>
@@ -4208,9 +4203,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="2:8">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="6" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>299</v>
@@ -4225,9 +4220,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="2:8">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="6" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>299</v>
@@ -4242,9 +4237,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="2:8">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="6" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>299</v>
@@ -4259,9 +4254,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="2:8">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="6" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>299</v>
@@ -4276,9 +4271,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="2:8">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>299</v>
@@ -4293,9 +4288,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="2:8">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="6" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>299</v>
@@ -4310,9 +4305,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="2:8">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>299</v>
@@ -4327,9 +4322,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="2:8">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>299</v>
@@ -4344,9 +4339,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="2:8">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>299</v>
@@ -4361,21 +4356,21 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>71</v>
@@ -4390,20 +4385,25 @@
         <v>19</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L32" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
   </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change name to diagnostics.csv
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -551,7 +551,7 @@
     <t xml:space="preserve">37637-6</t>
   </si>
   <si>
-    <t xml:space="preserve">link=diagnostik.csv;column=diagnostik_code</t>
+    <t xml:space="preserve">link=diagnostics.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
@@ -1564,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Merge various .csv files in one misc.csv (miscellaneous)
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -749,7 +749,7 @@
     <t xml:space="preserve">Dachauer Straße 112</t>
   </si>
   <si>
-    <t xml:space="preserve">link=streets.csv;column=street_address_line</t>
+    <t xml:space="preserve">link=misc.csv;column=street_address_line</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
@@ -851,7 +851,7 @@
     <t xml:space="preserve">Kicker</t>
   </si>
   <si>
-    <t xml:space="preserve">link=family_names.csv;column=family_name</t>
+    <t xml:space="preserve">link=misc.csv;column=family_name</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
@@ -896,7 +896,7 @@
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
-    <t xml:space="preserve">link=first_names.csv;column=first_name</t>
+    <t xml:space="preserve">link=misc.csv;column=first_name</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
@@ -1564,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E90" activeCellId="0" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Change format parameter -> date_format and removed **kwargs in DateGenerator
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -311,7 +311,7 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+    <t xml:space="preserve">date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
@@ -365,7 +365,7 @@
     <t xml:space="preserve">20150117160900</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+    <t xml:space="preserve">date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
   </si>
   <si>
     <t xml:space="preserve">1..n</t>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">201501171650</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+    <t xml:space="preserve">date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnostik !!!!!!!!</t>
@@ -413,7 +413,7 @@
     <t xml:space="preserve">20150118</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+    <t xml:space="preserve">date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
@@ -452,7 +452,7 @@
     <t xml:space="preserve">20150118073500</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmddhhmmss</t>
+    <t xml:space="preserve">date_format=yyyymmddhhmmss</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">202006201603</t>
   </si>
   <si>
-    <t xml:space="preserve">format=yyyymmddhhmm</t>
+    <t xml:space="preserve">date_format=yyyymmddhhmm</t>
   </si>
   <si>
     <t xml:space="preserve">nach entlassung</t>
@@ -1564,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E90" activeCellId="0" sqref="E90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
misc.csv in individual_attributes.csv and requirements.txt fixed
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D230D88-353E-4246-8736-343AEC4CE401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,1163 +27,1144 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="374">
   <si>
-    <t xml:space="preserve">Variable name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generation type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Block Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardinality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DWH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportmittel Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transportmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[1,2,3,4,OTH]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH,NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blutdruck_sys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herzfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postleitzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=01067-99998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsidentifikation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_iknr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=100000000-999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise mit Versicherungsnamen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1000000000-9999999999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kinda sus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/id/@extension
+    <t>Variable name</t>
+  </si>
+  <si>
+    <t>Concept Id</t>
+  </si>
+  <si>
+    <t>Default values</t>
+  </si>
+  <si>
+    <t>Generation type</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Nullflavor</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Block Cardinality</t>
+  </si>
+  <si>
+    <t>Cardinality</t>
+  </si>
+  <si>
+    <t>Commentar</t>
+  </si>
+  <si>
+    <t>DWH</t>
+  </si>
+  <si>
+    <t>Pfad</t>
+  </si>
+  <si>
+    <t>Transportmittel Code</t>
+  </si>
+  <si>
+    <t>transportmittel</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>value_set=[1,2,3,4,OTH]</t>
+  </si>
+  <si>
+    <t>OTH,NA</t>
+  </si>
+  <si>
+    <t>generating</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t>blutdruck_sys</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>scope=0-300</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry herzfrequenz</t>
+  </si>
+  <si>
+    <t>herzfrequenz</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>postleitzahl</t>
+  </si>
+  <si>
+    <t>scope=01067-99998</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
+  </si>
+  <si>
+    <t>Versicherungsidentifikation</t>
+  </si>
+  <si>
+    <t>versicherung_iknr</t>
+  </si>
+  <si>
+    <t>scope=100000000-999999999</t>
+  </si>
+  <si>
+    <t>0..n</t>
+  </si>
+  <si>
+    <t>Blockweise mit Versicherungsnamen</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
+  </si>
+  <si>
+    <t>Organisation ID</t>
+  </si>
+  <si>
+    <t>organisation_id</t>
+  </si>
+  <si>
+    <t>scope=1000000000-9999999999</t>
+  </si>
+  <si>
+    <t>kinda sus</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/id/@extension
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/id/@extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Allergien spezifisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergien_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|Allergien|Antibiotika : |</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonstige Allergien sollten hier genannt werden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ersteinschaetzung_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">|triageval|5|triageval|</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste Verweise auf triageEVAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Körpertemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kerntemperatur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0.0-45.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UUID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/setId/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo Schwangerschaftsstatus code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schwangerschaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kein Fehler bei Gender Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS verbale Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_verbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was Bei Summe, wenn einer fehlt?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung Codesystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.276.0.76.5.438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234567890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dokument_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/id/@extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geburtsdatum patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geburtsdatum_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19960531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerdedauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">symptomdauer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_ranking_skala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rankin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valueset(1-6)?</t>
+    <t>Allergien spezifisch</t>
+  </si>
+  <si>
+    <t>allergien_txt</t>
+  </si>
+  <si>
+    <t>|Allergien|Antibiotika : |</t>
+  </si>
+  <si>
+    <t>Sonstige Allergien sollten hier genannt werden</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung text</t>
+  </si>
+  <si>
+    <t>ersteinschaetzung_text</t>
+  </si>
+  <si>
+    <t>|triageval|5|triageval|</t>
+  </si>
+  <si>
+    <t>Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Körpertemperatur</t>
+  </si>
+  <si>
+    <t>kerntemperatur</t>
+  </si>
+  <si>
+    <t>0.335</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>scope=0.0-45.0</t>
+  </si>
+  <si>
+    <t>Version ID</t>
+  </si>
+  <si>
+    <t>version_id</t>
+  </si>
+  <si>
+    <t>0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/setId/@extension</t>
+  </si>
+  <si>
+    <t>Basisinfo Schwangerschaftsstatus code</t>
+  </si>
+  <si>
+    <t>schwangerschaft</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>scope=0-1</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS verbale Antwort</t>
+  </si>
+  <si>
+    <t>gcs_verbal</t>
+  </si>
+  <si>
+    <t>scope=1-5</t>
+  </si>
+  <si>
+    <t>Was Bei Summe, wenn einer fehlt?</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung Codesystem</t>
+  </si>
+  <si>
+    <t>triage_system</t>
+  </si>
+  <si>
+    <t>1.2.276.0.76.5.438</t>
+  </si>
+  <si>
+    <t>value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/id/@extension</t>
+  </si>
+  <si>
+    <t>Document ID</t>
+  </si>
+  <si>
+    <t>dokument_id</t>
+  </si>
+  <si>
+    <t>14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/id/@extension</t>
+  </si>
+  <si>
+    <t>Geburtsdatum patient</t>
+  </si>
+  <si>
+    <t>geburtsdatum_ts</t>
+  </si>
+  <si>
+    <t>19960531</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerdedauer</t>
+  </si>
+  <si>
+    <t>symptomdauer</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>scope=0-99</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
+  </si>
+  <si>
+    <t>Basisinfo_ranking_skala</t>
+  </si>
+  <si>
+    <t>rankin</t>
+  </si>
+  <si>
+    <t>scope=0-6</t>
+  </si>
+  <si>
+    <t>Valueset(1-6)?</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text </t>
   </si>
   <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS Augenöffnen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_augen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erstellung durch Author zeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">author_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117160900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1..n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/time/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum der DokumentErstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datum_erstellung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150117163300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201501171650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik !!!!!!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Beginn der Symptome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerde_begin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Patientenkontakt Ankunfszeit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aufnahme_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118070100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Therapiebeginn, Aufnahme, Behandlung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">therapiebeginn_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118071200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Begin des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118073500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmmss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ende des Arztkontaktes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_arztkontakt_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118075100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verlegungs-/Entlassungszeitpunkt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung_ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20150118083000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O..1 =&gt; Problem mit Dependency Triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
+    <t>Vitalparameter Entry GCS Augenöffnen</t>
+  </si>
+  <si>
+    <t>gcs_augen</t>
+  </si>
+  <si>
+    <t>scope=1-4</t>
+  </si>
+  <si>
+    <t>Erstellung durch Author zeit</t>
+  </si>
+  <si>
+    <t>author_ts</t>
+  </si>
+  <si>
+    <t>20150117160900</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>1..n</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/time/@value</t>
+  </si>
+  <si>
+    <t>Datum der DokumentErstellung</t>
+  </si>
+  <si>
+    <t>datum_erstellung</t>
+  </si>
+  <si>
+    <t>20150117163300</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t>diagnostik_ts</t>
+  </si>
+  <si>
+    <t>201501171650</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>Diagnostik !!!!!!!!</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Beginn der Symptome</t>
+  </si>
+  <si>
+    <t>beschwerde_begin</t>
+  </si>
+  <si>
+    <t>20150118</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Start Patientenkontakt Ankunfszeit</t>
+  </si>
+  <si>
+    <t>aufnahme_ts</t>
+  </si>
+  <si>
+    <t>20150118070100</t>
+  </si>
+  <si>
+    <t>startunkt</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Therapiebeginn, Aufnahme, Behandlung</t>
+  </si>
+  <si>
+    <t>therapiebeginn_ts</t>
+  </si>
+  <si>
+    <t>20150118071200</t>
+  </si>
+  <si>
+    <t>Begin des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118073500</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmddhhmmss</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
+  </si>
+  <si>
+    <t>Ende des Arztkontaktes</t>
+  </si>
+  <si>
+    <t>end_arztkontakt_ts</t>
+  </si>
+  <si>
+    <t>20150118075100</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
+  </si>
+  <si>
+    <t>Verlegungs-/Entlassungszeitpunkt</t>
+  </si>
+  <si>
+    <t>entlassung_ts</t>
+  </si>
+  <si>
+    <t>20150118083000</t>
+  </si>
+  <si>
+    <t>O..1 =&gt; Problem mit Dependency Triage</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
 ClinicalDocument/componentOf/encompassingEncounter/effectiveTime/high/@value</t>
   </si>
   <si>
-    <t xml:space="preserve">Ersteinschätzung zeit start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nach entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschätzung zeit ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage_ts_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">202006201608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
+    <t>Ersteinschätzung zeit start</t>
+  </si>
+  <si>
+    <t>triage_ts_start</t>
+  </si>
+  <si>
+    <t>202006201603</t>
+  </si>
+  <si>
+    <t>date_format=yyyymmddhhmm</t>
+  </si>
+  <si>
+    <t>nach entlassung</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t>Ersteinschätzung zeit ende</t>
+  </si>
+  <si>
+    <t>triage_ts_end</t>
+  </si>
+  <si>
+    <t>202006201608</t>
+  </si>
+  <si>
+    <t>effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
 Beispiel: Für Gesundheitsdienstleister, die einen Patienten heute in der Klinik sehen anamenstisch einen Herzinfarkt erheben, der vor fünf Jahren stattgefunden hat, ist effectiveTime: vor fünf Jahren.
 Die effectiveTime hier ist die definitive Angabe, ob die zugrunde liegende Erkrankung behoben ist. effectiveTime.low ist der Beginn des Problems für den Patienten. Wenn das Problem noch nicht gelöst ist, wird effectiveTime.high nicht gesetzt. Wenn bekannt ist, dass das Problem gelöst werden kann, dann ist effectiveTime.high vorhanden. Wenn der genaue Zeitpunkt der Lösung des Problems nicht bekannt ist, dann ist effectiveTime.high vorhanden und auf nullFlavor "UNK" gesetzt.</t>
   </si>
   <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH,UNK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nullflavor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Code Welche Untersuchung?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37637-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=diagnostics.csv;column=diagnostik_code</t>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
+  </si>
+  <si>
+    <t>Beschwerde Code</t>
+  </si>
+  <si>
+    <t>cedis</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>link=cedis.csv;column=cedis</t>
+  </si>
+  <si>
+    <t>OTH,UNK</t>
+  </si>
+  <si>
+    <t>nullflavor</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
+  </si>
+  <si>
+    <t>Diagnostik Code Welche Untersuchung?</t>
+  </si>
+  <si>
+    <t>diagnostik_code</t>
+  </si>
+  <si>
+    <t>37637-6</t>
+  </si>
+  <si>
+    <t>link=diagnostics.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
   </si>
   <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo multiresistente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3MRGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTH</t>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t>Basisinfo multiresistente</t>
+  </si>
+  <si>
+    <t>keime</t>
+  </si>
+  <si>
+    <t>3MRGN</t>
+  </si>
+  <si>
+    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t>OTH</t>
   </si>
   <si>
     <t xml:space="preserve">	Multiresistenter Keim Ja/Nein/Verdacht; wenn angegeben soll, dass der in observation.value angegebene Keim NICHT vorliegt, wird observation.@negationInd="true" gesetzt. Bei "Verdacht" ist der Befundstatus in observation.value.qualifier entsprechend zu setzen.</t>
   </si>
   <si>
-    <t xml:space="preserve">EntlassungsGrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=1-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ersteinschaetzung code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beide Systeme haben 1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atemfrequenz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry GCS motorische Antwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_motorisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Sauerstoffsättigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saettigung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry  Schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schmerzskala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=0-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Glasgoe Coma Scale Summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gcs_summe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=3-15</t>
+    <t>EntlassungsGrund</t>
+  </si>
+  <si>
+    <t>entlassung</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>scope=1-6</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
+  </si>
+  <si>
+    <t>Ersteinschaetzung code</t>
+  </si>
+  <si>
+    <t>triage</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Atemfrequenz</t>
+  </si>
+  <si>
+    <t>atemfrequenz</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry GCS motorische Antwort</t>
+  </si>
+  <si>
+    <t>gcs_motorisch</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Sauerstoffsättigung</t>
+  </si>
+  <si>
+    <t>saettigung</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>scope=0-100</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry  Schmerzskala</t>
+  </si>
+  <si>
+    <t>schmerzskala</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>scope=0-10</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Glasgoe Coma Scale Summe</t>
+  </si>
+  <si>
+    <t>gcs_summe</t>
+  </si>
+  <si>
+    <t>scope=3-15</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
   </si>
   <si>
-    <t xml:space="preserve">Aufnahme ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">987654321-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regex=\d{9}-\d\d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
+    <t>Aufnahme ID</t>
+  </si>
+  <si>
+    <t>encounter_id</t>
+  </si>
+  <si>
+    <t>987654321-04</t>
+  </si>
+  <si>
+    <t>regex=\d{9}-\d\d</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
   </si>
   <si>
     <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
   </si>
   <si>
-    <t xml:space="preserve">beschwerde_liste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ-Verschlechterung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verweise auf Beschwerde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text/content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[B, D, A]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notfallanamnese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notfallanamnese</t>
+    <t>beschwerde_liste</t>
+  </si>
+  <si>
+    <t>AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t>Verweise auf Beschwerde</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (links)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_links</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>value_set=[B, D, A]</t>
+  </si>
+  <si>
+    <t>Notfallanamnese</t>
+  </si>
+  <si>
+    <t>notfallanamnese</t>
   </si>
   <si>
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t xml:space="preserve">ChatGPT Text gnerierung aus allen Parametern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (links)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_links</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[D, M, C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenweite (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenweite_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitalparameter Entry Pupillenreaktion (rechts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pupillenreaktion_rechts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street Address Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dachauer Straße 112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=misc.csv;column=street_address_line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abschlussdiagnose Freitext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chatGPT text aus Beschwerde code generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. med.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschwerde originaltext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beschwerden_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durchfall und Erbrechen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ist 0..1 in doku soll aber immer da sein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_display_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extremity X-ray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basisinfo_tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tetanusschutz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[true,false]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NI</t>
+    <t>ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (links)</t>
+  </si>
+  <si>
+    <t>pupillenweite_links</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>value_set=[D, M, C]</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenweite (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenweite_rechts</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Vitalparameter Entry Pupillenreaktion (rechts)</t>
+  </si>
+  <si>
+    <t>pupillenreaktion_rechts</t>
+  </si>
+  <si>
+    <t>Street Address Line</t>
+  </si>
+  <si>
+    <t>street_address_line</t>
+  </si>
+  <si>
+    <t>Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
+  </si>
+  <si>
+    <t>Abschlussdiagnose Freitext</t>
+  </si>
+  <si>
+    <t>diagnose_txt</t>
+  </si>
+  <si>
+    <t>Distorsion unteres Sprunggelenk (S96.3)</t>
+  </si>
+  <si>
+    <t>chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t>Author prefix</t>
+  </si>
+  <si>
+    <t>prefix_author</t>
+  </si>
+  <si>
+    <t>Dr. med.</t>
+  </si>
+  <si>
+    <t>value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
+  </si>
+  <si>
+    <t>Beschwerde originaltext</t>
+  </si>
+  <si>
+    <t>beschwerden_txt</t>
+  </si>
+  <si>
+    <t>Durchfall und Erbrechen</t>
+  </si>
+  <si>
+    <t>ist 0..1 in doku soll aber immer da sein</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
+  </si>
+  <si>
+    <t>Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t>diagnostik_display_name</t>
+  </si>
+  <si>
+    <t>Extremity X-ray</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Blockweise Diagnostik REMOVE</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t>Basisinfo_tetanusschutz</t>
+  </si>
+  <si>
+    <t>tetanusschutz</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>value_set=[true,false]</t>
+  </si>
+  <si>
+    <t>NI</t>
   </si>
   <si>
     <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
   </si>
   <si>
-    <t xml:space="preserve">Antibiotikaallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_antibiotika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kicker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=misc.csv;column=family_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zuweisung Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zuweisung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KVNDAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[M,F,UN]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=misc.csv;column=first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">München</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=clinics.csv;column=city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik Ergebnis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ergebnis_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[PB, OPB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blockweise Generieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family_author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regensburger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik ganzer Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S93.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungs Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">versicherung_txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selbstzahler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versicherungsfall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insurance_case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/participant/associatedEntity/code/@code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organisation_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
+    <t>Antibiotikaallergie</t>
+  </si>
+  <si>
+    <t>allergie_antibiotika</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
+  </si>
+  <si>
+    <t>Patient family name</t>
+  </si>
+  <si>
+    <t>family_patient</t>
+  </si>
+  <si>
+    <t>Kicker</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
+  </si>
+  <si>
+    <t>Zuweisung Code</t>
+  </si>
+  <si>
+    <t>zuweisung</t>
+  </si>
+  <si>
+    <t>KVNDAK</t>
+  </si>
+  <si>
+    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>value_set=[M,F,UN]</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
+  </si>
+  <si>
+    <t>Author given name</t>
+  </si>
+  <si>
+    <t>given_author</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>München</t>
+  </si>
+  <si>
+    <t>link=clinics.csv;column=city</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
+  </si>
+  <si>
+    <t>Diagnostik Ergebnis</t>
+  </si>
+  <si>
+    <t>diagnostik_ergebnis_code</t>
+  </si>
+  <si>
+    <t>OPB</t>
+  </si>
+  <si>
+    <t>value_set=[PB, OPB]</t>
+  </si>
+  <si>
+    <t>Blockweise Generieren</t>
+  </si>
+  <si>
+    <t>Author family name</t>
+  </si>
+  <si>
+    <t>family_author</t>
+  </si>
+  <si>
+    <t>Regensburger</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
+  </si>
+  <si>
+    <t>Diagnostik ganzer Text</t>
+  </si>
+  <si>
+    <t>diagnostik_text</t>
+  </si>
+  <si>
+    <t>Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE</t>
+  </si>
+  <si>
+    <t>diagnose_code</t>
+  </si>
+  <si>
+    <t>S93.6</t>
+  </si>
+  <si>
+    <t>link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
+  </si>
+  <si>
+    <t>NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
+  </si>
+  <si>
+    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
+  </si>
+  <si>
+    <t>Versicherungs Name</t>
+  </si>
+  <si>
+    <t>versicherung_txt</t>
+  </si>
+  <si>
+    <t>Selbstzahler</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedOrganisation/name</t>
+  </si>
+  <si>
+    <t>Versicherungsfall</t>
+  </si>
+  <si>
+    <t>insurance_case</t>
+  </si>
+  <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>value_set=[FAMDEP,SELF]</t>
+  </si>
+  <si>
+    <t>If FAMDEP then AssociatedPerson</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
+  </si>
+  <si>
+    <t>Organisation name</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
+    <t>Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/author/representedOrganisation/name
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/name</t>
   </si>
   <si>
-    <t xml:space="preserve">Patient given name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">given_patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergien vorhanden?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mindestens eine Allergy obsseration muss da sein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kontrastmittelallergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonstige allergien vorhanden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allergie_sonstige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auf Diagnose abstimmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scope=10-120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_arztkontakt_endarztkontakt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_endarztkontakt_entlassung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_entlassung_triagestart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_triagestart_triageend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_diagnostik_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_associatedPerson_given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_associatedPerson_family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_blutgase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_urinschnelltest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ekg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_sonographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_echokardiographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct_kopf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_ct_trauma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_wirbelsaeule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_thorax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_becken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_extremitaeten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_roentgen_sonstiges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnostik_mrt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose ICD10 CODE Qualifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnose_qualifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value_set=[V,G,A,Z];number=3</t>
+    <t>Patient given name</t>
+  </si>
+  <si>
+    <t>given_patient</t>
+  </si>
+  <si>
+    <t>Timo</t>
+  </si>
+  <si>
+    <t>ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
+  </si>
+  <si>
+    <t>Allergien vorhanden?</t>
+  </si>
+  <si>
+    <t>allergie</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>mindestens eine Allergy obsseration muss da sein</t>
+  </si>
+  <si>
+    <t>Kontrastmittelallergie</t>
+  </si>
+  <si>
+    <t>allergie_kontrastmittel</t>
+  </si>
+  <si>
+    <t>sonstige allergien vorhanden</t>
+  </si>
+  <si>
+    <t>allergie_sonstige</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE originalText</t>
+  </si>
+  <si>
+    <t>diagnose_name</t>
+  </si>
+  <si>
+    <t>Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
+  </si>
+  <si>
+    <t>number=3</t>
+  </si>
+  <si>
+    <t>Auf Diagnose abstimmen</t>
+  </si>
+  <si>
+    <t>_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t>scope=10-120</t>
+  </si>
+  <si>
+    <t>_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t>_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t>_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t>_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t>_triagestart_triageend</t>
+  </si>
+  <si>
+    <t>_diagnostik_id</t>
+  </si>
+  <si>
+    <t>_associatedPerson_given</t>
+  </si>
+  <si>
+    <t>_associatedPerson_family</t>
+  </si>
+  <si>
+    <t>diagnostik_labor</t>
+  </si>
+  <si>
+    <t>diagnostik_blutgase</t>
+  </si>
+  <si>
+    <t>diagnostik_urinschnelltest</t>
+  </si>
+  <si>
+    <t>diagnostik_ekg</t>
+  </si>
+  <si>
+    <t>diagnostik_sonographie</t>
+  </si>
+  <si>
+    <t>diagnostik_echokardiographie</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_kopf</t>
+  </si>
+  <si>
+    <t>diagnostik_ct</t>
+  </si>
+  <si>
+    <t>diagnostik_ct_trauma</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_wirbelsaeule</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_thorax</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_becken</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_extremitaeten</t>
+  </si>
+  <si>
+    <t>diagnostik_roentgen_sonstiges</t>
+  </si>
+  <si>
+    <t>diagnostik_mrt</t>
+  </si>
+  <si>
+    <t>Diagnose ICD10 CODE Qualifier</t>
+  </si>
+  <si>
+    <t>diagnose_qualifier</t>
+  </si>
+  <si>
+    <t>value_set=[V,G,A,Z];number=3</t>
+  </si>
+  <si>
+    <t>link=individual_attributes.csv;column=street_address_line</t>
+  </si>
+  <si>
+    <t>link=individual_attributes.csv;column=family_name</t>
+  </si>
+  <si>
+    <t>link=individual_attributes.csv;column=first_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1188,7 +1174,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1203,7 +1189,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -1227,7 +1213,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1235,93 +1221,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1380,60 +1307,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145f82"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e87331"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186c24"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1465,7 +1408,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1489,7 +1432,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1549,42 +1492,41 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="77.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="112.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
+    <col min="1" max="1" width="38.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="3" customWidth="1"/>
+    <col min="7" max="8" width="20.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="112.75" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1622,14 +1564,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1657,14 +1599,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1691,14 +1633,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1725,14 +1667,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1759,14 +1701,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="2">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1795,14 +1737,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="2">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1831,7 +1773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1844,9 +1786,12 @@
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1861,7 +1806,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1874,9 +1819,12 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1891,7 +1839,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1927,7 +1875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1954,7 +1902,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1990,7 +1938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:13">
       <c r="A13" s="6" t="s">
         <v>74</v>
       </c>
@@ -2026,7 +1974,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -2042,9 +1990,11 @@
       <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2056,7 +2006,7 @@
       </c>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2072,9 +2022,11 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2086,7 +2038,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -2099,9 +2051,12 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2113,7 +2068,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2129,9 +2084,11 @@
       <c r="E17" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2143,7 +2100,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2178,7 +2135,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2194,9 +2151,11 @@
       <c r="E19" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2211,7 +2170,7 @@
       </c>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:13">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -2245,7 +2204,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2278,7 +2237,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2294,9 +2253,11 @@
       <c r="E22" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2308,7 +2269,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -2344,7 +2305,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
@@ -2377,7 +2338,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>132</v>
       </c>
@@ -2393,9 +2354,11 @@
       <c r="E25" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2410,7 +2373,7 @@
       </c>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>137</v>
       </c>
@@ -2443,7 +2406,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>140</v>
       </c>
@@ -2459,9 +2422,11 @@
       <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2473,7 +2438,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -2489,9 +2454,11 @@
       <c r="E28" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2503,7 +2470,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:13" ht="30">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -2519,9 +2486,11 @@
       <c r="E29" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2536,7 +2505,7 @@
       </c>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -2552,9 +2521,11 @@
       <c r="E30" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
         <v>19</v>
       </c>
@@ -2569,7 +2540,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" s="1" customFormat="true" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:13" ht="360">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -2585,9 +2556,11 @@
       <c r="E31" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
         <v>18</v>
       </c>
@@ -2602,7 +2575,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>165</v>
       </c>
@@ -2638,7 +2611,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:13" ht="16.5" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>172</v>
       </c>
@@ -2672,7 +2645,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>178</v>
       </c>
@@ -2708,7 +2681,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -2744,7 +2717,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>189</v>
       </c>
@@ -2760,9 +2733,11 @@
       <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2777,7 +2752,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -2813,7 +2788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:13">
       <c r="A38" s="6" t="s">
         <v>196</v>
       </c>
@@ -2849,7 +2824,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>199</v>
       </c>
@@ -2885,7 +2860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
@@ -2921,7 +2896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>207</v>
       </c>
@@ -2957,7 +2932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
@@ -2990,7 +2965,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -3020,7 +2995,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:13">
       <c r="A44" s="6" t="s">
         <v>221</v>
       </c>
@@ -3058,7 +3033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -3085,7 +3060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:13">
       <c r="A46" s="6" t="s">
         <v>229</v>
       </c>
@@ -3123,7 +3098,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:13">
       <c r="A47" s="6" t="s">
         <v>233</v>
       </c>
@@ -3161,7 +3136,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:13">
       <c r="A48" s="6" t="s">
         <v>236</v>
       </c>
@@ -3199,7 +3174,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>238</v>
       </c>
@@ -3213,7 +3188,7 @@
         <v>14</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>241</v>
+        <v>371</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -3229,30 +3204,33 @@
         <v>45</v>
       </c>
       <c r="L49" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>20</v>
@@ -3262,21 +3240,21 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3292,90 +3270,95 @@
         <v>45</v>
       </c>
       <c r="L51" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="D52" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L52" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="M52" s="3"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="M52" s="3"/>
-    </row>
-    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>260</v>
-      </c>
+      <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L53" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M53" s="3"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="M53" s="3"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>17</v>
@@ -3385,7 +3368,7 @@
         <v>18</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>20</v>
@@ -3394,21 +3377,21 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>270</v>
-      </c>
       <c r="C55" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
@@ -3424,28 +3407,30 @@
         <v>20</v>
       </c>
       <c r="L55" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="D56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>275</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>115</v>
       </c>
@@ -3453,25 +3438,25 @@
         <v>45</v>
       </c>
       <c r="L56" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M56" s="3"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="M56" s="3"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>278</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>280</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11" t="s">
@@ -3485,28 +3470,30 @@
         <v>20</v>
       </c>
       <c r="L57" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>285</v>
-      </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>19</v>
       </c>
@@ -3514,29 +3501,31 @@
         <v>20</v>
       </c>
       <c r="L58" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="M58" s="3"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="M58" s="3"/>
-    </row>
-    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="D59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>290</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
@@ -3544,25 +3533,25 @@
         <v>45</v>
       </c>
       <c r="L59" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="M59" s="3"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M59" s="3"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="D60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
@@ -3578,33 +3567,35 @@
         <v>45</v>
       </c>
       <c r="L60" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>300</v>
-      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>20</v>
@@ -3614,25 +3605,27 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:13">
       <c r="A62" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>275</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
@@ -3640,26 +3633,29 @@
         <v>45</v>
       </c>
       <c r="L62" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M62" s="3"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="M62" s="3"/>
-    </row>
-    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="D63" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
         <v>115</v>
       </c>
@@ -3671,21 +3667,21 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:13">
       <c r="A64" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>169</v>
@@ -3700,31 +3696,34 @@
         <v>19</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L64" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>317</v>
-      </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
         <v>19</v>
       </c>
@@ -3732,56 +3731,60 @@
         <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="M65" s="3"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="M65" s="3"/>
-    </row>
-    <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L66" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="M66" s="3"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="M66" s="3"/>
-    </row>
-    <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>26</v>
       </c>
@@ -3795,29 +3798,31 @@
         <v>45</v>
       </c>
       <c r="L67" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="M67" s="3"/>
-    </row>
-    <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="D68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>290</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
@@ -3825,25 +3830,25 @@
         <v>45</v>
       </c>
       <c r="L68" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="M68" s="3"/>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="M68" s="3"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="D69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
@@ -3856,30 +3861,30 @@
         <v>19</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3895,24 +3900,24 @@
         <v>20</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
@@ -3928,24 +3933,24 @@
         <v>20</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>71</v>
@@ -3960,24 +3965,24 @@
         <v>19</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="B73" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3985,15 +3990,15 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:13">
       <c r="B74" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -4001,15 +4006,15 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:13">
       <c r="B75" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -4017,15 +4022,15 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:13">
       <c r="B76" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -4033,15 +4038,15 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:13">
       <c r="B77" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -4049,15 +4054,15 @@
       </c>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:13">
       <c r="B78" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -4065,23 +4070,23 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:13">
       <c r="B79" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:13">
       <c r="B80" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>290</v>
+        <v>373</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
@@ -4089,9 +4094,9 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="2:8">
       <c r="B81" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>14</v>
@@ -4101,276 +4106,276 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="2:8">
       <c r="B82" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="2:8">
       <c r="B83" s="6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="2:8">
       <c r="B84" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="2:8">
       <c r="B85" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="2:8">
       <c r="B86" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="2:8">
       <c r="B87" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="2:8">
       <c r="B88" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="2:8">
       <c r="B89" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="2:8">
       <c r="B90" s="6" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="2:8">
       <c r="B91" s="6" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="2:8">
       <c r="B92" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="2:8">
       <c r="B93" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="2:8">
       <c r="B94" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="2:8">
       <c r="B95" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="2:8">
       <c r="B96" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:12">
       <c r="A97" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>71</v>
@@ -4385,25 +4390,20 @@
         <v>19</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L32" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
+    <hyperlink ref="L32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed toml to  command
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D230D88-353E-4246-8736-343AEC4CE401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0752B67-6B30-4B67-BE07-C7BEB30BADC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,13 +1145,13 @@
     <t>value_set=[V,G,A,Z];number=3</t>
   </si>
   <si>
-    <t>link=individual_attributes.csv;column=street_address_line</t>
-  </si>
-  <si>
     <t>link=individual_attributes.csv;column=family_name</t>
   </si>
   <si>
     <t>link=individual_attributes.csv;column=first_name</t>
+  </si>
+  <si>
+    <t>link=individual_attributes.csv;column=street_name</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -3188,7 +3188,7 @@
         <v>14</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -3424,7 +3424,7 @@
         <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
@@ -3519,7 +3519,7 @@
         <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
@@ -3619,7 +3619,7 @@
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
@@ -3816,7 +3816,7 @@
         <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
@@ -4086,7 +4086,7 @@
         <v>14</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">

</xml_diff>

<commit_message>
Change English -> German
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0752B67-6B30-4B67-BE07-C7BEB30BADC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,1144 +22,1163 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="374">
   <si>
-    <t>Variable name</t>
-  </si>
-  <si>
-    <t>Concept Id</t>
-  </si>
-  <si>
-    <t>Default values</t>
-  </si>
-  <si>
-    <t>Generation type</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>Nullflavor</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Block Cardinality</t>
-  </si>
-  <si>
-    <t>Cardinality</t>
-  </si>
-  <si>
-    <t>Commentar</t>
-  </si>
-  <si>
-    <t>DWH</t>
-  </si>
-  <si>
-    <t>Pfad</t>
-  </si>
-  <si>
-    <t>Transportmittel Code</t>
-  </si>
-  <si>
-    <t>transportmittel</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>value_set=[1,2,3,4,OTH]</t>
-  </si>
-  <si>
-    <t>OTH,NA</t>
-  </si>
-  <si>
-    <t>generating</t>
-  </si>
-  <si>
-    <t>0..1</t>
-  </si>
-  <si>
-    <t>1..1</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry systolischer Blutdruck</t>
-  </si>
-  <si>
-    <t>blutdruck_sys</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>scope=0-300</t>
-  </si>
-  <si>
-    <t>implemented</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry herzfrequenz</t>
-  </si>
-  <si>
-    <t>herzfrequenz</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>postleitzahl</t>
-  </si>
-  <si>
-    <t>scope=01067-99998</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
-  </si>
-  <si>
-    <t>Versicherungsidentifikation</t>
-  </si>
-  <si>
-    <t>versicherung_iknr</t>
-  </si>
-  <si>
-    <t>scope=100000000-999999999</t>
-  </si>
-  <si>
-    <t>0..n</t>
-  </si>
-  <si>
-    <t>Blockweise mit Versicherungsnamen</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
-  </si>
-  <si>
-    <t>Organisation ID</t>
-  </si>
-  <si>
-    <t>organisation_id</t>
-  </si>
-  <si>
-    <t>scope=1000000000-9999999999</t>
-  </si>
-  <si>
-    <t>kinda sus</t>
-  </si>
-  <si>
-    <t>nein</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/representedOrganisation/id/@extension
+    <t xml:space="preserve">Variable name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generation type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nullflavor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block Cardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportmethode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transportmethode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[1,2,3,4,OTH]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH,NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systolischer Blutdruck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blutdruck_sys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herzfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herzfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postleitzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postleitzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=01067-99998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherung_iknr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=100000000-999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0..n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise mit Versicherungsnamen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/scopingOrganisation/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisationsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organisation_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1000000000-9999999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinda sus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/id/@extension
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/id/@extension</t>
   </si>
   <si>
-    <t>Allergien spezifisch</t>
-  </si>
-  <si>
-    <t>allergien_txt</t>
-  </si>
-  <si>
-    <t>|Allergien|Antibiotika : |</t>
-  </si>
-  <si>
-    <t>Sonstige Allergien sollten hier genannt werden</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t>Ersteinschätzung text</t>
-  </si>
-  <si>
-    <t>ersteinschaetzung_text</t>
-  </si>
-  <si>
-    <t>|triageval|5|triageval|</t>
-  </si>
-  <si>
-    <t>Liste Verweise auf triageEVAL</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/text</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Körpertemperatur</t>
-  </si>
-  <si>
-    <t>kerntemperatur</t>
-  </si>
-  <si>
-    <t>0.335</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>scope=0.0-45.0</t>
-  </si>
-  <si>
-    <t>Version ID</t>
-  </si>
-  <si>
-    <t>version_id</t>
-  </si>
-  <si>
-    <t>0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
-  </si>
-  <si>
-    <t>UUID</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/setId/@extension</t>
-  </si>
-  <si>
-    <t>Basisinfo Schwangerschaftsstatus code</t>
-  </si>
-  <si>
-    <t>schwangerschaft</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>scope=0-1</t>
-  </si>
-  <si>
-    <t>UNK</t>
-  </si>
-  <si>
-    <t>Kein Fehler bei Gender Male</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry GCS verbale Antwort</t>
-  </si>
-  <si>
-    <t>gcs_verbal</t>
-  </si>
-  <si>
-    <t>scope=1-5</t>
-  </si>
-  <si>
-    <t>Was Bei Summe, wenn einer fehlt?</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
-  </si>
-  <si>
-    <t>Ersteinschaetzung Codesystem</t>
-  </si>
-  <si>
-    <t>triage_system</t>
-  </si>
-  <si>
-    <t>1.2.276.0.76.5.438</t>
-  </si>
-  <si>
-    <t>value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
-  </si>
-  <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
-    <t>patient_id</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/id/@extension</t>
-  </si>
-  <si>
-    <t>Document ID</t>
-  </si>
-  <si>
-    <t>dokument_id</t>
-  </si>
-  <si>
-    <t>14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/id/@extension</t>
-  </si>
-  <si>
-    <t>Geburtsdatum patient</t>
-  </si>
-  <si>
-    <t>geburtsdatum_ts</t>
-  </si>
-  <si>
-    <t>19960531</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
-  </si>
-  <si>
-    <t>Beschwerdedauer</t>
-  </si>
-  <si>
-    <t>symptomdauer</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>scope=0-99</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
-  </si>
-  <si>
-    <t>Basisinfo_ranking_skala</t>
-  </si>
-  <si>
-    <t>rankin</t>
-  </si>
-  <si>
-    <t>scope=0-6</t>
-  </si>
-  <si>
-    <t>Valueset(1-6)?</t>
+    <t xml:space="preserve">Allergien spezifisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergien_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|Allergien|Antibiotika : |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige Allergien sollten hier genannt werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschätzung text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ersteinschaetzung_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|triageval|5|triageval|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste Verweise auf triageEVAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Körpertemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerntemperatur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0.0-45.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versionsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0ff0f2d6-ddc2-4300-a5e6-b0aecd1a7dcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/setId/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schwangerschaftsstatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schwangerschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kein Fehler bei Gender Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCS verbale Antwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_verbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was Bei Summe, wenn einer fehlt?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/entryRelationship/observation/value/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschaetzung Codesystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.276.0.76.5.438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[1.2.276.0.76.5.437, 1.2.276.0.76.5.438]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/value/@codeSystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patientsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentsidentifikation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dokument_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14025fda-3f25-4c64-8883-4f7e6cabc0b6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/id/@extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geburtsdatum patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geburtsdatum_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19960531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/birthTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerdedauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">symptomdauer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo_ranking_skala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rankin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valueset(1-6)?</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/text </t>
   </si>
   <si>
-    <t>Vitalparameter Entry GCS Augenöffnen</t>
-  </si>
-  <si>
-    <t>gcs_augen</t>
-  </si>
-  <si>
-    <t>scope=1-4</t>
-  </si>
-  <si>
-    <t>Erstellung durch Author zeit</t>
-  </si>
-  <si>
-    <t>author_ts</t>
-  </si>
-  <si>
-    <t>20150117160900</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>1..n</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/time/@value</t>
-  </si>
-  <si>
-    <t>Datum der DokumentErstellung</t>
-  </si>
-  <si>
-    <t>datum_erstellung</t>
-  </si>
-  <si>
-    <t>20150117163300</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t>Diagnostik Zeitpunkt</t>
-  </si>
-  <si>
-    <t>diagnostik_ts</t>
-  </si>
-  <si>
-    <t>201501171650</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>Diagnostik !!!!!!!!</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
-  </si>
-  <si>
-    <t>Beschwerde Beginn der Symptome</t>
-  </si>
-  <si>
-    <t>beschwerde_begin</t>
-  </si>
-  <si>
-    <t>20150118</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Start Patientenkontakt Ankunfszeit</t>
-  </si>
-  <si>
-    <t>aufnahme_ts</t>
-  </si>
-  <si>
-    <t>20150118070100</t>
-  </si>
-  <si>
-    <t>startunkt</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Therapiebeginn, Aufnahme, Behandlung</t>
-  </si>
-  <si>
-    <t>therapiebeginn_ts</t>
-  </si>
-  <si>
-    <t>20150118071200</t>
-  </si>
-  <si>
-    <t>Begin des Arztkontaktes</t>
-  </si>
-  <si>
-    <t>arztkontakt_ts</t>
-  </si>
-  <si>
-    <t>20150118073500</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmddhhmmss</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
-  </si>
-  <si>
-    <t>Ende des Arztkontaktes</t>
-  </si>
-  <si>
-    <t>end_arztkontakt_ts</t>
-  </si>
-  <si>
-    <t>20150118075100</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
-  </si>
-  <si>
-    <t>Verlegungs-/Entlassungszeitpunkt</t>
-  </si>
-  <si>
-    <t>entlassung_ts</t>
-  </si>
-  <si>
-    <t>20150118083000</t>
-  </si>
-  <si>
-    <t>O..1 =&gt; Problem mit Dependency Triage</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
+    <t xml:space="preserve">GCS Augenöffnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_augen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung durch Author zeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150117160900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1..n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/time/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum der Dokumenterstellung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datum_erstellung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150117163300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Zeitpunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201501171650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik !!!!!!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/effectiveTime/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde Beginn der Symptome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beschwerde_begin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Patientenkontakt Aufnahmezeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aufnahme_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118070100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapiebeginn, Aufnahme, Behandlung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">therapiebeginn_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118071200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begin des Arztkontaktes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arztkontakt_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118073500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmddhhmmss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende des Arztkontaktes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_arztkontakt_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118075100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/performer/time/high/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verlegungs-/Entlassungszeitpunkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entlassung_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20150118083000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O..1 =&gt; Problem mit Dependency Triage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/documentationOf/serviceEvent/effectiveTime/high/@value, 
 ClinicalDocument/componentOf/encompassingEncounter/effectiveTime/high/@value</t>
   </si>
   <si>
-    <t>Ersteinschätzung zeit start</t>
-  </si>
-  <si>
-    <t>triage_ts_start</t>
-  </si>
-  <si>
-    <t>202006201603</t>
-  </si>
-  <si>
-    <t>date_format=yyyymmddhhmm</t>
-  </si>
-  <si>
-    <t>nach entlassung</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
-  </si>
-  <si>
-    <t>Ersteinschätzung zeit ende</t>
-  </si>
-  <si>
-    <t>triage_ts_end</t>
-  </si>
-  <si>
-    <t>202006201608</t>
-  </si>
-  <si>
-    <t>effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
+    <t xml:space="preserve">Ersteinschätzung zeit start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_ts_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202006201603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_format=yyyymmddhhmm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nach entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschätzung zeit ende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage_ts_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202006201608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveTime wird auch als "biologisch relevante Zeit" bezeichnet und ist der Zeitpunkt oder Zeitraum, für den die Beobachtung für den Patienten gilt.
 Beispiel: Für Gesundheitsdienstleister, die einen Patienten heute in der Klinik sehen anamenstisch einen Herzinfarkt erheben, der vor fünf Jahren stattgefunden hat, ist effectiveTime: vor fünf Jahren.
 Die effectiveTime hier ist die definitive Angabe, ob die zugrunde liegende Erkrankung behoben ist. effectiveTime.low ist der Beginn des Problems für den Patienten. Wenn das Problem noch nicht gelöst ist, wird effectiveTime.high nicht gesetzt. Wenn bekannt ist, dass das Problem gelöst werden kann, dann ist effectiveTime.high vorhanden. Wenn der genaue Zeitpunkt der Lösung des Problems nicht bekannt ist, dann ist effectiveTime.high vorhanden und auf nullFlavor "UNK" gesetzt.</t>
   </si>
   <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
-  </si>
-  <si>
-    <t>Beschwerde Code</t>
-  </si>
-  <si>
-    <t>cedis</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>link=cedis.csv;column=cedis</t>
-  </si>
-  <si>
-    <t>OTH,UNK</t>
-  </si>
-  <si>
-    <t>nullflavor</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
-  </si>
-  <si>
-    <t>Diagnostik Code Welche Untersuchung?</t>
-  </si>
-  <si>
-    <t>diagnostik_code</t>
-  </si>
-  <si>
-    <t>37637-6</t>
-  </si>
-  <si>
-    <t>link=diagnostics.csv;column=diagnostik_code</t>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/high/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH,UNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nullflavor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Code Welche Untersuchung?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37637-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=diagnostics.csv;column=diagnostik_code</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise Generieren </t>
   </si>
   <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
-  </si>
-  <si>
-    <t>Basisinfo multiresistente</t>
-  </si>
-  <si>
-    <t>keime</t>
-  </si>
-  <si>
-    <t>3MRGN</t>
-  </si>
-  <si>
-    <t>value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
-  </si>
-  <si>
-    <t>OTH</t>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo multiresistente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3MRGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[AMRO,MRSA, 3MRGN, 4MRGN, VRE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTH</t>
   </si>
   <si>
     <t xml:space="preserve">	Multiresistenter Keim Ja/Nein/Verdacht; wenn angegeben soll, dass der in observation.value angegebene Keim NICHT vorliegt, wird observation.@negationInd="true" gesetzt. Bei "Verdacht" ist der Befundstatus in observation.value.qualifier entsprechend zu setzen.</t>
   </si>
   <si>
-    <t>EntlassungsGrund</t>
-  </si>
-  <si>
-    <t>entlassung</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>scope=1-6</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
-  </si>
-  <si>
-    <t>Ersteinschaetzung code</t>
-  </si>
-  <si>
-    <t>triage</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Beide Systeme haben 1-5</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Atemfrequenz</t>
-  </si>
-  <si>
-    <t>atemfrequenz</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry GCS motorische Antwort</t>
-  </si>
-  <si>
-    <t>gcs_motorisch</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Sauerstoffsättigung</t>
-  </si>
-  <si>
-    <t>saettigung</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>scope=0-100</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry  Schmerzskala</t>
-  </si>
-  <si>
-    <t>schmerzskala</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>scope=0-10</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Glasgoe Coma Scale Summe</t>
-  </si>
-  <si>
-    <t>gcs_summe</t>
-  </si>
-  <si>
-    <t>scope=3-15</t>
+    <t xml:space="preserve">EntlassungsGrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=1-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ersteinschaetzung code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beide Systeme haben 1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atemfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atemfrequenz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCS motorische Antwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_motorisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauerstoffsättigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saettigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schmerzskala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schmerzskala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=0-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glasgow Coma Scale Summe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcs_summe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=3-15</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
   </si>
   <si>
-    <t>Aufnahme ID</t>
-  </si>
-  <si>
-    <t>encounter_id</t>
-  </si>
-  <si>
-    <t>987654321-04</t>
-  </si>
-  <si>
-    <t>regex=\d{9}-\d\d</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
+    <t xml:space="preserve">Aufnahme ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aufnahme_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654321-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regex=\d{9}-\d\d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/id/@extension</t>
   </si>
   <si>
     <t xml:space="preserve">Beschwerde bei Vorstellung Textfeld Liste mit allen Beschwerden </t>
   </si>
   <si>
-    <t>beschwerde_liste</t>
-  </si>
-  <si>
-    <t>AZ-Verschlechterung</t>
-  </si>
-  <si>
-    <t>Verweise auf Beschwerde</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/text/content</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenreaktion (links)</t>
-  </si>
-  <si>
-    <t>pupillenreaktion_links</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>value_set=[B, D, A]</t>
-  </si>
-  <si>
-    <t>Notfallanamnese</t>
-  </si>
-  <si>
-    <t>notfallanamnese</t>
+    <t xml:space="preserve">beschwerde_liste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ-Verschlechterung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verweise auf Beschwerde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/text/content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupillenreaktion (links)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenreaktion_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[B, D, A]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notfallanamnese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notfallanamnese</t>
   </si>
   <si>
     <t xml:space="preserve">Bei einem Hausbesuch im Pflegeheim...    </t>
   </si>
   <si>
-    <t>ChatGPT Text gnerierung aus allen Parametern</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenweite (links)</t>
-  </si>
-  <si>
-    <t>pupillenweite_links</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>value_set=[D, M, C]</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenweite (rechts)</t>
-  </si>
-  <si>
-    <t>pupillenweite_rechts</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Vitalparameter Entry Pupillenreaktion (rechts)</t>
-  </si>
-  <si>
-    <t>pupillenreaktion_rechts</t>
-  </si>
-  <si>
-    <t>Street Address Line</t>
-  </si>
-  <si>
-    <t>street_address_line</t>
-  </si>
-  <si>
-    <t>Dachauer Straße 112</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
-  </si>
-  <si>
-    <t>Abschlussdiagnose Freitext</t>
-  </si>
-  <si>
-    <t>diagnose_txt</t>
-  </si>
-  <si>
-    <t>Distorsion unteres Sprunggelenk (S96.3)</t>
-  </si>
-  <si>
-    <t>chatGPT text aus Beschwerde code generieren</t>
-  </si>
-  <si>
-    <t>Author prefix</t>
-  </si>
-  <si>
-    <t>prefix_author</t>
-  </si>
-  <si>
-    <t>Dr. med.</t>
-  </si>
-  <si>
-    <t>value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
-  </si>
-  <si>
-    <t>Beschwerde originaltext</t>
-  </si>
-  <si>
-    <t>beschwerden_txt</t>
-  </si>
-  <si>
-    <t>Durchfall und Erbrechen</t>
-  </si>
-  <si>
-    <t>ist 0..1 in doku soll aber immer da sein</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
-  </si>
-  <si>
-    <t>Diagnostik  displayName</t>
-  </si>
-  <si>
-    <t>diagnostik_display_name</t>
-  </si>
-  <si>
-    <t>Extremity X-ray</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Blockweise Diagnostik REMOVE</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
-  </si>
-  <si>
-    <t>Basisinfo_tetanusschutz</t>
-  </si>
-  <si>
-    <t>tetanusschutz</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>value_set=[true,false]</t>
-  </si>
-  <si>
-    <t>NI</t>
+    <t xml:space="preserve">ChatGPT Text gnerierung aus allen Parametern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupillenweite (links)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenweite_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[D, M, C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupillenweite (rechts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenweite_rechts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupillenreaktion (rechts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupillenreaktion_rechts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straßenadressenzeile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strassenadressenzeile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dachauer Straße 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=individual_attributes.csv;column=strassenname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/streetAddressLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abschlussdiagnose Freitext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chatGPT text aus Beschwerde code generieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. med.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[Dr.med.,Dr.rer.med, Dr.rer.med., Dr.rer.Medic]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschwerde originaltext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beschwerden_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durchfall und Erbrechen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ist 0..1 in doku soll aber immer da sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/originalText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik  displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_display_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extremity X-ray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Diagnostik REMOVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/observation/code/@displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basisinfo_tetanusschutz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tetanusschutz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[true,false]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NI</t>
   </si>
   <si>
     <t xml:space="preserve">Bei Nullflavor=NI muss negationInd=false sein </t>
   </si>
   <si>
-    <t>Antibiotikaallergie</t>
-  </si>
-  <si>
-    <t>allergie_antibiotika</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
-  </si>
-  <si>
-    <t>Patient family name</t>
-  </si>
-  <si>
-    <t>family_patient</t>
-  </si>
-  <si>
-    <t>Kicker</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
-  </si>
-  <si>
-    <t>Zuweisung Code</t>
-  </si>
-  <si>
-    <t>zuweisung</t>
-  </si>
-  <si>
-    <t>KVNDAK</t>
-  </si>
-  <si>
-    <t>value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>value_set=[M,F,UN]</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
-  </si>
-  <si>
-    <t>Author given name</t>
-  </si>
-  <si>
-    <t>given_author</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>München</t>
-  </si>
-  <si>
-    <t>link=clinics.csv;column=city</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
-  </si>
-  <si>
-    <t>Diagnostik Ergebnis</t>
-  </si>
-  <si>
-    <t>diagnostik_ergebnis_code</t>
-  </si>
-  <si>
-    <t>OPB</t>
-  </si>
-  <si>
-    <t>value_set=[PB, OPB]</t>
-  </si>
-  <si>
-    <t>Blockweise Generieren</t>
-  </si>
-  <si>
-    <t>Author family name</t>
-  </si>
-  <si>
-    <t>family_author</t>
-  </si>
-  <si>
-    <t>Regensburger</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
-  </si>
-  <si>
-    <t>Diagnostik ganzer Text</t>
-  </si>
-  <si>
-    <t>diagnostik_text</t>
-  </si>
-  <si>
-    <t>Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE</t>
-  </si>
-  <si>
-    <t>diagnose_code</t>
-  </si>
-  <si>
-    <t>S93.6</t>
-  </si>
-  <si>
-    <t>link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
-  </si>
-  <si>
-    <t>NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
-  </si>
-  <si>
-    <t>ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
-  </si>
-  <si>
-    <t>Versicherungs Name</t>
-  </si>
-  <si>
-    <t>versicherung_txt</t>
-  </si>
-  <si>
-    <t>Selbstzahler</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/associatedOrganisation/name</t>
-  </si>
-  <si>
-    <t>Versicherungsfall</t>
-  </si>
-  <si>
-    <t>insurance_case</t>
-  </si>
-  <si>
-    <t>SELF</t>
-  </si>
-  <si>
-    <t>value_set=[FAMDEP,SELF]</t>
-  </si>
-  <si>
-    <t>If FAMDEP then AssociatedPerson</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/participant/associatedEntity/code/@code</t>
-  </si>
-  <si>
-    <t>Organisation name</t>
-  </si>
-  <si>
-    <t>organisation_name</t>
-  </si>
-  <si>
-    <t>Städtisches Klinikum München GmbH</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/author/representedOrganisation/name
+    <t xml:space="preserve">Antibiotikaallergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_antibiotika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@negationInd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient Nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nachname_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=individual_attributes.csv;column=nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zuweisung Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zuweisung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KVNDAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[VAP, KVNPIK, KVNDAK, RD, NA, KLINV, NPHYS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/participant/participantRole/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[M,F,UN]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author Vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vorname_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stadt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">München</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=clinics.csv;column=stadt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik Ergebnis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ergebnis_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[PB, OPB]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blockweise Generieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author family name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nachname_author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regensburger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostik ganzer Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Röntgenuntersuchung des Sprunggelenks: einfache Distorsionsverletzung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S93.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen;number=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungs Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherung_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selbstzahler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/associatedOrganisation/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungsfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherungsfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[FAMDEP,SELF]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If FAMDEP then AssociatedPerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/participant/associatedEntity/code/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organisation_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
 ClinicalDocument/custodian/assignedCustodian/representedCustodianOrganization/name</t>
   </si>
   <si>
-    <t>Patient given name</t>
-  </si>
-  <si>
-    <t>given_patient</t>
-  </si>
-  <si>
-    <t>Timo</t>
-  </si>
-  <si>
-    <t>ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
-  </si>
-  <si>
-    <t>Allergien vorhanden?</t>
-  </si>
-  <si>
-    <t>allergie</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>mindestens eine Allergy obsseration muss da sein</t>
-  </si>
-  <si>
-    <t>Kontrastmittelallergie</t>
-  </si>
-  <si>
-    <t>allergie_kontrastmittel</t>
-  </si>
-  <si>
-    <t>sonstige allergien vorhanden</t>
-  </si>
-  <si>
-    <t>allergie_sonstige</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE originalText</t>
-  </si>
-  <si>
-    <t>diagnose_name</t>
-  </si>
-  <si>
-    <t>Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
-  </si>
-  <si>
-    <t>number=3</t>
-  </si>
-  <si>
-    <t>Auf Diagnose abstimmen</t>
-  </si>
-  <si>
-    <t>_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t>scope=10-120</t>
-  </si>
-  <si>
-    <t>_therapiebeginn_arztkontakt</t>
-  </si>
-  <si>
-    <t>_arztkontakt_endarztkontakt</t>
-  </si>
-  <si>
-    <t>_endarztkontakt_entlassung</t>
-  </si>
-  <si>
-    <t>_entlassung_triagestart</t>
-  </si>
-  <si>
-    <t>_triagestart_triageend</t>
-  </si>
-  <si>
-    <t>_diagnostik_id</t>
-  </si>
-  <si>
-    <t>_associatedPerson_given</t>
-  </si>
-  <si>
-    <t>_associatedPerson_family</t>
-  </si>
-  <si>
-    <t>diagnostik_labor</t>
-  </si>
-  <si>
-    <t>diagnostik_blutgase</t>
-  </si>
-  <si>
-    <t>diagnostik_urinschnelltest</t>
-  </si>
-  <si>
-    <t>diagnostik_ekg</t>
-  </si>
-  <si>
-    <t>diagnostik_sonographie</t>
-  </si>
-  <si>
-    <t>diagnostik_echokardiographie</t>
-  </si>
-  <si>
-    <t>diagnostik_ct_kopf</t>
-  </si>
-  <si>
-    <t>diagnostik_ct</t>
-  </si>
-  <si>
-    <t>diagnostik_ct_trauma</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_wirbelsaeule</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_thorax</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_becken</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_extremitaeten</t>
-  </si>
-  <si>
-    <t>diagnostik_roentgen_sonstiges</t>
-  </si>
-  <si>
-    <t>diagnostik_mrt</t>
-  </si>
-  <si>
-    <t>Diagnose ICD10 CODE Qualifier</t>
-  </si>
-  <si>
-    <t>diagnose_qualifier</t>
-  </si>
-  <si>
-    <t>value_set=[V,G,A,Z];number=3</t>
-  </si>
-  <si>
-    <t>link=individual_attributes.csv;column=family_name</t>
-  </si>
-  <si>
-    <t>link=individual_attributes.csv;column=first_name</t>
-  </si>
-  <si>
-    <t>link=individual_attributes.csv;column=street_name</t>
+    <t xml:space="preserve">Patient given name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vorname_patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link=individual_attributes.csv;column=vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/patient/name/given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allergien vorhanden?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mindestens eine Allergy obsseration muss da sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontrastmittelallergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_kontrastmittel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonstige allergien vorhanden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allergie_sonstige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auf Diagnose abstimmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_aufnahme_therapiebeginn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scope=10-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_arztkontakt_endarztkontakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_endarztkontakt_entlassung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_entlassung_triagestart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_triagestart_triageend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_diagnostik_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_associatedPerson_vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_associatedPerson_nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_blutgase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_urinschnelltest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ekg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_sonographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_echokardiographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct_kopf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_ct_trauma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_wirbelsaeule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_thorax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_becken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_extremitaeten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_roentgen_sonstiges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostik_mrt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose ICD10 CODE Qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnose_qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[V,G,A,Z];number=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1174,7 +1188,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1189,7 +1203,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -1203,6 +1217,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1213,7 +1233,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1221,34 +1241,97 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="13">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1307,76 +1390,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="145F82"/>
+        <a:srgbClr val="145f82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E87331"/>
+        <a:srgbClr val="e87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="186C24"/>
+        <a:srgbClr val="186c24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1408,7 +1475,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1432,7 +1499,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1492,41 +1559,42 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="38.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="3" customWidth="1"/>
-    <col min="7" max="8" width="20.25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="112.75" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="77.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="112.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1564,14 +1632,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1599,14 +1667,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1633,14 +1701,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1667,14 +1735,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="2" t="n">
         <v>80636</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1701,14 +1769,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="2" t="n">
         <v>987654321</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1737,14 +1805,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="2" t="n">
         <v>9814184919</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1773,7 +1841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1786,12 +1854,9 @@
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1806,7 +1871,7 @@
       </c>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1819,12 +1884,9 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1839,7 +1901,7 @@
       </c>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1875,7 +1937,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1902,7 +1964,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -1938,7 +2000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>74</v>
       </c>
@@ -1974,7 +2036,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>79</v>
       </c>
@@ -1990,11 +2052,9 @@
       <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2006,7 +2066,7 @@
       </c>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2022,11 +2082,9 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2038,7 +2096,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
@@ -2051,12 +2109,9 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2123,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2084,11 +2139,9 @@
       <c r="E17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2100,7 +2153,7 @@
       </c>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -2135,7 +2188,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -2151,11 +2204,9 @@
       <c r="E19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2170,7 +2221,7 @@
       </c>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -2204,7 +2255,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2237,7 +2288,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -2253,11 +2304,9 @@
       <c r="E22" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2269,7 +2318,7 @@
       </c>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -2305,7 +2354,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>127</v>
       </c>
@@ -2338,7 +2387,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>132</v>
       </c>
@@ -2354,11 +2403,9 @@
       <c r="E25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2420,7 @@
       </c>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>137</v>
       </c>
@@ -2406,7 +2453,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>140</v>
       </c>
@@ -2422,11 +2469,9 @@
       <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2438,7 +2483,7 @@
       </c>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -2454,11 +2499,9 @@
       <c r="E28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2470,7 +2513,7 @@
       </c>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="30">
+    <row r="29" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -2486,11 +2529,9 @@
       <c r="E29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2546,7 @@
       </c>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>154</v>
       </c>
@@ -2521,11 +2562,9 @@
       <c r="E30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
         <v>19</v>
       </c>
@@ -2540,7 +2579,7 @@
       </c>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" ht="360">
+    <row r="31" s="1" customFormat="true" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>160</v>
       </c>
@@ -2556,11 +2595,9 @@
       <c r="E31" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
         <v>18</v>
       </c>
@@ -2575,7 +2612,7 @@
       </c>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>165</v>
       </c>
@@ -2611,7 +2648,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16.5" customHeight="1">
+    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>172</v>
       </c>
@@ -2645,7 +2682,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>178</v>
       </c>
@@ -2681,7 +2718,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -2717,7 +2754,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>189</v>
       </c>
@@ -2733,11 +2770,9 @@
       <c r="E36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2752,7 +2787,7 @@
       </c>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>193</v>
       </c>
@@ -2788,7 +2823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>196</v>
       </c>
@@ -2824,7 +2859,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>199</v>
       </c>
@@ -2860,7 +2895,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
@@ -2896,7 +2931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>207</v>
       </c>
@@ -2932,7 +2967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
@@ -2965,7 +3000,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -2995,7 +3030,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>221</v>
       </c>
@@ -3033,7 +3068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>225</v>
       </c>
@@ -3060,7 +3095,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>229</v>
       </c>
@@ -3098,7 +3133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
         <v>233</v>
       </c>
@@ -3136,7 +3171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>236</v>
       </c>
@@ -3174,7 +3209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>238</v>
       </c>
@@ -3188,7 +3223,7 @@
         <v>14</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>373</v>
+        <v>241</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -3204,33 +3239,30 @@
         <v>45</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>20</v>
@@ -3240,21 +3272,21 @@
       </c>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3270,95 +3302,90 @@
         <v>45</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H53" s="1"/>
+        <v>260</v>
+      </c>
       <c r="I53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>17</v>
@@ -3368,7 +3395,7 @@
         <v>18</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>20</v>
@@ -3377,21 +3404,21 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
@@ -3407,30 +3434,28 @@
         <v>20</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F56" s="1"/>
+        <v>275</v>
+      </c>
       <c r="G56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>115</v>
       </c>
@@ -3438,25 +3463,25 @@
         <v>45</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F57" s="11"/>
       <c r="G57" s="11" t="s">
@@ -3470,30 +3495,28 @@
         <v>20</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>285</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>19</v>
       </c>
@@ -3501,31 +3524,29 @@
         <v>20</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>275</v>
+      </c>
       <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
@@ -3533,25 +3554,25 @@
         <v>45</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
@@ -3567,35 +3588,33 @@
         <v>45</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>299</v>
+      </c>
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>20</v>
@@ -3605,27 +3624,25 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>275</v>
+      </c>
       <c r="G62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
@@ -3633,29 +3650,26 @@
         <v>45</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
         <v>115</v>
       </c>
@@ -3667,21 +3681,21 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>169</v>
@@ -3696,34 +3710,31 @@
         <v>19</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
         <v>19</v>
       </c>
@@ -3731,60 +3742,56 @@
         <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>321</v>
+      </c>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
         <v>26</v>
       </c>
@@ -3798,31 +3805,29 @@
         <v>45</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M67" s="3"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="F68" s="1"/>
+        <v>331</v>
+      </c>
       <c r="G68" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
@@ -3830,25 +3835,25 @@
         <v>45</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
@@ -3861,30 +3866,30 @@
         <v>19</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>332</v>
-      </c>
       <c r="D70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
@@ -3900,24 +3905,24 @@
         <v>20</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
@@ -3933,24 +3938,24 @@
         <v>20</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>71</v>
@@ -3965,24 +3970,24 @@
         <v>19</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
@@ -3990,15 +3995,15 @@
       </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
@@ -4006,15 +4011,15 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
@@ -4022,15 +4027,15 @@
       </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
@@ -4038,15 +4043,15 @@
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
@@ -4054,15 +4059,15 @@
       </c>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
@@ -4070,23 +4075,23 @@
       </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>372</v>
+        <v>331</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
@@ -4094,9 +4099,9 @@
       </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="2:8">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>14</v>
@@ -4106,276 +4111,276 @@
       </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="2:8">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="6" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="2:8">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="6" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="2:8">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="6" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="2:8">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="6" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="2:8">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="6" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="2:8">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="6" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="2:8">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="6" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="2:8">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="6" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="2:8">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="6" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="2:8">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="6" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="2:8">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="6" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="2:8">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="6" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="2:8">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="2:8">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="2:8">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>71</v>
@@ -4390,20 +4395,25 @@
         <v>19</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L32" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
   </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change scope to range for clarity
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-300</t>
+    <t xml:space="preserve">range=0-300</t>
   </si>
   <si>
     <t xml:space="preserve">implemented</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">postleitzahl</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=01067-99998</t>
+    <t xml:space="preserve">range=01067-99998</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/postalCode</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">versicherung_iknr</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=100000000-999999999</t>
+    <t xml:space="preserve">range=100000000-999999999</t>
   </si>
   <si>
     <t xml:space="preserve">0..n</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">organisation_id</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=1000000000-9999999999</t>
+    <t xml:space="preserve">range=1000000000-9999999999</t>
   </si>
   <si>
     <t xml:space="preserve">kinda sus</t>
@@ -206,7 +206,7 @@
     <t xml:space="preserve">float</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0.0-45.0</t>
+    <t xml:space="preserve">range=0.0-45.0</t>
   </si>
   <si>
     <t xml:space="preserve">Versionsidentifikation</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-1</t>
+    <t xml:space="preserve">range=0-1</t>
   </si>
   <si>
     <t xml:space="preserve">UNK</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">gcs_verbal</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=1-5</t>
+    <t xml:space="preserve">range=1-5</t>
   </si>
   <si>
     <t xml:space="preserve">Was Bei Summe, wenn einer fehlt?</t>
@@ -326,7 +326,7 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-99</t>
+    <t xml:space="preserve">range=0-99</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/act/effectiveTime/width/@value</t>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">rankin</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-6</t>
+    <t xml:space="preserve">range=0-6</t>
   </si>
   <si>
     <t xml:space="preserve">Valueset(1-6)?</t>
@@ -353,7 +353,7 @@
     <t xml:space="preserve">gcs_augen</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=1-4</t>
+    <t xml:space="preserve">range=1-4</t>
   </si>
   <si>
     <t xml:space="preserve">Erstellung durch Author zeit</t>
@@ -590,7 +590,7 @@
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=1-6</t>
+    <t xml:space="preserve">range=1-6</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/componentOf/encompassingEncounter/dischargeDispositionCode/@code</t>
@@ -635,7 +635,7 @@
     <t xml:space="preserve">88</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-100</t>
+    <t xml:space="preserve">range=0-100</t>
   </si>
   <si>
     <t xml:space="preserve">Schmerzskala</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">9</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=0-10</t>
+    <t xml:space="preserve">range=0-10</t>
   </si>
   <si>
     <t xml:space="preserve">Glasgow Coma Scale Summe</t>
@@ -656,7 +656,7 @@
     <t xml:space="preserve">gcs_summe</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=3-15</t>
+    <t xml:space="preserve">range=3-15</t>
   </si>
   <si>
     <t xml:space="preserve">Blockweise 0..1 Sollte Summe sein aus den drei anderen GCS (wird nicht Validiert) </t>
@@ -1071,7 +1071,7 @@
     <t xml:space="preserve">_aufnahme_therapiebeginn</t>
   </si>
   <si>
-    <t xml:space="preserve">scope=10-120</t>
+    <t xml:space="preserve">range=10-120</t>
   </si>
   <si>
     <t xml:space="preserve">_therapiebeginn_arztkontakt</t>
@@ -1577,8 +1577,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Create new column in Excel: "Nullable" indicating, if variable can contains NullFlavors
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="380">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Parameters</t>
   </si>
   <si>
+    <t xml:space="preserve">Nullable</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nullflavor</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">range=10-120</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
     <t xml:space="preserve">implemented</t>
   </si>
   <si>
@@ -296,6 +302,9 @@
   </si>
   <si>
     <t xml:space="preserve">date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">UNK</t>
@@ -1606,10 +1615,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:XFD96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F92" activeCellId="0" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1619,13 +1628,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="115.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="31.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="112.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="3" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="31.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="112.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="1" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,1688 +1674,1876 @@
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="3"/>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="M12" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M14" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M16" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>16</v>
+        <v>69</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M17" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K18" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="J18" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="L18" s="1" t="s">
-        <v>75</v>
+        <v>45</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M19" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>93</v>
+      <c r="M21" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M22" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M23" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="6"/>
       <c r="L24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>41</v>
+        <v>114</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="M25" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M26" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>122</v>
+        <v>43</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M27" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M30" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M31" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>143</v>
+        <v>45</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="6" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>74</v>
+        <v>140</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="M38" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="6" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>86</v>
+        <v>21</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M47" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="1"/>
       <c r="H48" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>170</v>
+        <v>45</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M49" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N49" s="3"/>
     </row>
     <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>68</v>
+        <v>178</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="M50" s="0"/>
+        <v>70</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N50" s="0"/>
     </row>
     <row r="51" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="M51" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N51" s="3"/>
     </row>
     <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>40</v>
+        <v>188</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="M52" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N52" s="3"/>
     </row>
     <row r="53" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>190</v>
+        <v>42</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L53" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="M53" s="0"/>
+        <v>193</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M53" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="N53" s="0"/>
     </row>
     <row r="54" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>195</v>
+        <v>43</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="M54" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N54" s="0"/>
     </row>
     <row r="55" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>16</v>
+        <v>203</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J55" s="6"/>
-      <c r="K55" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K55" s="6"/>
       <c r="L55" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M55" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="N55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M56" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>16</v>
+        <v>211</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M57" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N57" s="3"/>
     </row>
     <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>16</v>
+        <v>216</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>217</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M58" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="N58" s="3"/>
     </row>
     <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M59" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N59" s="0"/>
     </row>
     <row r="60" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="M60" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N60" s="3"/>
     </row>
     <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>174</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>16</v>
+        <v>109</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J61" s="6"/>
-      <c r="K61" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K61" s="6"/>
       <c r="L61" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M61" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N61" s="3"/>
     </row>
     <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>40</v>
+        <v>188</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>231</v>
+        <v>42</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>43</v>
+        <v>234</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M62" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N63" s="0"/>
+        <v>70</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="O63" s="0"/>
       <c r="P63" s="0"/>
       <c r="Q63" s="0"/>
@@ -19720,1101 +19917,1198 @@
     </row>
     <row r="64" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>86</v>
+        <v>243</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="M64" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="N64" s="3"/>
     </row>
     <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K65" s="1" t="s">
-        <v>86</v>
+      <c r="F65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="M65" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="M66" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N66" s="3"/>
     </row>
     <row r="67" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>9814184919</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>48</v>
+        <v>255</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>253</v>
+        <v>76</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>86</v>
+        <v>256</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="M67" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N67" s="3"/>
     </row>
     <row r="68" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="M68" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N68" s="0"/>
     </row>
     <row r="69" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K69" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="M69" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="N69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>80636</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J70" s="6"/>
-      <c r="K70" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K70" s="6"/>
       <c r="L70" s="1" t="s">
-        <v>266</v>
+        <v>45</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K71" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>271</v>
+        <v>88</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="F73" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J73" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K73" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J74" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J75" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>41</v>
+        <v>290</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>43</v>
+        <v>291</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M76" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" s="1"/>
       <c r="H77" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J77" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="1"/>
       <c r="H78" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J78" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I79" s="1"/>
       <c r="J79" s="1" t="s">
-        <v>299</v>
+        <v>43</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>43</v>
+        <v>302</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>152</v>
+        <v>45</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G80" s="1"/>
       <c r="H80" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>304</v>
+        <v>88</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81" s="1"/>
       <c r="H81" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>86</v>
+        <v>42</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>309</v>
+        <v>88</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K82" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="J82" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="L82" s="1" t="s">
-        <v>312</v>
+        <v>45</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>315</v>
+        <v>94</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I83" s="1"/>
       <c r="J83" s="1" t="s">
-        <v>316</v>
+        <v>42</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>43</v>
+        <v>319</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>164</v>
+        <v>45</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G84" s="1"/>
       <c r="H84" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K84" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="J84" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="L84" s="1" t="s">
-        <v>81</v>
+        <v>45</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>323</v>
+        <v>94</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>48</v>
+        <v>326</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J85" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>324</v>
+        <v>45</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M86" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="K86" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="M86" s="0"/>
+      <c r="N86" s="0"/>
     </row>
     <row r="87" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K87" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J87" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="M87" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N87" s="0"/>
     </row>
     <row r="88" s="1" customFormat="true" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J88" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>86</v>
+        <v>340</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K88" s="10" t="s">
+        <v>341</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="M88" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N88" s="0"/>
     </row>
     <row r="89" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>41</v>
+      <c r="F89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>343</v>
+        <v>43</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>43</v>
+        <v>346</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="M89" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="N89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>987654321</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G90" s="1"/>
       <c r="H90" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>348</v>
+        <v>76</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L90" s="11" t="s">
-        <v>349</v>
+        <v>351</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M90" s="11" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K91" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="M91" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="N91" s="0"/>
     </row>
     <row r="92" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>40</v>
+        <v>360</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>86</v>
+        <v>361</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="M92" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="N92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>86</v>
+        <v>178</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>363</v>
+        <v>88</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K94" s="1" t="s">
-        <v>86</v>
+        <v>243</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="M94" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="N94" s="0"/>
     </row>
     <row r="95" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K95" s="1" t="s">
-        <v>86</v>
+        <v>25</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="M95" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="N95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H96" s="12"/>
-      <c r="I96" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K96" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I96" s="12"/>
+      <c r="J96" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>376</v>
+        <v>45</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L25" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
+    <hyperlink ref="M25" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Change generator logic. It generates a list that has a length = number of patients. Then with a given probability there would be removed some entries
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1617,8 +1617,8 @@
   </sheetPr>
   <dimension ref="A1:XFD96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F92" activeCellId="0" sqref="F92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E79" activeCellId="0" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Change temporary generator for Strings to produce not empty strings (for validation purposes). Adjust correct names for diagnosen with underscore and number
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -388,7 +388,7 @@
     <t xml:space="preserve">Diagnose ICD10 CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnose_code</t>
+    <t xml:space="preserve">diagnose_code_1</t>
   </si>
   <si>
     <t xml:space="preserve">S93.6</t>
@@ -406,7 +406,7 @@
     <t xml:space="preserve">Diagnose ICD10 CODE originalText</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnose_name</t>
+    <t xml:space="preserve">diagnose_name_1</t>
   </si>
   <si>
     <t xml:space="preserve">Verstauchung und Zerrung sonstiger und nicht näher bezeichneter Teile des Fußes</t>
@@ -418,7 +418,7 @@
     <t xml:space="preserve">Diagnose ICD10 CODE Qualifier</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnose_qualifier</t>
+    <t xml:space="preserve">diagnose_qualifier_1</t>
   </si>
   <si>
     <t xml:space="preserve">value_set=[V,G,A,Z]</t>
@@ -427,7 +427,7 @@
     <t xml:space="preserve">Abschlussdiagnose Freitext</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnose_txt</t>
+    <t xml:space="preserve">diagnose_txt_1</t>
   </si>
   <si>
     <t xml:space="preserve">Distorsion unteres Sprunggelenk (S96.3)</t>
@@ -1300,7 +1300,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1310,10 +1310,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1351,31 +1347,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF467886"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1616,10 +1587,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1635,48 +1606,47 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="31.75"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="112.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="1" width="9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1810,7 +1780,6 @@
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -1831,7 +1800,6 @@
       <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -1895,7 +1863,7 @@
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1961,7 +1929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1996,7 +1964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -2028,11 +1996,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2060,11 +2028,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2088,7 +2056,7 @@
       <c r="J17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -2133,11 +2101,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2238,11 +2206,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -2309,7 +2277,7 @@
       <c r="A24" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C24" s="2" t="n">
@@ -2333,7 +2301,7 @@
       <c r="J24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="5"/>
       <c r="L24" s="1" t="s">
         <v>70</v>
       </c>
@@ -2341,7 +2309,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>110</v>
       </c>
@@ -2375,7 +2343,7 @@
       <c r="L25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="7" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2411,7 +2379,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>121</v>
       </c>
@@ -2452,7 +2420,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
@@ -2490,7 +2458,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>131</v>
       </c>
@@ -2531,7 +2499,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>134</v>
       </c>
@@ -2563,11 +2531,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>139</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2587,10 +2555,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -2613,7 +2581,7 @@
       <c r="A33" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>145</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2636,7 +2604,7 @@
       <c r="A34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2659,7 +2627,7 @@
       <c r="A35" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -2682,7 +2650,7 @@
       <c r="A36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -2705,7 +2673,7 @@
       <c r="A37" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -2728,7 +2696,7 @@
       <c r="A38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -2748,10 +2716,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -2771,10 +2739,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2794,10 +2762,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2820,7 +2788,7 @@
       <c r="A42" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2840,10 +2808,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -2863,10 +2831,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -2952,11 +2920,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>179</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -3004,7 +2972,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>185</v>
       </c>
@@ -3036,11 +3004,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>190</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -3078,7 +3046,7 @@
       <c r="A51" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>196</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -3105,7 +3073,7 @@
       <c r="L51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M51" s="9" t="s">
+      <c r="M51" s="8" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3141,11 +3109,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>206</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -3169,7 +3137,7 @@
       <c r="J53" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K53" s="6"/>
+      <c r="K53" s="5"/>
       <c r="L53" s="1" t="s">
         <v>70</v>
       </c>
@@ -3178,10 +3146,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>211</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -3205,7 +3173,7 @@
       <c r="J54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K54" s="6" t="s">
+      <c r="K54" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L54" s="1" t="s">
@@ -3215,11 +3183,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="55" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -3243,7 +3211,7 @@
       <c r="J55" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="K55" s="5" t="s">
         <v>217</v>
       </c>
       <c r="L55" s="1" t="s">
@@ -3253,11 +3221,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -3281,7 +3249,7 @@
       <c r="J56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K56" s="6" t="s">
+      <c r="K56" s="5" t="s">
         <v>222</v>
       </c>
       <c r="L56" s="1" t="s">
@@ -3295,7 +3263,7 @@
       <c r="A57" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>224</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -3323,7 +3291,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>228</v>
       </c>
@@ -3355,11 +3323,11 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>234</v>
       </c>
       <c r="C59" s="2" t="n">
@@ -3383,7 +3351,7 @@
       <c r="J59" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K59" s="6"/>
+      <c r="K59" s="5"/>
       <c r="L59" s="1" t="s">
         <v>70</v>
       </c>
@@ -3391,11 +3359,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>236</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -3429,11 +3397,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>241</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -3448,7 +3416,6 @@
       <c r="F61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
         <v>18</v>
       </c>
@@ -3458,7 +3425,7 @@
       <c r="J61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K61" s="6" t="s">
+      <c r="K61" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L61" s="1" t="s">
@@ -3468,7 +3435,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>245</v>
       </c>
@@ -3500,7 +3467,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>250</v>
       </c>
@@ -3532,7 +3499,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>254</v>
       </c>
@@ -3561,7 +3528,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>258</v>
       </c>
@@ -3691,7 +3658,7 @@
       <c r="J68" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K68" s="6"/>
+      <c r="K68" s="5"/>
       <c r="L68" s="1" t="s">
         <v>45</v>
       </c>
@@ -3735,10 +3702,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="5" t="s">
         <v>281</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -3765,7 +3732,7 @@
       <c r="J70" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K70" s="6" t="s">
+      <c r="K70" s="5" t="s">
         <v>115</v>
       </c>
       <c r="L70" s="1" t="s">
@@ -3776,10 +3743,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="5" t="s">
         <v>285</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -3806,7 +3773,7 @@
       <c r="J71" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K71" s="6" t="s">
+      <c r="K71" s="5" t="s">
         <v>115</v>
       </c>
       <c r="L71" s="1" t="s">
@@ -3817,10 +3784,10 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>288</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -3847,7 +3814,7 @@
       <c r="J72" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K72" s="6" t="s">
+      <c r="K72" s="5" t="s">
         <v>115</v>
       </c>
       <c r="L72" s="1" t="s">
@@ -3858,10 +3825,10 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>292</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -3888,7 +3855,7 @@
       <c r="J73" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K73" s="6" t="s">
+      <c r="K73" s="5" t="s">
         <v>115</v>
       </c>
       <c r="L73" s="1" t="s">
@@ -3902,7 +3869,7 @@
       <c r="A74" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>294</v>
       </c>
       <c r="C74" s="2" t="s">
@@ -3937,7 +3904,7 @@
       <c r="A75" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="5" t="s">
         <v>298</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -3961,7 +3928,7 @@
       <c r="J75" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K75" s="6" t="s">
+      <c r="K75" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L75" s="1" t="s">
@@ -3975,7 +3942,7 @@
       <c r="A76" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="5" t="s">
         <v>302</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -3999,7 +3966,7 @@
       <c r="J76" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K76" s="6" t="s">
+      <c r="K76" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L76" s="1" t="s">
@@ -4013,7 +3980,7 @@
       <c r="A77" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="5" t="s">
         <v>305</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -4197,7 +4164,7 @@
       <c r="A82" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="6" t="s">
         <v>327</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -4358,7 +4325,7 @@
       <c r="J86" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K86" s="9" t="s">
+      <c r="K86" s="8" t="s">
         <v>347</v>
       </c>
       <c r="L86" s="1" t="s">
@@ -4445,7 +4412,7 @@
       <c r="A89" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="5" t="s">
         <v>360</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -4611,17 +4578,17 @@
       <c r="D94" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="5" t="s">
         <v>384</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G94" s="6"/>
-      <c r="H94" s="6" t="s">
+      <c r="G94" s="5"/>
+      <c r="H94" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I94" s="6"/>
+      <c r="I94" s="5"/>
       <c r="J94" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Make "versicherung_txt" is dependent from "versicherungsfall"
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="384">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -104,12 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">_aufnahme_therapiebeginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostik ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_diagnostik_id</t>
   </si>
   <si>
     <t xml:space="preserve">Zeit zwischen Endarztkontakt und Entlassung</t>
@@ -1587,10 +1581,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1735,10 +1729,16 @@
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,90 +1808,105 @@
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,13 +1917,13 @@
         <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -1917,16 +1932,16 @@
         <v>18</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,80 +1952,77 @@
         <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M14" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M15" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>17</v>
@@ -2018,31 +2030,37 @@
       <c r="H16" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="J16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -2051,36 +2069,33 @@
         <v>18</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M17" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>17</v>
@@ -2088,473 +2103,461 @@
       <c r="H18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M18" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I19" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="J19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M20" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M21" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>174</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="J23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="K23" s="5"/>
       <c r="L23" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>174</v>
+      <c r="B24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>71</v>
+      <c r="M24" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>116</v>
+        <v>86</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="J26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M26" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="F28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="J29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M29" s="1" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E30" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>142</v>
       </c>
@@ -2562,19 +2565,19 @@
         <v>143</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,19 +2588,19 @@
         <v>145</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,19 +2611,19 @@
         <v>147</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,19 +2634,19 @@
         <v>149</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,19 +2657,19 @@
         <v>151</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,19 +2680,19 @@
         <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,19 +2703,19 @@
         <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,19 +2726,19 @@
         <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,19 +2749,19 @@
         <v>159</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,19 +2772,19 @@
         <v>161</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2792,19 +2795,19 @@
         <v>163</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,146 +2818,155 @@
         <v>165</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>87</v>
+        <v>41</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>177</v>
+        <v>92</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>183</v>
+        <v>61</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>17</v>
@@ -2963,167 +2975,171 @@
         <v>18</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M49" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>21</v>
+      <c r="E52" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>203</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="K52" s="5"/>
       <c r="L52" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>17</v>
@@ -3132,34 +3148,36 @@
         <v>18</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K53" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="L53" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>210</v>
+      <c r="A54" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>17</v>
@@ -3168,36 +3186,36 @@
         <v>18</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>9</v>
+        <v>215</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>209</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>213</v>
+      <c r="A55" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>17</v>
@@ -3206,121 +3224,119 @@
         <v>18</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K55" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K56" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M56" s="1" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>224</v>
+        <v>226</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J57" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M57" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>174</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>231</v>
+        <v>107</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="K58" s="5"/>
       <c r="L58" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>232</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,88 +3346,90 @@
       <c r="B59" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C59" s="2" t="n">
-        <v>174</v>
+      <c r="C59" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>109</v>
+        <v>236</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L59" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K59" s="5"/>
-      <c r="L59" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M59" s="1" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>21</v>
+        <v>241</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>193</v>
+        <v>17</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>239</v>
+        <v>41</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>171</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>243</v>
+        <v>24</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>17</v>
@@ -3419,37 +3437,31 @@
       <c r="H61" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="J61" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K61" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>71</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>17</v>
@@ -3458,30 +3470,27 @@
         <v>18</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>248</v>
+        <v>21</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>17</v>
@@ -3490,94 +3499,100 @@
         <v>18</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>9814184919</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C65" s="2" t="n">
-        <v>9814184919</v>
+        <v>262</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>260</v>
+        <v>21</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K65" s="1" t="s">
-        <v>261</v>
+        <v>41</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>17</v>
@@ -3585,301 +3600,301 @@
       <c r="H66" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="J66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M66" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>80636</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K67" s="5"/>
+      <c r="L67" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M67" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C68" s="2" t="n">
-        <v>80636</v>
+        <v>274</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K68" s="5"/>
+        <v>40</v>
+      </c>
       <c r="L68" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>276</v>
+      <c r="A69" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>279</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="1" t="s">
         <v>291</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>292</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>286</v>
+        <v>205</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M73" s="1" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>207</v>
+        <v>297</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>17</v>
@@ -3887,34 +3902,37 @@
       <c r="H74" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I74" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="J74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>296</v>
+        <v>41</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>171</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>299</v>
+        <v>213</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>17</v>
@@ -3923,112 +3941,109 @@
         <v>18</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J76" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K76" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L76" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M76" s="1" t="s">
-        <v>71</v>
+        <v>306</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>220</v>
+        <v>309</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>17</v>
@@ -4037,217 +4052,217 @@
         <v>18</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>316</v>
+        <v>205</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>317</v>
+        <v>67</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>95</v>
+        <v>322</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M80" s="1" t="s">
-        <v>321</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>325</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>49</v>
+        <v>326</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>324</v>
+        <v>17</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>325</v>
+        <v>41</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B82" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="C82" s="2" t="n">
+        <v>3</v>
+      </c>
       <c r="D82" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>81</v>
+        <v>329</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>17</v>
+        <v>92</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="I82" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L82" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L82" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M82" s="1" t="s">
-        <v>83</v>
+        <v>331</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C83" s="2" t="n">
-        <v>3</v>
+        <v>333</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E83" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M83" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>221</v>
+        <v>339</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>17</v>
@@ -4256,171 +4271,168 @@
         <v>18</v>
       </c>
       <c r="J84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L84" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K84" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="L84" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M84" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J85" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K85" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="L86" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L85" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K86" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M86" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>987654321</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="J87" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="L87" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K87" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="L87" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M87" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C88" s="2" t="n">
-        <v>987654321</v>
+        <v>357</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>356</v>
+        <v>21</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>357</v>
+        <v>41</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E89" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="F89" s="1" t="s">
         <v>17</v>
       </c>
@@ -4428,30 +4440,30 @@
         <v>18</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>365</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>366</v>
+        <v>181</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>17</v>
@@ -4460,30 +4472,30 @@
         <v>18</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K90" s="1" t="s">
-        <v>367</v>
+        <v>41</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>183</v>
+        <v>24</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>17</v>
@@ -4492,30 +4504,30 @@
         <v>18</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>248</v>
+        <v>25</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>17</v>
@@ -4524,84 +4536,53 @@
         <v>18</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>382</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H93" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I93" s="5"/>
       <c r="J93" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C94" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I94" s="5"/>
-      <c r="J94" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L94" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M94" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M25" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
+    <hyperlink ref="M24" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Make "vorname_patient" as String to generate it in second step depending on gender
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="384">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">lookup</t>
   </si>
   <si>
-    <t xml:space="preserve">link=individual_attributes.csv;column=vorname</t>
+    <t xml:space="preserve">link=individual_attributes.csv;column=vorname_m</t>
   </si>
   <si>
     <t xml:space="preserve">Zeit zwischen Aufnahmezeit und Therapiebeginn</t>
@@ -1583,8 +1583,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="E88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4495,7 +4495,7 @@
         <v>24</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>246</v>
+        <v>25</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>17</v>
@@ -4524,10 +4524,7 @@
         <v>377</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Add insurance eGK number as variable
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="388">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -1081,6 +1081,18 @@
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/component/structuredBody/component/section/entry/observation/effectiveTime/low/@value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versicherungs eGK Nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">versicherung_egk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regex=[A-Z]\d{9}</t>
   </si>
   <si>
     <t xml:space="preserve">Versicherungsidentifikation</t>
@@ -1294,7 +1306,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1329,6 +1341,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1581,10 +1597,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4357,58 +4373,58 @@
       <c r="B87" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C87" s="2" t="n">
-        <v>987654321</v>
+      <c r="C87" s="9" t="s">
+        <v>354</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K87" s="1" t="s">
-        <v>355</v>
+        <v>41</v>
       </c>
       <c r="L87" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M87" s="1" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="C88" s="2" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="F88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K88" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J88" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>43</v>
@@ -4421,7 +4437,7 @@
       <c r="A89" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="5" t="s">
         <v>362</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -4430,49 +4446,49 @@
       <c r="D89" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F89" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M89" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K89" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="L89" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="D90" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="F90" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K90" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>86</v>
@@ -4492,10 +4508,7 @@
         <v>373</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>25</v>
+        <v>181</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>17</v>
@@ -4504,7 +4517,7 @@
         <v>18</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>86</v>
@@ -4524,7 +4537,10 @@
         <v>377</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>17</v>
@@ -4555,28 +4571,56 @@
       <c r="D93" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="F93" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M93" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5" t="s">
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I93" s="5"/>
-      <c r="J93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L93" s="1" t="s">
+      <c r="I94" s="5"/>
+      <c r="J94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L94" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M93" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="M94" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M24" r:id="rId1" display="ClinicalDicument/component/structuredBody/component/section/entry/act/entryRelationship/observation/value/@code"/>

</xml_diff>

<commit_message>
german to english in calculated dependency
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkramer\PycharmProjects\cda-test-data-generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511F7242-06F5-467D-97E8-B265730DC5EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F8F7F-07ED-4E41-A0EF-B9D08EC6C880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -945,9 +945,6 @@
     <t>München</t>
   </si>
   <si>
-    <t>link=clinics.csv;column=stadt</t>
-  </si>
-  <si>
     <t>ClinicalDocument/recordTarget/patientRole/addr/city</t>
   </si>
   <si>
@@ -1416,24 +1413,6 @@
     <t>diagnosis_qualifier_1</t>
   </si>
   <si>
-    <t>doctor_contact_end_doctor_contact</t>
-  </si>
-  <si>
-    <t>admission_therapy_start</t>
-  </si>
-  <si>
-    <t>end_doctor_contact_discharge</t>
-  </si>
-  <si>
-    <t>discharge_triage_start</t>
-  </si>
-  <si>
-    <t>therapy_start_doctor_contact</t>
-  </si>
-  <si>
-    <t>triage_start_triage_end</t>
-  </si>
-  <si>
     <t>tetanus_vaccination</t>
   </si>
   <si>
@@ -1447,13 +1426,34 @@
   </si>
   <si>
     <t>allergy_other</t>
+  </si>
+  <si>
+    <t>delta_admission_therapy_start</t>
+  </si>
+  <si>
+    <t>delta_therapy_start_doctor_contact</t>
+  </si>
+  <si>
+    <t>delta_doctor_contact_end_doctor_contact</t>
+  </si>
+  <si>
+    <t>delta_end_doctor_contact_discharge</t>
+  </si>
+  <si>
+    <t>delta_discharge_triage_start</t>
+  </si>
+  <si>
+    <t>delta_triage_start_triage_end</t>
+  </si>
+  <si>
+    <t>link=clinics.csv;column=city</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1499,6 +1499,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1521,7 +1526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -1536,6 +1541,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1800,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1826,10 +1834,9 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1855,10 +1862,10 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -1875,7 +1882,7 @@
         <v>174</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>175</v>
@@ -1910,7 +1917,7 @@
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>113</v>
@@ -1942,16 +1949,16 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>176</v>
@@ -1972,7 +1979,7 @@
         <v>82</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2015,22 +2022,22 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -2051,7 +2058,7 @@
         <v>82</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2062,7 +2069,7 @@
         <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D7" s="2">
         <v>80636</v>
@@ -2104,7 +2111,7 @@
         <v>303</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>304</v>
@@ -2113,7 +2120,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>305</v>
+        <v>472</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>16</v>
@@ -2134,21 +2141,21 @@
         <v>82</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -2169,7 +2176,7 @@
         <v>82</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -2180,7 +2187,7 @@
         <v>244</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>245</v>
@@ -2256,7 +2263,7 @@
         <v>217</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>218</v>
@@ -2335,7 +2342,7 @@
         <v>269</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>270</v>
@@ -2370,16 +2377,16 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>21</v>
@@ -2403,7 +2410,7 @@
         <v>82</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2414,7 +2421,7 @@
         <v>239</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>240</v>
@@ -2452,7 +2459,7 @@
         <v>252</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D17" s="2">
         <v>9814184919</v>
@@ -2496,7 +2503,7 @@
         <v>257</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>258</v>
@@ -2528,22 +2535,22 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>347</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>348</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>16</v>
@@ -2563,22 +2570,22 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>361</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>16</v>
@@ -2590,7 +2597,7 @@
         <v>36</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M20" s="1">
         <v>19</v>
@@ -2599,7 +2606,7 @@
         <v>82</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2607,13 +2614,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>21</v>
@@ -2639,13 +2646,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>19</v>
@@ -2665,13 +2672,13 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D23" s="2">
         <v>987654321</v>
@@ -2680,7 +2687,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>16</v>
@@ -2695,7 +2702,7 @@
         <v>70</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M23" s="1">
         <v>22</v>
@@ -2704,21 +2711,21 @@
         <v>39</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>19</v>
@@ -2739,21 +2746,21 @@
         <v>39</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>57</v>
@@ -2791,7 +2798,7 @@
         <v>189</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>190</v>
@@ -2832,7 +2839,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>56</v>
@@ -2870,7 +2877,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>180</v>
@@ -2908,7 +2915,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>68</v>
@@ -2949,7 +2956,7 @@
         <v>183</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>184</v>
@@ -2993,7 +3000,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>74</v>
@@ -3028,13 +3035,13 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
@@ -3043,13 +3050,13 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>88</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>44</v>
@@ -3067,27 +3074,27 @@
         <v>39</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>16</v>
@@ -3107,7 +3114,7 @@
         <v>39</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -3118,7 +3125,7 @@
         <v>248</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>249</v>
@@ -3153,7 +3160,7 @@
         <v>92</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>93</v>
@@ -3191,7 +3198,7 @@
         <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>86</v>
@@ -3226,13 +3233,13 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>200</v>
@@ -3265,7 +3272,7 @@
         <v>39</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -3320,7 +3327,7 @@
         <v>97</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>98</v>
@@ -3361,7 +3368,7 @@
         <v>194</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>195</v>
@@ -3393,22 +3400,22 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>16</v>
@@ -3420,7 +3427,7 @@
         <v>37</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M41" s="1">
         <v>40</v>
@@ -3429,27 +3436,27 @@
         <v>39</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="60">
       <c r="A42" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>16</v>
@@ -3461,7 +3468,7 @@
         <v>36</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M42" s="1">
         <v>41</v>
@@ -3470,21 +3477,21 @@
         <v>82</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
@@ -3502,7 +3509,7 @@
         <v>37</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M43" s="1">
         <v>42</v>
@@ -3511,27 +3518,27 @@
         <v>39</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>16</v>
@@ -3549,7 +3556,7 @@
         <v>39</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -3560,7 +3567,7 @@
         <v>298</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>213</v>
@@ -3645,7 +3652,7 @@
         <v>229</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>230</v>
@@ -3683,13 +3690,13 @@
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>43</v>
@@ -3704,7 +3711,7 @@
         <v>88</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>44</v>
@@ -3713,7 +3720,7 @@
         <v>36</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M48" s="1">
         <v>47</v>
@@ -3730,10 +3737,10 @@
         <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>163</v>
@@ -3768,7 +3775,7 @@
         <v>166</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>167</v>
@@ -3812,7 +3819,7 @@
         <v>157</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>134</v>
@@ -3844,7 +3851,7 @@
         <v>159</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>134</v>
@@ -3876,7 +3883,7 @@
         <v>151</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>134</v>
@@ -3908,7 +3915,7 @@
         <v>153</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>134</v>
@@ -3940,7 +3947,7 @@
         <v>155</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>134</v>
@@ -3972,7 +3979,7 @@
         <v>139</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>134</v>
@@ -4004,7 +4011,7 @@
         <v>137</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>134</v>
@@ -4036,7 +4043,7 @@
         <v>147</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>134</v>
@@ -4068,7 +4075,7 @@
         <v>149</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>134</v>
@@ -4100,7 +4107,7 @@
         <v>133</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>134</v>
@@ -4132,7 +4139,7 @@
         <v>172</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>134</v>
@@ -4164,7 +4171,7 @@
         <v>145</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>134</v>
@@ -4196,7 +4203,7 @@
         <v>161</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>134</v>
@@ -4228,7 +4235,7 @@
         <v>141</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>134</v>
@@ -4260,7 +4267,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>134</v>
@@ -4292,7 +4299,7 @@
         <v>61</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>62</v>
@@ -4336,7 +4343,7 @@
         <v>291</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>292</v>
@@ -4380,7 +4387,7 @@
         <v>102</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D68" s="2">
         <v>174</v>
@@ -4422,7 +4429,7 @@
         <v>227</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D69" s="2">
         <v>174</v>
@@ -4464,7 +4471,7 @@
         <v>207</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>208</v>
@@ -4508,7 +4515,7 @@
         <v>199</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>200</v>
@@ -4594,7 +4601,7 @@
         <v>204</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>205</v>
@@ -4638,7 +4645,7 @@
         <v>281</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>282</v>
@@ -4685,7 +4692,7 @@
         <v>285</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>279</v>
@@ -4732,7 +4739,7 @@
         <v>274</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>275</v>
@@ -4779,7 +4786,7 @@
         <v>278</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>279</v>
@@ -4826,7 +4833,7 @@
         <v>234</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>235</v>
@@ -4870,7 +4877,7 @@
         <v>295</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>208</v>
@@ -4914,7 +4921,7 @@
         <v>50</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>51</v>
@@ -4946,13 +4953,13 @@
     </row>
     <row r="81" spans="1:15">
       <c r="A81" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>34</v>
@@ -4996,7 +5003,7 @@
         <v>42</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>43</v>
@@ -5037,7 +5044,7 @@
         <v>46</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>34</v>
@@ -5078,7 +5085,7 @@
         <v>48</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>34</v>
@@ -5119,7 +5126,7 @@
         <v>129</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>130</v>
@@ -5157,7 +5164,7 @@
         <v>116</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>117</v>
@@ -5204,7 +5211,7 @@
         <v>122</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>123</v>
@@ -5248,7 +5255,7 @@
         <v>126</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>123</v>
@@ -5294,8 +5301,8 @@
       <c r="B89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>462</v>
+      <c r="C89" s="10" t="s">
+        <v>468</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>14</v>
@@ -5320,8 +5327,8 @@
       <c r="B90" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>463</v>
+      <c r="C90" s="10" t="s">
+        <v>466</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>14</v>
@@ -5346,8 +5353,8 @@
       <c r="B91" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>464</v>
+      <c r="C91" s="10" t="s">
+        <v>469</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>14</v>
@@ -5372,8 +5379,8 @@
       <c r="B92" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>465</v>
+      <c r="C92" s="10" t="s">
+        <v>470</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>14</v>
@@ -5398,8 +5405,8 @@
       <c r="B93" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>466</v>
+      <c r="C93" s="10" t="s">
+        <v>467</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -5424,8 +5431,8 @@
       <c r="B94" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>467</v>
+      <c r="C94" s="10" t="s">
+        <v>471</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Remove config.toml from program Add new command-line parameters: --o, --xlsx, --xslt to program
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="476">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t xml:space="preserve">Städtisches Klinikum München GmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_set=[Beispiel_Klinik]</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/author/representedOrganisation/name
@@ -1612,7 +1615,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1869,7 +1872,7 @@
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I87" activeCellId="0" sqref="I87"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2575,6 +2578,9 @@
       <c r="E18" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2594,27 +2600,27 @@
         <v>31</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>20</v>
@@ -2634,22 +2640,22 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>20</v>
@@ -2661,7 +2667,7 @@
         <v>50</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="N20" s="1" t="n">
         <v>19</v>
@@ -2670,21 +2676,21 @@
         <v>31</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>48</v>
@@ -2707,16 +2713,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>68</v>
@@ -2736,13 +2742,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>987654321</v>
@@ -2751,7 +2757,7 @@
         <v>40</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>20</v>
@@ -2766,7 +2772,7 @@
         <v>112</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="N23" s="1" t="n">
         <v>22</v>
@@ -2775,21 +2781,21 @@
         <v>42</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>68</v>
@@ -2810,21 +2816,21 @@
         <v>42</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>29</v>
@@ -2851,27 +2857,27 @@
         <v>42</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>20</v>
@@ -2883,7 +2889,7 @@
         <v>50</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N26" s="6" t="n">
         <v>25</v>
@@ -2892,27 +2898,27 @@
         <v>42</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>20</v>
@@ -2930,27 +2936,27 @@
         <v>42</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
@@ -2968,27 +2974,27 @@
         <v>31</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>20</v>
@@ -3009,36 +3015,36 @@
         <v>42</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>56</v>
@@ -3047,7 +3053,7 @@
         <v>50</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N30" s="5" t="n">
         <v>29</v>
@@ -3056,21 +3062,21 @@
         <v>42</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>29</v>
@@ -3088,7 +3094,7 @@
         <v>50</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N31" s="6" t="n">
         <v>30</v>
@@ -3097,18 +3103,18 @@
         <v>42</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>3</v>
@@ -3117,16 +3123,16 @@
         <v>68</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>56</v>
@@ -3144,27 +3150,27 @@
         <v>42</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>20</v>
@@ -3185,21 +3191,21 @@
         <v>42</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>68</v>
@@ -3214,27 +3220,27 @@
         <v>22</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N34" s="1" t="n">
         <v>33</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>68</v>
@@ -3249,7 +3255,7 @@
         <v>22</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N35" s="5" t="n">
         <v>34</v>
@@ -3258,36 +3264,36 @@
         <v>42</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>21</v>
@@ -3302,36 +3308,36 @@
         <v>31</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>21</v>
@@ -3349,36 +3355,36 @@
         <v>42</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>56</v>
@@ -3387,7 +3393,7 @@
         <v>22</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N38" s="1" t="n">
         <v>37</v>
@@ -3396,33 +3402,33 @@
         <v>42</v>
       </c>
       <c r="P38" s="9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>21</v>
@@ -3431,7 +3437,7 @@
         <v>22</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N39" s="1" t="n">
         <v>38</v>
@@ -3440,21 +3446,21 @@
         <v>31</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>68</v>
@@ -3469,7 +3475,7 @@
         <v>22</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="N40" s="1" t="n">
         <v>39</v>
@@ -3478,27 +3484,27 @@
         <v>31</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>20</v>
@@ -3510,7 +3516,7 @@
         <v>22</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N41" s="1" t="n">
         <v>40</v>
@@ -3519,27 +3525,27 @@
         <v>42</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>20</v>
@@ -3551,7 +3557,7 @@
         <v>50</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N42" s="1" t="n">
         <v>41</v>
@@ -3560,27 +3566,27 @@
         <v>31</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>20</v>
@@ -3592,7 +3598,7 @@
         <v>22</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N43" s="1" t="n">
         <v>42</v>
@@ -3601,27 +3607,27 @@
         <v>42</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>20</v>
@@ -3639,36 +3645,36 @@
         <v>42</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>56</v>
@@ -3677,7 +3683,7 @@
         <v>22</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N45" s="5" t="n">
         <v>44</v>
@@ -3686,27 +3692,27 @@
         <v>42</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>20</v>
@@ -3718,7 +3724,7 @@
         <v>22</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="N46" s="5" t="n">
         <v>45</v>
@@ -3727,36 +3733,36 @@
         <v>42</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>56</v>
@@ -3765,7 +3771,7 @@
         <v>50</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="N47" s="5" t="n">
         <v>46</v>
@@ -3774,36 +3780,36 @@
         <v>42</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>56</v>
@@ -3812,7 +3818,7 @@
         <v>50</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="N48" s="1" t="n">
         <v>47</v>
@@ -3821,21 +3827,21 @@
         <v>42</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>68</v>
@@ -3856,27 +3862,27 @@
         <v>31</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>20</v>
@@ -3891,7 +3897,7 @@
         <v>22</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N50" s="1" t="n">
         <v>49</v>
@@ -3900,36 +3906,36 @@
         <v>42</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>21</v>
@@ -3940,31 +3946,31 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>21</v>
@@ -3975,31 +3981,31 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>21</v>
@@ -4010,31 +4016,31 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>21</v>
@@ -4045,31 +4051,31 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>21</v>
@@ -4080,31 +4086,31 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>21</v>
@@ -4115,31 +4121,31 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>21</v>
@@ -4150,31 +4156,31 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>21</v>
@@ -4185,31 +4191,31 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>21</v>
@@ -4220,31 +4226,31 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>21</v>
@@ -4255,31 +4261,31 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>21</v>
@@ -4290,31 +4296,31 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>21</v>
@@ -4325,31 +4331,31 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>21</v>
@@ -4360,31 +4366,31 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>21</v>
@@ -4395,31 +4401,31 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>21</v>
@@ -4430,22 +4436,22 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>20</v>
@@ -4469,27 +4475,27 @@
         <v>23</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>20</v>
@@ -4513,18 +4519,18 @@
         <v>23</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>174</v>
@@ -4533,7 +4539,7 @@
         <v>40</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>20</v>
@@ -4555,18 +4561,18 @@
         <v>23</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D69" s="2" t="n">
         <v>174</v>
@@ -4575,7 +4581,7 @@
         <v>40</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>20</v>
@@ -4597,27 +4603,27 @@
         <v>23</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>20</v>
@@ -4632,7 +4638,7 @@
         <v>22</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="N70" s="5" t="n">
         <v>69</v>
@@ -4641,27 +4647,27 @@
         <v>23</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>20</v>
@@ -4683,27 +4689,27 @@
         <v>23</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>20</v>
@@ -4718,7 +4724,7 @@
         <v>22</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="N72" s="5" t="n">
         <v>71</v>
@@ -4727,27 +4733,27 @@
         <v>23</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>20</v>
@@ -4771,36 +4777,36 @@
         <v>23</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>56</v>
@@ -4812,7 +4818,7 @@
         <v>22</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N74" s="5" t="n">
         <v>73</v>
@@ -4821,36 +4827,36 @@
         <v>23</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>56</v>
@@ -4862,7 +4868,7 @@
         <v>22</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N75" s="5" t="n">
         <v>74</v>
@@ -4871,36 +4877,36 @@
         <v>23</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>56</v>
@@ -4912,7 +4918,7 @@
         <v>22</v>
       </c>
       <c r="M76" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N76" s="5" t="n">
         <v>75</v>
@@ -4921,36 +4927,36 @@
         <v>23</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>56</v>
@@ -4962,7 +4968,7 @@
         <v>22</v>
       </c>
       <c r="M77" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N77" s="5" t="n">
         <v>76</v>
@@ -4971,27 +4977,27 @@
         <v>23</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>20</v>
@@ -5015,27 +5021,27 @@
         <v>23</v>
       </c>
       <c r="P78" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>20</v>
@@ -5059,21 +5065,21 @@
         <v>23</v>
       </c>
       <c r="P79" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>68</v>
@@ -5088,7 +5094,7 @@
         <v>22</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N80" s="1" t="n">
         <v>79</v>
@@ -5097,27 +5103,27 @@
         <v>42</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>20</v>
@@ -5132,7 +5138,7 @@
         <v>22</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="N81" s="1" t="n">
         <v>80</v>
@@ -5141,27 +5147,27 @@
         <v>42</v>
       </c>
       <c r="P81" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>20</v>
@@ -5182,27 +5188,27 @@
         <v>42</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>20</v>
@@ -5223,27 +5229,27 @@
         <v>42</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>20</v>
@@ -5264,21 +5270,21 @@
         <v>42</v>
       </c>
       <c r="P84" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>68</v>
@@ -5293,7 +5299,7 @@
         <v>22</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="N85" s="1" t="n">
         <v>84</v>
@@ -5302,36 +5308,36 @@
         <v>42</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>21</v>
@@ -5343,7 +5349,7 @@
         <v>22</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="N86" s="1" t="n">
         <v>85</v>
@@ -5352,33 +5358,33 @@
         <v>42</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>21</v>
@@ -5390,7 +5396,7 @@
         <v>22</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N87" s="1" t="n">
         <v>86</v>
@@ -5399,36 +5405,36 @@
         <v>31</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>21</v>
@@ -5440,7 +5446,7 @@
         <v>22</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N88" s="1" t="n">
         <v>87</v>
@@ -5449,24 +5455,24 @@
         <v>31</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>20</v>
@@ -5480,19 +5486,19 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>20</v>
@@ -5506,19 +5512,19 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>20</v>
@@ -5532,19 +5538,19 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>20</v>
@@ -5558,19 +5564,19 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -5584,19 +5590,19 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Replace link= in Excel file with relative to excel links.
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -169,7 +169,7 @@
     <t xml:space="preserve">lookup</t>
   </si>
   <si>
-    <t xml:space="preserve">link=individual_attributes.csv;column=strassenname</t>
+    <t xml:space="preserve">link=value_sets/individual_attributes.csv;column=strassenname</t>
   </si>
   <si>
     <t xml:space="preserve">0..1</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">München</t>
   </si>
   <si>
-    <t xml:space="preserve">link=clinics.csv;column=city</t>
+    <t xml:space="preserve">link=value_sets/clinics.csv;column=city</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/recordTarget/patientRole/addr/city</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">Kicker</t>
   </si>
   <si>
-    <t xml:space="preserve">link=individual_attributes.csv;column=nachname</t>
+    <t xml:space="preserve">link=value_sets/individual_attributes.csv;column=nachname</t>
   </si>
   <si>
     <t xml:space="preserve">1..n</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">Martin</t>
   </si>
   <si>
-    <t xml:space="preserve">link=individual_attributes.csv;column=vorname_m</t>
+    <t xml:space="preserve">link=value_sets/individual_attributes.csv;column=vorname_m</t>
   </si>
   <si>
     <t xml:space="preserve">ClinicalDocument/author/assignedAuthor/assignedPerson/name/given</t>
@@ -730,7 +730,7 @@
     <t xml:space="preserve">254</t>
   </si>
   <si>
-    <t xml:space="preserve">link=cedis.csv;column=cedis</t>
+    <t xml:space="preserve">link=value_sets/cedis.csv;column=cedis</t>
   </si>
   <si>
     <t xml:space="preserve">OTH,UNK</t>
@@ -1360,7 +1360,7 @@
     <t xml:space="preserve">S93.6</t>
   </si>
   <si>
-    <t xml:space="preserve">link=icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen</t>
+    <t xml:space="preserve">link=value_sets/icd10gm2023.csv;column=Schlüsselnummer ohne Strich, Stern und  Ausrufezeichen</t>
   </si>
   <si>
     <t xml:space="preserve">NegationInd für ausschluss Es gäbe hier noch qualifier als Child</t>
@@ -1871,8 +1871,8 @@
   </sheetPr>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F74" activeCellId="0" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add Empty Enum type and empty generator for generating empty values
</commit_message>
<xml_diff>
--- a/resources/CDAVariables.xlsx
+++ b/resources/CDAVariables.xlsx
@@ -1871,22 +1871,22 @@
   </sheetPr>
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F74" activeCellId="0" sqref="F74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="35.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="70"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="29.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="96.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="31.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.25"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9"/>

</xml_diff>